<commit_message>
Se crea la funcionalida de descarga de inficadores financieros en Excel y PDF
</commit_message>
<xml_diff>
--- a/public/DownloadExcels/Equipos_Herramientas_y_Maquinaria.xlsx
+++ b/public/DownloadExcels/Equipos_Herramientas_y_Maquinaria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Mario\Desktop\Ecopcion Definitivo\ecopFront\public\DownloadExcels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F593F978-96E5-4DBC-BC58-20C02167C5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20996D98-5084-4CAC-88E0-7C76FA758667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -859,7 +859,7 @@
   <dimension ref="A1:Z881"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J7" sqref="B6:J7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se ajusta logica para creacion masiva de assets
</commit_message>
<xml_diff>
--- a/public/DownloadExcels/Equipos_Herramientas_y_Maquinaria.xlsx
+++ b/public/DownloadExcels/Equipos_Herramientas_y_Maquinaria.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Reyes\OneDrive - Top Drive Group\Escritorio\CARLOS\Ecop\ecopFront\public\DownloadExcels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Mario\Desktop\Ecopcion Definitivo\ecopFront\public\DownloadExcels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5E9FB9-C899-4D2E-84C1-D89D2E0505DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7A2E4A-1746-4EC1-B9A7-9E217C06D7BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INVENTARIO DE ACTIVOS" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="3" r:id="rId2"/>
-    <sheet name="Lista desplegable" sheetId="2" r:id="rId3"/>
+    <sheet name="Lista desplegable" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>INVENTARIO DE MAQUINARIA, EQUIPOS Y/O HERRAMIENTAS</t>
   </si>
@@ -82,9 +81,6 @@
   </si>
   <si>
     <t>Tarifas ReteFuente</t>
-  </si>
-  <si>
-    <t>No Aplica</t>
   </si>
   <si>
     <t>Si el equipo, máquina o herramienta tiene IVA ¿Cuál es el porcentaje de IVA aplicable?
@@ -279,6 +275,9 @@
   </si>
   <si>
     <t>Pagos al exterior y dividendos</t>
+  </si>
+  <si>
+    <t>No aplica</t>
   </si>
 </sst>
 </file>
@@ -504,7 +503,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -665,6 +664,12 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -676,6 +681,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -990,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC881"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1007,21 +1015,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -1040,21 +1048,21 @@
       <c r="AC1" s="1"/>
     </row>
     <row r="2" spans="1:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -1073,21 +1081,21 @@
       <c r="AC2" s="1"/>
     </row>
     <row r="3" spans="1:29" ht="246.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
-        <v>23</v>
+      <c r="A3" s="60" t="s">
+        <v>22</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -1129,13 +1137,13 @@
         <v>2</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L4" s="14" t="s">
         <v>14</v>
@@ -1165,7 +1173,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>9</v>
@@ -1180,25 +1188,25 @@
         <v>10</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J5" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="19" t="s">
-        <v>29</v>
-      </c>
       <c r="L5" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M5" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -1227,10 +1235,10 @@
       <c r="E6" s="23"/>
       <c r="F6" s="25"/>
       <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="25"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
       <c r="J6" s="25"/>
-      <c r="K6" s="23"/>
+      <c r="K6" s="57"/>
       <c r="L6" s="24"/>
       <c r="M6" s="24"/>
       <c r="N6" s="1"/>
@@ -1260,10 +1268,10 @@
       <c r="E7" s="23"/>
       <c r="F7" s="25"/>
       <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="25"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
       <c r="J7" s="25"/>
-      <c r="K7" s="23"/>
+      <c r="K7" s="57"/>
       <c r="L7" s="24"/>
       <c r="M7" s="24"/>
       <c r="N7" s="1"/>
@@ -1293,10 +1301,10 @@
       <c r="E8" s="23"/>
       <c r="F8" s="25"/>
       <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="25"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="56"/>
       <c r="J8" s="25"/>
-      <c r="K8" s="23"/>
+      <c r="K8" s="57"/>
       <c r="L8" s="24"/>
       <c r="M8" s="24"/>
       <c r="N8" s="1"/>
@@ -1326,10 +1334,10 @@
       <c r="E9" s="23"/>
       <c r="F9" s="25"/>
       <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="25"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="56"/>
       <c r="J9" s="25"/>
-      <c r="K9" s="23"/>
+      <c r="K9" s="57"/>
       <c r="L9" s="24"/>
       <c r="M9" s="24"/>
       <c r="N9" s="1"/>
@@ -1359,10 +1367,10 @@
       <c r="E10" s="23"/>
       <c r="F10" s="25"/>
       <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="25"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
       <c r="J10" s="25"/>
-      <c r="K10" s="23"/>
+      <c r="K10" s="57"/>
       <c r="L10" s="24"/>
       <c r="M10" s="24"/>
       <c r="N10" s="1"/>
@@ -1392,10 +1400,10 @@
       <c r="E11" s="23"/>
       <c r="F11" s="25"/>
       <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="25"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="56"/>
       <c r="J11" s="25"/>
-      <c r="K11" s="23"/>
+      <c r="K11" s="57"/>
       <c r="L11" s="24"/>
       <c r="M11" s="24"/>
       <c r="N11" s="1"/>
@@ -1425,10 +1433,10 @@
       <c r="E12" s="23"/>
       <c r="F12" s="25"/>
       <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="25"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
       <c r="J12" s="25"/>
-      <c r="K12" s="23"/>
+      <c r="K12" s="57"/>
       <c r="L12" s="24"/>
       <c r="M12" s="24"/>
       <c r="N12" s="1"/>
@@ -1458,10 +1466,10 @@
       <c r="E13" s="23"/>
       <c r="F13" s="25"/>
       <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="25"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="56"/>
       <c r="J13" s="25"/>
-      <c r="K13" s="23"/>
+      <c r="K13" s="57"/>
       <c r="L13" s="24"/>
       <c r="M13" s="24"/>
       <c r="N13" s="1"/>
@@ -1491,10 +1499,10 @@
       <c r="E14" s="10"/>
       <c r="F14" s="11"/>
       <c r="G14" s="12"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="25"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
       <c r="J14" s="25"/>
-      <c r="K14" s="23"/>
+      <c r="K14" s="57"/>
       <c r="L14" s="24"/>
       <c r="M14" s="24"/>
       <c r="N14" s="1"/>
@@ -1524,10 +1532,10 @@
       <c r="E15" s="4"/>
       <c r="F15" s="5"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="25"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
       <c r="J15" s="25"/>
-      <c r="K15" s="23"/>
+      <c r="K15" s="57"/>
       <c r="L15" s="24"/>
       <c r="M15" s="24"/>
       <c r="N15" s="1"/>
@@ -1557,10 +1565,10 @@
       <c r="E16" s="4"/>
       <c r="F16" s="5"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="25"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
       <c r="J16" s="25"/>
-      <c r="K16" s="23"/>
+      <c r="K16" s="57"/>
       <c r="L16" s="24"/>
       <c r="M16" s="24"/>
       <c r="N16" s="1"/>
@@ -1590,10 +1598,10 @@
       <c r="E17" s="4"/>
       <c r="F17" s="5"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="25"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="56"/>
       <c r="J17" s="25"/>
-      <c r="K17" s="23"/>
+      <c r="K17" s="57"/>
       <c r="L17" s="24"/>
       <c r="M17" s="24"/>
       <c r="N17" s="1"/>
@@ -1623,10 +1631,10 @@
       <c r="E18" s="4"/>
       <c r="F18" s="5"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="25"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
       <c r="J18" s="25"/>
-      <c r="K18" s="23"/>
+      <c r="K18" s="57"/>
       <c r="L18" s="24"/>
       <c r="M18" s="24"/>
       <c r="N18" s="1"/>
@@ -1656,10 +1664,10 @@
       <c r="E19" s="4"/>
       <c r="F19" s="5"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="25"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
       <c r="J19" s="25"/>
-      <c r="K19" s="23"/>
+      <c r="K19" s="57"/>
       <c r="L19" s="24"/>
       <c r="M19" s="24"/>
       <c r="N19" s="1"/>
@@ -1689,10 +1697,10 @@
       <c r="E20" s="4"/>
       <c r="F20" s="5"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="25"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="56"/>
       <c r="J20" s="25"/>
-      <c r="K20" s="23"/>
+      <c r="K20" s="57"/>
       <c r="L20" s="24"/>
       <c r="M20" s="24"/>
       <c r="N20" s="1"/>
@@ -1722,10 +1730,10 @@
       <c r="E21" s="4"/>
       <c r="F21" s="5"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="25"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="56"/>
       <c r="J21" s="25"/>
-      <c r="K21" s="23"/>
+      <c r="K21" s="57"/>
       <c r="L21" s="24"/>
       <c r="M21" s="24"/>
       <c r="N21" s="1"/>
@@ -1755,10 +1763,10 @@
       <c r="E22" s="4"/>
       <c r="F22" s="5"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="25"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="56"/>
       <c r="J22" s="25"/>
-      <c r="K22" s="23"/>
+      <c r="K22" s="57"/>
       <c r="L22" s="24"/>
       <c r="M22" s="24"/>
       <c r="N22" s="1"/>
@@ -1788,10 +1796,10 @@
       <c r="E23" s="4"/>
       <c r="F23" s="5"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="25"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
       <c r="J23" s="25"/>
-      <c r="K23" s="23"/>
+      <c r="K23" s="57"/>
       <c r="L23" s="24"/>
       <c r="M23" s="24"/>
       <c r="N23" s="1"/>
@@ -1821,10 +1829,10 @@
       <c r="E24" s="4"/>
       <c r="F24" s="5"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="25"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="56"/>
       <c r="J24" s="25"/>
-      <c r="K24" s="23"/>
+      <c r="K24" s="57"/>
       <c r="L24" s="24"/>
       <c r="M24" s="24"/>
       <c r="N24" s="1"/>
@@ -1854,10 +1862,10 @@
       <c r="E25" s="4"/>
       <c r="F25" s="5"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="25"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="56"/>
       <c r="J25" s="25"/>
-      <c r="K25" s="23"/>
+      <c r="K25" s="57"/>
       <c r="L25" s="24"/>
       <c r="M25" s="24"/>
       <c r="N25" s="1"/>
@@ -1887,10 +1895,10 @@
       <c r="E26" s="4"/>
       <c r="F26" s="5"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="25"/>
+      <c r="H26" s="56"/>
+      <c r="I26" s="56"/>
       <c r="J26" s="25"/>
-      <c r="K26" s="23"/>
+      <c r="K26" s="57"/>
       <c r="L26" s="24"/>
       <c r="M26" s="24"/>
       <c r="N26" s="1"/>
@@ -1920,10 +1928,10 @@
       <c r="E27" s="4"/>
       <c r="F27" s="5"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="25"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="56"/>
       <c r="J27" s="25"/>
-      <c r="K27" s="23"/>
+      <c r="K27" s="57"/>
       <c r="L27" s="24"/>
       <c r="M27" s="24"/>
       <c r="N27" s="1"/>
@@ -1953,10 +1961,10 @@
       <c r="E28" s="4"/>
       <c r="F28" s="5"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="25"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="56"/>
       <c r="J28" s="25"/>
-      <c r="K28" s="23"/>
+      <c r="K28" s="57"/>
       <c r="L28" s="24"/>
       <c r="M28" s="24"/>
       <c r="N28" s="1"/>
@@ -1986,10 +1994,10 @@
       <c r="E29" s="4"/>
       <c r="F29" s="5"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="25"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="56"/>
       <c r="J29" s="25"/>
-      <c r="K29" s="23"/>
+      <c r="K29" s="57"/>
       <c r="L29" s="24"/>
       <c r="M29" s="24"/>
       <c r="N29" s="1"/>
@@ -2019,10 +2027,10 @@
       <c r="E30" s="4"/>
       <c r="F30" s="5"/>
       <c r="G30" s="6"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="25"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
       <c r="J30" s="25"/>
-      <c r="K30" s="23"/>
+      <c r="K30" s="57"/>
       <c r="L30" s="24"/>
       <c r="M30" s="24"/>
       <c r="N30" s="1"/>
@@ -2052,10 +2060,10 @@
       <c r="E31" s="4"/>
       <c r="F31" s="5"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="25"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
       <c r="J31" s="25"/>
-      <c r="K31" s="23"/>
+      <c r="K31" s="57"/>
       <c r="L31" s="24"/>
       <c r="M31" s="24"/>
       <c r="N31" s="1"/>
@@ -2085,10 +2093,10 @@
       <c r="E32" s="4"/>
       <c r="F32" s="5"/>
       <c r="G32" s="6"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="25"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="56"/>
       <c r="J32" s="25"/>
-      <c r="K32" s="23"/>
+      <c r="K32" s="57"/>
       <c r="L32" s="24"/>
       <c r="M32" s="24"/>
       <c r="N32" s="1"/>
@@ -2118,10 +2126,10 @@
       <c r="E33" s="4"/>
       <c r="F33" s="5"/>
       <c r="G33" s="6"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="25"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="56"/>
       <c r="J33" s="25"/>
-      <c r="K33" s="23"/>
+      <c r="K33" s="57"/>
       <c r="L33" s="24"/>
       <c r="M33" s="24"/>
       <c r="N33" s="1"/>
@@ -2151,10 +2159,10 @@
       <c r="E34" s="4"/>
       <c r="F34" s="5"/>
       <c r="G34" s="6"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="25"/>
+      <c r="H34" s="56"/>
+      <c r="I34" s="56"/>
       <c r="J34" s="25"/>
-      <c r="K34" s="23"/>
+      <c r="K34" s="57"/>
       <c r="L34" s="24"/>
       <c r="M34" s="24"/>
       <c r="N34" s="1"/>
@@ -2184,10 +2192,10 @@
       <c r="E35" s="4"/>
       <c r="F35" s="5"/>
       <c r="G35" s="6"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="25"/>
+      <c r="H35" s="56"/>
+      <c r="I35" s="56"/>
       <c r="J35" s="25"/>
-      <c r="K35" s="23"/>
+      <c r="K35" s="57"/>
       <c r="L35" s="24"/>
       <c r="M35" s="24"/>
       <c r="N35" s="1"/>
@@ -2217,10 +2225,10 @@
       <c r="E36" s="4"/>
       <c r="F36" s="5"/>
       <c r="G36" s="6"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="25"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="56"/>
       <c r="J36" s="25"/>
-      <c r="K36" s="23"/>
+      <c r="K36" s="57"/>
       <c r="L36" s="24"/>
       <c r="M36" s="24"/>
       <c r="N36" s="1"/>
@@ -2250,10 +2258,10 @@
       <c r="E37" s="4"/>
       <c r="F37" s="5"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="26"/>
-      <c r="I37" s="25"/>
+      <c r="H37" s="56"/>
+      <c r="I37" s="56"/>
       <c r="J37" s="25"/>
-      <c r="K37" s="23"/>
+      <c r="K37" s="57"/>
       <c r="L37" s="24"/>
       <c r="M37" s="24"/>
       <c r="N37" s="1"/>
@@ -2283,10 +2291,10 @@
       <c r="E38" s="4"/>
       <c r="F38" s="5"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="25"/>
+      <c r="H38" s="56"/>
+      <c r="I38" s="56"/>
       <c r="J38" s="25"/>
-      <c r="K38" s="23"/>
+      <c r="K38" s="57"/>
       <c r="L38" s="24"/>
       <c r="M38" s="24"/>
       <c r="N38" s="1"/>
@@ -2316,10 +2324,10 @@
       <c r="E39" s="4"/>
       <c r="F39" s="5"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="25"/>
+      <c r="H39" s="56"/>
+      <c r="I39" s="56"/>
       <c r="J39" s="25"/>
-      <c r="K39" s="23"/>
+      <c r="K39" s="57"/>
       <c r="L39" s="24"/>
       <c r="M39" s="24"/>
       <c r="N39" s="1"/>
@@ -2349,10 +2357,10 @@
       <c r="E40" s="4"/>
       <c r="F40" s="5"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="26"/>
-      <c r="I40" s="25"/>
+      <c r="H40" s="56"/>
+      <c r="I40" s="56"/>
       <c r="J40" s="25"/>
-      <c r="K40" s="23"/>
+      <c r="K40" s="57"/>
       <c r="L40" s="24"/>
       <c r="M40" s="24"/>
       <c r="N40" s="1"/>
@@ -2382,10 +2390,10 @@
       <c r="E41" s="4"/>
       <c r="F41" s="5"/>
       <c r="G41" s="6"/>
-      <c r="H41" s="26"/>
-      <c r="I41" s="25"/>
+      <c r="H41" s="56"/>
+      <c r="I41" s="56"/>
       <c r="J41" s="25"/>
-      <c r="K41" s="23"/>
+      <c r="K41" s="57"/>
       <c r="L41" s="24"/>
       <c r="M41" s="24"/>
       <c r="N41" s="1"/>
@@ -2415,10 +2423,10 @@
       <c r="E42" s="4"/>
       <c r="F42" s="5"/>
       <c r="G42" s="6"/>
-      <c r="H42" s="26"/>
-      <c r="I42" s="25"/>
+      <c r="H42" s="56"/>
+      <c r="I42" s="56"/>
       <c r="J42" s="25"/>
-      <c r="K42" s="23"/>
+      <c r="K42" s="57"/>
       <c r="L42" s="24"/>
       <c r="M42" s="24"/>
       <c r="N42" s="1"/>
@@ -2448,10 +2456,10 @@
       <c r="E43" s="4"/>
       <c r="F43" s="5"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="25"/>
+      <c r="H43" s="56"/>
+      <c r="I43" s="56"/>
       <c r="J43" s="25"/>
-      <c r="K43" s="23"/>
+      <c r="K43" s="57"/>
       <c r="L43" s="24"/>
       <c r="M43" s="24"/>
       <c r="N43" s="1"/>
@@ -2481,10 +2489,10 @@
       <c r="E44" s="4"/>
       <c r="F44" s="5"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="25"/>
+      <c r="H44" s="56"/>
+      <c r="I44" s="56"/>
       <c r="J44" s="25"/>
-      <c r="K44" s="23"/>
+      <c r="K44" s="57"/>
       <c r="L44" s="24"/>
       <c r="M44" s="24"/>
       <c r="N44" s="1"/>
@@ -2514,10 +2522,10 @@
       <c r="E45" s="4"/>
       <c r="F45" s="5"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="25"/>
+      <c r="H45" s="56"/>
+      <c r="I45" s="56"/>
       <c r="J45" s="25"/>
-      <c r="K45" s="23"/>
+      <c r="K45" s="57"/>
       <c r="L45" s="24"/>
       <c r="M45" s="24"/>
       <c r="N45" s="1"/>
@@ -2547,10 +2555,10 @@
       <c r="E46" s="4"/>
       <c r="F46" s="5"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="26"/>
-      <c r="I46" s="25"/>
+      <c r="H46" s="56"/>
+      <c r="I46" s="56"/>
       <c r="J46" s="25"/>
-      <c r="K46" s="23"/>
+      <c r="K46" s="57"/>
       <c r="L46" s="24"/>
       <c r="M46" s="24"/>
       <c r="N46" s="1"/>
@@ -2580,10 +2588,10 @@
       <c r="E47" s="4"/>
       <c r="F47" s="5"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="25"/>
+      <c r="H47" s="56"/>
+      <c r="I47" s="56"/>
       <c r="J47" s="25"/>
-      <c r="K47" s="23"/>
+      <c r="K47" s="57"/>
       <c r="L47" s="24"/>
       <c r="M47" s="24"/>
       <c r="N47" s="1"/>
@@ -2613,10 +2621,10 @@
       <c r="E48" s="4"/>
       <c r="F48" s="5"/>
       <c r="G48" s="6"/>
-      <c r="H48" s="26"/>
-      <c r="I48" s="25"/>
+      <c r="H48" s="56"/>
+      <c r="I48" s="56"/>
       <c r="J48" s="25"/>
-      <c r="K48" s="23"/>
+      <c r="K48" s="57"/>
       <c r="L48" s="24"/>
       <c r="M48" s="24"/>
       <c r="N48" s="1"/>
@@ -2646,10 +2654,10 @@
       <c r="E49" s="4"/>
       <c r="F49" s="5"/>
       <c r="G49" s="6"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="25"/>
+      <c r="H49" s="56"/>
+      <c r="I49" s="56"/>
       <c r="J49" s="25"/>
-      <c r="K49" s="23"/>
+      <c r="K49" s="57"/>
       <c r="L49" s="24"/>
       <c r="M49" s="24"/>
       <c r="N49" s="1"/>
@@ -2679,10 +2687,10 @@
       <c r="E50" s="4"/>
       <c r="F50" s="5"/>
       <c r="G50" s="6"/>
-      <c r="H50" s="26"/>
-      <c r="I50" s="25"/>
+      <c r="H50" s="56"/>
+      <c r="I50" s="56"/>
       <c r="J50" s="25"/>
-      <c r="K50" s="23"/>
+      <c r="K50" s="57"/>
       <c r="L50" s="24"/>
       <c r="M50" s="24"/>
       <c r="N50" s="1"/>
@@ -2712,10 +2720,10 @@
       <c r="E51" s="4"/>
       <c r="F51" s="5"/>
       <c r="G51" s="6"/>
-      <c r="H51" s="26"/>
-      <c r="I51" s="25"/>
+      <c r="H51" s="56"/>
+      <c r="I51" s="56"/>
       <c r="J51" s="25"/>
-      <c r="K51" s="23"/>
+      <c r="K51" s="57"/>
       <c r="L51" s="24"/>
       <c r="M51" s="24"/>
       <c r="N51" s="1"/>
@@ -2745,10 +2753,10 @@
       <c r="E52" s="4"/>
       <c r="F52" s="5"/>
       <c r="G52" s="6"/>
-      <c r="H52" s="26"/>
-      <c r="I52" s="25"/>
+      <c r="H52" s="56"/>
+      <c r="I52" s="56"/>
       <c r="J52" s="25"/>
-      <c r="K52" s="23"/>
+      <c r="K52" s="57"/>
       <c r="L52" s="24"/>
       <c r="M52" s="24"/>
       <c r="N52" s="1"/>
@@ -2778,10 +2786,10 @@
       <c r="E53" s="4"/>
       <c r="F53" s="5"/>
       <c r="G53" s="6"/>
-      <c r="H53" s="26"/>
-      <c r="I53" s="25"/>
+      <c r="H53" s="56"/>
+      <c r="I53" s="56"/>
       <c r="J53" s="25"/>
-      <c r="K53" s="23"/>
+      <c r="K53" s="57"/>
       <c r="L53" s="24"/>
       <c r="M53" s="24"/>
       <c r="N53" s="1"/>
@@ -2811,10 +2819,10 @@
       <c r="E54" s="4"/>
       <c r="F54" s="5"/>
       <c r="G54" s="6"/>
-      <c r="H54" s="26"/>
-      <c r="I54" s="25"/>
+      <c r="H54" s="56"/>
+      <c r="I54" s="56"/>
       <c r="J54" s="25"/>
-      <c r="K54" s="23"/>
+      <c r="K54" s="57"/>
       <c r="L54" s="24"/>
       <c r="M54" s="24"/>
       <c r="N54" s="1"/>
@@ -2844,10 +2852,10 @@
       <c r="E55" s="4"/>
       <c r="F55" s="5"/>
       <c r="G55" s="6"/>
-      <c r="H55" s="26"/>
-      <c r="I55" s="25"/>
+      <c r="H55" s="56"/>
+      <c r="I55" s="56"/>
       <c r="J55" s="25"/>
-      <c r="K55" s="23"/>
+      <c r="K55" s="57"/>
       <c r="L55" s="24"/>
       <c r="M55" s="24"/>
       <c r="N55" s="1"/>
@@ -2877,10 +2885,10 @@
       <c r="E56" s="4"/>
       <c r="F56" s="5"/>
       <c r="G56" s="6"/>
-      <c r="H56" s="26"/>
-      <c r="I56" s="25"/>
+      <c r="H56" s="56"/>
+      <c r="I56" s="56"/>
       <c r="J56" s="25"/>
-      <c r="K56" s="23"/>
+      <c r="K56" s="57"/>
       <c r="L56" s="24"/>
       <c r="M56" s="24"/>
       <c r="N56" s="1"/>
@@ -2910,10 +2918,10 @@
       <c r="E57" s="4"/>
       <c r="F57" s="5"/>
       <c r="G57" s="6"/>
-      <c r="H57" s="26"/>
-      <c r="I57" s="25"/>
+      <c r="H57" s="56"/>
+      <c r="I57" s="56"/>
       <c r="J57" s="25"/>
-      <c r="K57" s="23"/>
+      <c r="K57" s="57"/>
       <c r="L57" s="24"/>
       <c r="M57" s="24"/>
       <c r="N57" s="1"/>
@@ -2943,10 +2951,10 @@
       <c r="E58" s="4"/>
       <c r="F58" s="5"/>
       <c r="G58" s="6"/>
-      <c r="H58" s="26"/>
-      <c r="I58" s="25"/>
+      <c r="H58" s="56"/>
+      <c r="I58" s="56"/>
       <c r="J58" s="25"/>
-      <c r="K58" s="23"/>
+      <c r="K58" s="57"/>
       <c r="L58" s="24"/>
       <c r="M58" s="24"/>
       <c r="N58" s="1"/>
@@ -2976,10 +2984,10 @@
       <c r="E59" s="4"/>
       <c r="F59" s="5"/>
       <c r="G59" s="6"/>
-      <c r="H59" s="26"/>
-      <c r="I59" s="25"/>
+      <c r="H59" s="56"/>
+      <c r="I59" s="56"/>
       <c r="J59" s="25"/>
-      <c r="K59" s="23"/>
+      <c r="K59" s="57"/>
       <c r="L59" s="24"/>
       <c r="M59" s="24"/>
       <c r="N59" s="1"/>
@@ -3009,10 +3017,10 @@
       <c r="E60" s="4"/>
       <c r="F60" s="5"/>
       <c r="G60" s="6"/>
-      <c r="H60" s="26"/>
-      <c r="I60" s="25"/>
+      <c r="H60" s="56"/>
+      <c r="I60" s="56"/>
       <c r="J60" s="25"/>
-      <c r="K60" s="23"/>
+      <c r="K60" s="57"/>
       <c r="L60" s="24"/>
       <c r="M60" s="24"/>
       <c r="N60" s="1"/>
@@ -3042,10 +3050,10 @@
       <c r="E61" s="4"/>
       <c r="F61" s="5"/>
       <c r="G61" s="6"/>
-      <c r="H61" s="26"/>
-      <c r="I61" s="25"/>
+      <c r="H61" s="56"/>
+      <c r="I61" s="56"/>
       <c r="J61" s="25"/>
-      <c r="K61" s="23"/>
+      <c r="K61" s="57"/>
       <c r="L61" s="24"/>
       <c r="M61" s="24"/>
       <c r="N61" s="1"/>
@@ -3075,10 +3083,10 @@
       <c r="E62" s="4"/>
       <c r="F62" s="5"/>
       <c r="G62" s="6"/>
-      <c r="H62" s="26"/>
-      <c r="I62" s="25"/>
+      <c r="H62" s="56"/>
+      <c r="I62" s="56"/>
       <c r="J62" s="25"/>
-      <c r="K62" s="23"/>
+      <c r="K62" s="57"/>
       <c r="L62" s="24"/>
       <c r="M62" s="24"/>
       <c r="N62" s="1"/>
@@ -3108,10 +3116,10 @@
       <c r="E63" s="4"/>
       <c r="F63" s="5"/>
       <c r="G63" s="6"/>
-      <c r="H63" s="26"/>
-      <c r="I63" s="25"/>
+      <c r="H63" s="56"/>
+      <c r="I63" s="56"/>
       <c r="J63" s="25"/>
-      <c r="K63" s="23"/>
+      <c r="K63" s="57"/>
       <c r="L63" s="24"/>
       <c r="M63" s="24"/>
       <c r="N63" s="1"/>
@@ -3141,10 +3149,10 @@
       <c r="E64" s="4"/>
       <c r="F64" s="5"/>
       <c r="G64" s="6"/>
-      <c r="H64" s="26"/>
-      <c r="I64" s="25"/>
+      <c r="H64" s="56"/>
+      <c r="I64" s="56"/>
       <c r="J64" s="25"/>
-      <c r="K64" s="23"/>
+      <c r="K64" s="57"/>
       <c r="L64" s="24"/>
       <c r="M64" s="24"/>
       <c r="N64" s="1"/>
@@ -3174,10 +3182,10 @@
       <c r="E65" s="4"/>
       <c r="F65" s="5"/>
       <c r="G65" s="6"/>
-      <c r="H65" s="26"/>
-      <c r="I65" s="25"/>
+      <c r="H65" s="56"/>
+      <c r="I65" s="56"/>
       <c r="J65" s="25"/>
-      <c r="K65" s="23"/>
+      <c r="K65" s="57"/>
       <c r="L65" s="24"/>
       <c r="M65" s="24"/>
       <c r="N65" s="1"/>
@@ -3207,10 +3215,10 @@
       <c r="E66" s="4"/>
       <c r="F66" s="5"/>
       <c r="G66" s="6"/>
-      <c r="H66" s="26"/>
-      <c r="I66" s="25"/>
+      <c r="H66" s="56"/>
+      <c r="I66" s="56"/>
       <c r="J66" s="25"/>
-      <c r="K66" s="23"/>
+      <c r="K66" s="57"/>
       <c r="L66" s="24"/>
       <c r="M66" s="24"/>
       <c r="N66" s="1"/>
@@ -3240,10 +3248,10 @@
       <c r="E67" s="4"/>
       <c r="F67" s="5"/>
       <c r="G67" s="6"/>
-      <c r="H67" s="26"/>
-      <c r="I67" s="25"/>
+      <c r="H67" s="56"/>
+      <c r="I67" s="56"/>
       <c r="J67" s="25"/>
-      <c r="K67" s="23"/>
+      <c r="K67" s="57"/>
       <c r="L67" s="24"/>
       <c r="M67" s="24"/>
       <c r="N67" s="1"/>
@@ -3273,10 +3281,10 @@
       <c r="E68" s="4"/>
       <c r="F68" s="5"/>
       <c r="G68" s="6"/>
-      <c r="H68" s="26"/>
-      <c r="I68" s="25"/>
+      <c r="H68" s="56"/>
+      <c r="I68" s="56"/>
       <c r="J68" s="25"/>
-      <c r="K68" s="23"/>
+      <c r="K68" s="57"/>
       <c r="L68" s="24"/>
       <c r="M68" s="24"/>
       <c r="N68" s="1"/>
@@ -3306,10 +3314,10 @@
       <c r="E69" s="4"/>
       <c r="F69" s="5"/>
       <c r="G69" s="6"/>
-      <c r="H69" s="26"/>
-      <c r="I69" s="25"/>
+      <c r="H69" s="56"/>
+      <c r="I69" s="56"/>
       <c r="J69" s="25"/>
-      <c r="K69" s="23"/>
+      <c r="K69" s="57"/>
       <c r="L69" s="24"/>
       <c r="M69" s="24"/>
       <c r="N69" s="1"/>
@@ -3339,10 +3347,10 @@
       <c r="E70" s="4"/>
       <c r="F70" s="5"/>
       <c r="G70" s="6"/>
-      <c r="H70" s="26"/>
-      <c r="I70" s="25"/>
+      <c r="H70" s="56"/>
+      <c r="I70" s="56"/>
       <c r="J70" s="25"/>
-      <c r="K70" s="23"/>
+      <c r="K70" s="57"/>
       <c r="L70" s="24"/>
       <c r="M70" s="24"/>
       <c r="N70" s="1"/>
@@ -3372,10 +3380,10 @@
       <c r="E71" s="4"/>
       <c r="F71" s="5"/>
       <c r="G71" s="6"/>
-      <c r="H71" s="26"/>
-      <c r="I71" s="25"/>
+      <c r="H71" s="56"/>
+      <c r="I71" s="56"/>
       <c r="J71" s="25"/>
-      <c r="K71" s="23"/>
+      <c r="K71" s="57"/>
       <c r="L71" s="24"/>
       <c r="M71" s="24"/>
       <c r="N71" s="1"/>
@@ -3405,10 +3413,10 @@
       <c r="E72" s="4"/>
       <c r="F72" s="5"/>
       <c r="G72" s="6"/>
-      <c r="H72" s="26"/>
-      <c r="I72" s="25"/>
+      <c r="H72" s="56"/>
+      <c r="I72" s="56"/>
       <c r="J72" s="25"/>
-      <c r="K72" s="23"/>
+      <c r="K72" s="57"/>
       <c r="L72" s="24"/>
       <c r="M72" s="24"/>
       <c r="N72" s="1"/>
@@ -3438,10 +3446,10 @@
       <c r="E73" s="4"/>
       <c r="F73" s="5"/>
       <c r="G73" s="6"/>
-      <c r="H73" s="26"/>
-      <c r="I73" s="25"/>
+      <c r="H73" s="56"/>
+      <c r="I73" s="56"/>
       <c r="J73" s="25"/>
-      <c r="K73" s="23"/>
+      <c r="K73" s="57"/>
       <c r="L73" s="24"/>
       <c r="M73" s="24"/>
       <c r="N73" s="1"/>
@@ -3471,10 +3479,10 @@
       <c r="E74" s="4"/>
       <c r="F74" s="5"/>
       <c r="G74" s="6"/>
-      <c r="H74" s="26"/>
-      <c r="I74" s="25"/>
+      <c r="H74" s="56"/>
+      <c r="I74" s="56"/>
       <c r="J74" s="25"/>
-      <c r="K74" s="23"/>
+      <c r="K74" s="57"/>
       <c r="L74" s="24"/>
       <c r="M74" s="24"/>
       <c r="N74" s="1"/>
@@ -3504,10 +3512,10 @@
       <c r="E75" s="4"/>
       <c r="F75" s="5"/>
       <c r="G75" s="6"/>
-      <c r="H75" s="26"/>
-      <c r="I75" s="25"/>
+      <c r="H75" s="56"/>
+      <c r="I75" s="56"/>
       <c r="J75" s="25"/>
-      <c r="K75" s="23"/>
+      <c r="K75" s="57"/>
       <c r="L75" s="24"/>
       <c r="M75" s="24"/>
       <c r="N75" s="1"/>
@@ -3537,10 +3545,10 @@
       <c r="E76" s="4"/>
       <c r="F76" s="5"/>
       <c r="G76" s="6"/>
-      <c r="H76" s="26"/>
-      <c r="I76" s="25"/>
+      <c r="H76" s="56"/>
+      <c r="I76" s="56"/>
       <c r="J76" s="25"/>
-      <c r="K76" s="23"/>
+      <c r="K76" s="57"/>
       <c r="L76" s="24"/>
       <c r="M76" s="24"/>
       <c r="N76" s="1"/>
@@ -3570,10 +3578,10 @@
       <c r="E77" s="4"/>
       <c r="F77" s="5"/>
       <c r="G77" s="6"/>
-      <c r="H77" s="26"/>
-      <c r="I77" s="25"/>
+      <c r="H77" s="56"/>
+      <c r="I77" s="56"/>
       <c r="J77" s="25"/>
-      <c r="K77" s="23"/>
+      <c r="K77" s="57"/>
       <c r="L77" s="24"/>
       <c r="M77" s="24"/>
       <c r="N77" s="1"/>
@@ -3603,10 +3611,10 @@
       <c r="E78" s="4"/>
       <c r="F78" s="5"/>
       <c r="G78" s="6"/>
-      <c r="H78" s="26"/>
-      <c r="I78" s="25"/>
+      <c r="H78" s="56"/>
+      <c r="I78" s="56"/>
       <c r="J78" s="25"/>
-      <c r="K78" s="23"/>
+      <c r="K78" s="57"/>
       <c r="L78" s="24"/>
       <c r="M78" s="24"/>
       <c r="N78" s="1"/>
@@ -3636,10 +3644,10 @@
       <c r="E79" s="4"/>
       <c r="F79" s="5"/>
       <c r="G79" s="6"/>
-      <c r="H79" s="26"/>
-      <c r="I79" s="25"/>
+      <c r="H79" s="56"/>
+      <c r="I79" s="56"/>
       <c r="J79" s="25"/>
-      <c r="K79" s="23"/>
+      <c r="K79" s="57"/>
       <c r="L79" s="24"/>
       <c r="M79" s="24"/>
       <c r="N79" s="1"/>
@@ -3669,10 +3677,10 @@
       <c r="E80" s="4"/>
       <c r="F80" s="5"/>
       <c r="G80" s="6"/>
-      <c r="H80" s="26"/>
-      <c r="I80" s="25"/>
+      <c r="H80" s="56"/>
+      <c r="I80" s="56"/>
       <c r="J80" s="25"/>
-      <c r="K80" s="23"/>
+      <c r="K80" s="57"/>
       <c r="L80" s="24"/>
       <c r="M80" s="24"/>
       <c r="N80" s="1"/>
@@ -3702,10 +3710,10 @@
       <c r="E81" s="4"/>
       <c r="F81" s="5"/>
       <c r="G81" s="6"/>
-      <c r="H81" s="26"/>
-      <c r="I81" s="25"/>
+      <c r="H81" s="56"/>
+      <c r="I81" s="56"/>
       <c r="J81" s="25"/>
-      <c r="K81" s="23"/>
+      <c r="K81" s="57"/>
       <c r="L81" s="24"/>
       <c r="M81" s="24"/>
       <c r="N81" s="1"/>
@@ -3735,10 +3743,10 @@
       <c r="E82" s="4"/>
       <c r="F82" s="5"/>
       <c r="G82" s="6"/>
-      <c r="H82" s="26"/>
-      <c r="I82" s="25"/>
+      <c r="H82" s="56"/>
+      <c r="I82" s="56"/>
       <c r="J82" s="25"/>
-      <c r="K82" s="23"/>
+      <c r="K82" s="57"/>
       <c r="L82" s="24"/>
       <c r="M82" s="24"/>
       <c r="N82" s="1"/>
@@ -3768,10 +3776,10 @@
       <c r="E83" s="4"/>
       <c r="F83" s="5"/>
       <c r="G83" s="6"/>
-      <c r="H83" s="26"/>
-      <c r="I83" s="25"/>
+      <c r="H83" s="56"/>
+      <c r="I83" s="56"/>
       <c r="J83" s="25"/>
-      <c r="K83" s="23"/>
+      <c r="K83" s="57"/>
       <c r="L83" s="24"/>
       <c r="M83" s="24"/>
       <c r="N83" s="1"/>
@@ -3801,10 +3809,10 @@
       <c r="E84" s="4"/>
       <c r="F84" s="5"/>
       <c r="G84" s="6"/>
-      <c r="H84" s="26"/>
-      <c r="I84" s="25"/>
+      <c r="H84" s="56"/>
+      <c r="I84" s="56"/>
       <c r="J84" s="25"/>
-      <c r="K84" s="23"/>
+      <c r="K84" s="57"/>
       <c r="L84" s="24"/>
       <c r="M84" s="24"/>
       <c r="N84" s="1"/>
@@ -3834,10 +3842,10 @@
       <c r="E85" s="4"/>
       <c r="F85" s="5"/>
       <c r="G85" s="6"/>
-      <c r="H85" s="26"/>
-      <c r="I85" s="25"/>
+      <c r="H85" s="56"/>
+      <c r="I85" s="56"/>
       <c r="J85" s="25"/>
-      <c r="K85" s="23"/>
+      <c r="K85" s="57"/>
       <c r="L85" s="24"/>
       <c r="M85" s="24"/>
       <c r="N85" s="1"/>
@@ -3867,10 +3875,10 @@
       <c r="E86" s="4"/>
       <c r="F86" s="5"/>
       <c r="G86" s="6"/>
-      <c r="H86" s="26"/>
-      <c r="I86" s="25"/>
+      <c r="H86" s="56"/>
+      <c r="I86" s="56"/>
       <c r="J86" s="25"/>
-      <c r="K86" s="23"/>
+      <c r="K86" s="57"/>
       <c r="L86" s="24"/>
       <c r="M86" s="24"/>
       <c r="N86" s="1"/>
@@ -3900,10 +3908,10 @@
       <c r="E87" s="4"/>
       <c r="F87" s="5"/>
       <c r="G87" s="6"/>
-      <c r="H87" s="26"/>
-      <c r="I87" s="25"/>
+      <c r="H87" s="56"/>
+      <c r="I87" s="56"/>
       <c r="J87" s="25"/>
-      <c r="K87" s="23"/>
+      <c r="K87" s="57"/>
       <c r="L87" s="24"/>
       <c r="M87" s="24"/>
       <c r="N87" s="1"/>
@@ -3933,10 +3941,10 @@
       <c r="E88" s="4"/>
       <c r="F88" s="5"/>
       <c r="G88" s="6"/>
-      <c r="H88" s="26"/>
-      <c r="I88" s="25"/>
+      <c r="H88" s="56"/>
+      <c r="I88" s="56"/>
       <c r="J88" s="25"/>
-      <c r="K88" s="23"/>
+      <c r="K88" s="57"/>
       <c r="L88" s="24"/>
       <c r="M88" s="24"/>
       <c r="N88" s="1"/>
@@ -3966,10 +3974,10 @@
       <c r="E89" s="4"/>
       <c r="F89" s="5"/>
       <c r="G89" s="6"/>
-      <c r="H89" s="26"/>
-      <c r="I89" s="25"/>
+      <c r="H89" s="56"/>
+      <c r="I89" s="56"/>
       <c r="J89" s="25"/>
-      <c r="K89" s="23"/>
+      <c r="K89" s="57"/>
       <c r="L89" s="24"/>
       <c r="M89" s="24"/>
       <c r="N89" s="1"/>
@@ -3999,10 +4007,10 @@
       <c r="E90" s="4"/>
       <c r="F90" s="5"/>
       <c r="G90" s="6"/>
-      <c r="H90" s="26"/>
-      <c r="I90" s="25"/>
+      <c r="H90" s="56"/>
+      <c r="I90" s="56"/>
       <c r="J90" s="25"/>
-      <c r="K90" s="23"/>
+      <c r="K90" s="57"/>
       <c r="L90" s="24"/>
       <c r="M90" s="24"/>
       <c r="N90" s="1"/>
@@ -4032,10 +4040,10 @@
       <c r="E91" s="4"/>
       <c r="F91" s="5"/>
       <c r="G91" s="6"/>
-      <c r="H91" s="26"/>
-      <c r="I91" s="25"/>
+      <c r="H91" s="56"/>
+      <c r="I91" s="56"/>
       <c r="J91" s="25"/>
-      <c r="K91" s="23"/>
+      <c r="K91" s="57"/>
       <c r="L91" s="24"/>
       <c r="M91" s="24"/>
       <c r="N91" s="1"/>
@@ -4065,10 +4073,10 @@
       <c r="E92" s="4"/>
       <c r="F92" s="5"/>
       <c r="G92" s="6"/>
-      <c r="H92" s="26"/>
-      <c r="I92" s="25"/>
+      <c r="H92" s="56"/>
+      <c r="I92" s="56"/>
       <c r="J92" s="25"/>
-      <c r="K92" s="23"/>
+      <c r="K92" s="57"/>
       <c r="L92" s="24"/>
       <c r="M92" s="24"/>
       <c r="N92" s="1"/>
@@ -4098,10 +4106,10 @@
       <c r="E93" s="4"/>
       <c r="F93" s="5"/>
       <c r="G93" s="6"/>
-      <c r="H93" s="26"/>
-      <c r="I93" s="25"/>
+      <c r="H93" s="56"/>
+      <c r="I93" s="56"/>
       <c r="J93" s="25"/>
-      <c r="K93" s="23"/>
+      <c r="K93" s="57"/>
       <c r="L93" s="24"/>
       <c r="M93" s="24"/>
       <c r="N93" s="1"/>
@@ -4131,10 +4139,10 @@
       <c r="E94" s="4"/>
       <c r="F94" s="5"/>
       <c r="G94" s="6"/>
-      <c r="H94" s="26"/>
-      <c r="I94" s="25"/>
+      <c r="H94" s="56"/>
+      <c r="I94" s="56"/>
       <c r="J94" s="25"/>
-      <c r="K94" s="23"/>
+      <c r="K94" s="57"/>
       <c r="L94" s="24"/>
       <c r="M94" s="24"/>
       <c r="N94" s="1"/>
@@ -4164,10 +4172,10 @@
       <c r="E95" s="4"/>
       <c r="F95" s="5"/>
       <c r="G95" s="6"/>
-      <c r="H95" s="26"/>
-      <c r="I95" s="25"/>
+      <c r="H95" s="56"/>
+      <c r="I95" s="56"/>
       <c r="J95" s="25"/>
-      <c r="K95" s="23"/>
+      <c r="K95" s="57"/>
       <c r="L95" s="24"/>
       <c r="M95" s="24"/>
       <c r="N95" s="1"/>
@@ -4197,10 +4205,10 @@
       <c r="E96" s="4"/>
       <c r="F96" s="5"/>
       <c r="G96" s="6"/>
-      <c r="H96" s="26"/>
-      <c r="I96" s="25"/>
+      <c r="H96" s="56"/>
+      <c r="I96" s="56"/>
       <c r="J96" s="25"/>
-      <c r="K96" s="23"/>
+      <c r="K96" s="57"/>
       <c r="L96" s="24"/>
       <c r="M96" s="24"/>
       <c r="N96" s="1"/>
@@ -4230,10 +4238,10 @@
       <c r="E97" s="4"/>
       <c r="F97" s="5"/>
       <c r="G97" s="6"/>
-      <c r="H97" s="26"/>
-      <c r="I97" s="25"/>
+      <c r="H97" s="56"/>
+      <c r="I97" s="56"/>
       <c r="J97" s="25"/>
-      <c r="K97" s="23"/>
+      <c r="K97" s="57"/>
       <c r="L97" s="24"/>
       <c r="M97" s="24"/>
       <c r="N97" s="1"/>
@@ -4263,10 +4271,10 @@
       <c r="E98" s="4"/>
       <c r="F98" s="5"/>
       <c r="G98" s="6"/>
-      <c r="H98" s="26"/>
-      <c r="I98" s="25"/>
+      <c r="H98" s="56"/>
+      <c r="I98" s="56"/>
       <c r="J98" s="25"/>
-      <c r="K98" s="23"/>
+      <c r="K98" s="57"/>
       <c r="L98" s="24"/>
       <c r="M98" s="24"/>
       <c r="N98" s="1"/>
@@ -4296,10 +4304,10 @@
       <c r="E99" s="4"/>
       <c r="F99" s="5"/>
       <c r="G99" s="6"/>
-      <c r="H99" s="26"/>
-      <c r="I99" s="25"/>
+      <c r="H99" s="56"/>
+      <c r="I99" s="56"/>
       <c r="J99" s="25"/>
-      <c r="K99" s="23"/>
+      <c r="K99" s="57"/>
       <c r="L99" s="24"/>
       <c r="M99" s="24"/>
       <c r="N99" s="1"/>
@@ -4329,10 +4337,10 @@
       <c r="E100" s="4"/>
       <c r="F100" s="5"/>
       <c r="G100" s="6"/>
-      <c r="H100" s="26"/>
-      <c r="I100" s="25"/>
+      <c r="H100" s="56"/>
+      <c r="I100" s="56"/>
       <c r="J100" s="25"/>
-      <c r="K100" s="23"/>
+      <c r="K100" s="57"/>
       <c r="L100" s="24"/>
       <c r="M100" s="24"/>
       <c r="N100" s="1"/>
@@ -4362,10 +4370,10 @@
       <c r="E101" s="4"/>
       <c r="F101" s="5"/>
       <c r="G101" s="6"/>
-      <c r="H101" s="26"/>
-      <c r="I101" s="25"/>
+      <c r="H101" s="56"/>
+      <c r="I101" s="56"/>
       <c r="J101" s="25"/>
-      <c r="K101" s="23"/>
+      <c r="K101" s="57"/>
       <c r="L101" s="24"/>
       <c r="M101" s="24"/>
       <c r="N101" s="1"/>
@@ -4395,10 +4403,10 @@
       <c r="E102" s="4"/>
       <c r="F102" s="5"/>
       <c r="G102" s="6"/>
-      <c r="H102" s="26"/>
-      <c r="I102" s="25"/>
+      <c r="H102" s="56"/>
+      <c r="I102" s="56"/>
       <c r="J102" s="25"/>
-      <c r="K102" s="23"/>
+      <c r="K102" s="57"/>
       <c r="L102" s="24"/>
       <c r="M102" s="24"/>
       <c r="N102" s="1"/>
@@ -4428,10 +4436,10 @@
       <c r="E103" s="4"/>
       <c r="F103" s="5"/>
       <c r="G103" s="6"/>
-      <c r="H103" s="26"/>
-      <c r="I103" s="25"/>
+      <c r="H103" s="56"/>
+      <c r="I103" s="56"/>
       <c r="J103" s="25"/>
-      <c r="K103" s="23"/>
+      <c r="K103" s="57"/>
       <c r="L103" s="24"/>
       <c r="M103" s="24"/>
       <c r="N103" s="1"/>
@@ -4461,10 +4469,10 @@
       <c r="E104" s="4"/>
       <c r="F104" s="5"/>
       <c r="G104" s="6"/>
-      <c r="H104" s="26"/>
-      <c r="I104" s="25"/>
+      <c r="H104" s="56"/>
+      <c r="I104" s="56"/>
       <c r="J104" s="25"/>
-      <c r="K104" s="23"/>
+      <c r="K104" s="57"/>
       <c r="L104" s="24"/>
       <c r="M104" s="24"/>
       <c r="N104" s="1"/>
@@ -4494,10 +4502,10 @@
       <c r="E105" s="4"/>
       <c r="F105" s="5"/>
       <c r="G105" s="6"/>
-      <c r="H105" s="26"/>
-      <c r="I105" s="25"/>
+      <c r="H105" s="56"/>
+      <c r="I105" s="56"/>
       <c r="J105" s="25"/>
-      <c r="K105" s="23"/>
+      <c r="K105" s="57"/>
       <c r="L105" s="24"/>
       <c r="M105" s="24"/>
       <c r="N105" s="1"/>
@@ -4527,10 +4535,10 @@
       <c r="E106" s="4"/>
       <c r="F106" s="5"/>
       <c r="G106" s="6"/>
-      <c r="H106" s="26"/>
-      <c r="I106" s="25"/>
+      <c r="H106" s="56"/>
+      <c r="I106" s="56"/>
       <c r="J106" s="25"/>
-      <c r="K106" s="23"/>
+      <c r="K106" s="57"/>
       <c r="L106" s="24"/>
       <c r="M106" s="24"/>
       <c r="N106" s="1"/>
@@ -4560,10 +4568,10 @@
       <c r="E107" s="4"/>
       <c r="F107" s="5"/>
       <c r="G107" s="6"/>
-      <c r="H107" s="26"/>
-      <c r="I107" s="25"/>
+      <c r="H107" s="56"/>
+      <c r="I107" s="56"/>
       <c r="J107" s="25"/>
-      <c r="K107" s="23"/>
+      <c r="K107" s="57"/>
       <c r="L107" s="24"/>
       <c r="M107" s="24"/>
       <c r="N107" s="1"/>
@@ -4593,10 +4601,10 @@
       <c r="E108" s="4"/>
       <c r="F108" s="5"/>
       <c r="G108" s="6"/>
-      <c r="H108" s="26"/>
-      <c r="I108" s="25"/>
+      <c r="H108" s="56"/>
+      <c r="I108" s="56"/>
       <c r="J108" s="25"/>
-      <c r="K108" s="23"/>
+      <c r="K108" s="57"/>
       <c r="L108" s="24"/>
       <c r="M108" s="24"/>
       <c r="N108" s="1"/>
@@ -4626,10 +4634,10 @@
       <c r="E109" s="4"/>
       <c r="F109" s="5"/>
       <c r="G109" s="6"/>
-      <c r="H109" s="26"/>
-      <c r="I109" s="25"/>
+      <c r="H109" s="56"/>
+      <c r="I109" s="56"/>
       <c r="J109" s="25"/>
-      <c r="K109" s="23"/>
+      <c r="K109" s="57"/>
       <c r="L109" s="24"/>
       <c r="M109" s="24"/>
       <c r="N109" s="1"/>
@@ -4659,10 +4667,10 @@
       <c r="E110" s="4"/>
       <c r="F110" s="5"/>
       <c r="G110" s="6"/>
-      <c r="H110" s="26"/>
-      <c r="I110" s="25"/>
+      <c r="H110" s="56"/>
+      <c r="I110" s="56"/>
       <c r="J110" s="25"/>
-      <c r="K110" s="23"/>
+      <c r="K110" s="57"/>
       <c r="L110" s="24"/>
       <c r="M110" s="24"/>
       <c r="N110" s="1"/>
@@ -4692,10 +4700,10 @@
       <c r="E111" s="4"/>
       <c r="F111" s="5"/>
       <c r="G111" s="6"/>
-      <c r="H111" s="26"/>
-      <c r="I111" s="25"/>
+      <c r="H111" s="56"/>
+      <c r="I111" s="56"/>
       <c r="J111" s="25"/>
-      <c r="K111" s="23"/>
+      <c r="K111" s="57"/>
       <c r="L111" s="24"/>
       <c r="M111" s="24"/>
       <c r="N111" s="1"/>
@@ -4725,10 +4733,10 @@
       <c r="E112" s="4"/>
       <c r="F112" s="5"/>
       <c r="G112" s="6"/>
-      <c r="H112" s="26"/>
-      <c r="I112" s="25"/>
+      <c r="H112" s="56"/>
+      <c r="I112" s="56"/>
       <c r="J112" s="25"/>
-      <c r="K112" s="23"/>
+      <c r="K112" s="57"/>
       <c r="L112" s="24"/>
       <c r="M112" s="24"/>
       <c r="N112" s="1"/>
@@ -4758,10 +4766,10 @@
       <c r="E113" s="4"/>
       <c r="F113" s="5"/>
       <c r="G113" s="6"/>
-      <c r="H113" s="26"/>
-      <c r="I113" s="25"/>
+      <c r="H113" s="56"/>
+      <c r="I113" s="56"/>
       <c r="J113" s="25"/>
-      <c r="K113" s="23"/>
+      <c r="K113" s="57"/>
       <c r="L113" s="24"/>
       <c r="M113" s="24"/>
       <c r="N113" s="1"/>
@@ -4791,10 +4799,10 @@
       <c r="E114" s="4"/>
       <c r="F114" s="5"/>
       <c r="G114" s="6"/>
-      <c r="H114" s="26"/>
-      <c r="I114" s="25"/>
+      <c r="H114" s="56"/>
+      <c r="I114" s="56"/>
       <c r="J114" s="25"/>
-      <c r="K114" s="23"/>
+      <c r="K114" s="57"/>
       <c r="L114" s="24"/>
       <c r="M114" s="24"/>
       <c r="N114" s="1"/>
@@ -4824,10 +4832,10 @@
       <c r="E115" s="4"/>
       <c r="F115" s="5"/>
       <c r="G115" s="6"/>
-      <c r="H115" s="26"/>
-      <c r="I115" s="25"/>
+      <c r="H115" s="56"/>
+      <c r="I115" s="56"/>
       <c r="J115" s="25"/>
-      <c r="K115" s="23"/>
+      <c r="K115" s="57"/>
       <c r="L115" s="24"/>
       <c r="M115" s="24"/>
       <c r="N115" s="1"/>
@@ -4857,10 +4865,10 @@
       <c r="E116" s="4"/>
       <c r="F116" s="5"/>
       <c r="G116" s="6"/>
-      <c r="H116" s="26"/>
-      <c r="I116" s="25"/>
+      <c r="H116" s="56"/>
+      <c r="I116" s="56"/>
       <c r="J116" s="25"/>
-      <c r="K116" s="23"/>
+      <c r="K116" s="57"/>
       <c r="L116" s="24"/>
       <c r="M116" s="24"/>
       <c r="N116" s="1"/>
@@ -4890,10 +4898,10 @@
       <c r="E117" s="4"/>
       <c r="F117" s="5"/>
       <c r="G117" s="6"/>
-      <c r="H117" s="26"/>
-      <c r="I117" s="25"/>
+      <c r="H117" s="56"/>
+      <c r="I117" s="56"/>
       <c r="J117" s="25"/>
-      <c r="K117" s="23"/>
+      <c r="K117" s="57"/>
       <c r="L117" s="24"/>
       <c r="M117" s="24"/>
       <c r="N117" s="1"/>
@@ -4923,10 +4931,10 @@
       <c r="E118" s="4"/>
       <c r="F118" s="5"/>
       <c r="G118" s="6"/>
-      <c r="H118" s="26"/>
-      <c r="I118" s="25"/>
+      <c r="H118" s="56"/>
+      <c r="I118" s="56"/>
       <c r="J118" s="25"/>
-      <c r="K118" s="23"/>
+      <c r="K118" s="57"/>
       <c r="L118" s="24"/>
       <c r="M118" s="24"/>
       <c r="N118" s="1"/>
@@ -4956,10 +4964,10 @@
       <c r="E119" s="4"/>
       <c r="F119" s="5"/>
       <c r="G119" s="6"/>
-      <c r="H119" s="26"/>
-      <c r="I119" s="25"/>
+      <c r="H119" s="56"/>
+      <c r="I119" s="56"/>
       <c r="J119" s="25"/>
-      <c r="K119" s="23"/>
+      <c r="K119" s="57"/>
       <c r="L119" s="24"/>
       <c r="M119" s="24"/>
       <c r="N119" s="1"/>
@@ -4989,10 +4997,10 @@
       <c r="E120" s="4"/>
       <c r="F120" s="5"/>
       <c r="G120" s="6"/>
-      <c r="H120" s="26"/>
-      <c r="I120" s="25"/>
+      <c r="H120" s="56"/>
+      <c r="I120" s="56"/>
       <c r="J120" s="25"/>
-      <c r="K120" s="23"/>
+      <c r="K120" s="57"/>
       <c r="L120" s="24"/>
       <c r="M120" s="24"/>
       <c r="N120" s="1"/>
@@ -5022,10 +5030,10 @@
       <c r="E121" s="4"/>
       <c r="F121" s="5"/>
       <c r="G121" s="6"/>
-      <c r="H121" s="26"/>
-      <c r="I121" s="25"/>
+      <c r="H121" s="56"/>
+      <c r="I121" s="56"/>
       <c r="J121" s="25"/>
-      <c r="K121" s="23"/>
+      <c r="K121" s="57"/>
       <c r="L121" s="24"/>
       <c r="M121" s="24"/>
       <c r="N121" s="1"/>
@@ -5055,10 +5063,10 @@
       <c r="E122" s="4"/>
       <c r="F122" s="5"/>
       <c r="G122" s="6"/>
-      <c r="H122" s="26"/>
-      <c r="I122" s="25"/>
+      <c r="H122" s="56"/>
+      <c r="I122" s="56"/>
       <c r="J122" s="25"/>
-      <c r="K122" s="23"/>
+      <c r="K122" s="57"/>
       <c r="L122" s="24"/>
       <c r="M122" s="24"/>
       <c r="N122" s="1"/>
@@ -5088,10 +5096,10 @@
       <c r="E123" s="4"/>
       <c r="F123" s="5"/>
       <c r="G123" s="6"/>
-      <c r="H123" s="26"/>
-      <c r="I123" s="25"/>
+      <c r="H123" s="56"/>
+      <c r="I123" s="56"/>
       <c r="J123" s="25"/>
-      <c r="K123" s="23"/>
+      <c r="K123" s="57"/>
       <c r="L123" s="24"/>
       <c r="M123" s="24"/>
       <c r="N123" s="1"/>
@@ -5121,10 +5129,10 @@
       <c r="E124" s="4"/>
       <c r="F124" s="5"/>
       <c r="G124" s="6"/>
-      <c r="H124" s="26"/>
-      <c r="I124" s="25"/>
+      <c r="H124" s="56"/>
+      <c r="I124" s="56"/>
       <c r="J124" s="25"/>
-      <c r="K124" s="23"/>
+      <c r="K124" s="57"/>
       <c r="L124" s="24"/>
       <c r="M124" s="24"/>
       <c r="N124" s="1"/>
@@ -5154,10 +5162,10 @@
       <c r="E125" s="4"/>
       <c r="F125" s="5"/>
       <c r="G125" s="6"/>
-      <c r="H125" s="26"/>
-      <c r="I125" s="25"/>
+      <c r="H125" s="56"/>
+      <c r="I125" s="56"/>
       <c r="J125" s="25"/>
-      <c r="K125" s="23"/>
+      <c r="K125" s="57"/>
       <c r="L125" s="24"/>
       <c r="M125" s="24"/>
       <c r="N125" s="1"/>
@@ -5187,10 +5195,10 @@
       <c r="E126" s="4"/>
       <c r="F126" s="5"/>
       <c r="G126" s="6"/>
-      <c r="H126" s="26"/>
-      <c r="I126" s="25"/>
+      <c r="H126" s="56"/>
+      <c r="I126" s="56"/>
       <c r="J126" s="25"/>
-      <c r="K126" s="23"/>
+      <c r="K126" s="57"/>
       <c r="L126" s="24"/>
       <c r="M126" s="24"/>
       <c r="N126" s="1"/>
@@ -5220,10 +5228,10 @@
       <c r="E127" s="4"/>
       <c r="F127" s="5"/>
       <c r="G127" s="6"/>
-      <c r="H127" s="26"/>
-      <c r="I127" s="25"/>
+      <c r="H127" s="56"/>
+      <c r="I127" s="56"/>
       <c r="J127" s="25"/>
-      <c r="K127" s="23"/>
+      <c r="K127" s="57"/>
       <c r="L127" s="24"/>
       <c r="M127" s="24"/>
       <c r="N127" s="1"/>
@@ -5253,10 +5261,10 @@
       <c r="E128" s="4"/>
       <c r="F128" s="5"/>
       <c r="G128" s="6"/>
-      <c r="H128" s="26"/>
-      <c r="I128" s="25"/>
+      <c r="H128" s="56"/>
+      <c r="I128" s="56"/>
       <c r="J128" s="25"/>
-      <c r="K128" s="23"/>
+      <c r="K128" s="57"/>
       <c r="L128" s="24"/>
       <c r="M128" s="24"/>
       <c r="N128" s="1"/>
@@ -5286,10 +5294,10 @@
       <c r="E129" s="4"/>
       <c r="F129" s="5"/>
       <c r="G129" s="6"/>
-      <c r="H129" s="26"/>
-      <c r="I129" s="25"/>
+      <c r="H129" s="56"/>
+      <c r="I129" s="56"/>
       <c r="J129" s="25"/>
-      <c r="K129" s="23"/>
+      <c r="K129" s="57"/>
       <c r="L129" s="24"/>
       <c r="M129" s="24"/>
       <c r="N129" s="1"/>
@@ -5319,10 +5327,10 @@
       <c r="E130" s="4"/>
       <c r="F130" s="5"/>
       <c r="G130" s="6"/>
-      <c r="H130" s="26"/>
-      <c r="I130" s="25"/>
+      <c r="H130" s="56"/>
+      <c r="I130" s="56"/>
       <c r="J130" s="25"/>
-      <c r="K130" s="23"/>
+      <c r="K130" s="57"/>
       <c r="L130" s="24"/>
       <c r="M130" s="24"/>
       <c r="N130" s="1"/>
@@ -5352,10 +5360,10 @@
       <c r="E131" s="4"/>
       <c r="F131" s="5"/>
       <c r="G131" s="6"/>
-      <c r="H131" s="26"/>
-      <c r="I131" s="25"/>
+      <c r="H131" s="56"/>
+      <c r="I131" s="56"/>
       <c r="J131" s="25"/>
-      <c r="K131" s="23"/>
+      <c r="K131" s="57"/>
       <c r="L131" s="24"/>
       <c r="M131" s="24"/>
       <c r="N131" s="1"/>
@@ -5385,10 +5393,10 @@
       <c r="E132" s="4"/>
       <c r="F132" s="5"/>
       <c r="G132" s="6"/>
-      <c r="H132" s="26"/>
-      <c r="I132" s="25"/>
+      <c r="H132" s="56"/>
+      <c r="I132" s="56"/>
       <c r="J132" s="25"/>
-      <c r="K132" s="23"/>
+      <c r="K132" s="57"/>
       <c r="L132" s="24"/>
       <c r="M132" s="24"/>
       <c r="N132" s="1"/>
@@ -5418,10 +5426,10 @@
       <c r="E133" s="4"/>
       <c r="F133" s="5"/>
       <c r="G133" s="6"/>
-      <c r="H133" s="26"/>
-      <c r="I133" s="25"/>
+      <c r="H133" s="56"/>
+      <c r="I133" s="56"/>
       <c r="J133" s="25"/>
-      <c r="K133" s="23"/>
+      <c r="K133" s="57"/>
       <c r="L133" s="24"/>
       <c r="M133" s="24"/>
       <c r="N133" s="1"/>
@@ -5451,10 +5459,10 @@
       <c r="E134" s="4"/>
       <c r="F134" s="5"/>
       <c r="G134" s="6"/>
-      <c r="H134" s="26"/>
-      <c r="I134" s="25"/>
+      <c r="H134" s="56"/>
+      <c r="I134" s="56"/>
       <c r="J134" s="25"/>
-      <c r="K134" s="23"/>
+      <c r="K134" s="57"/>
       <c r="L134" s="24"/>
       <c r="M134" s="24"/>
       <c r="N134" s="1"/>
@@ -5484,10 +5492,10 @@
       <c r="E135" s="4"/>
       <c r="F135" s="5"/>
       <c r="G135" s="6"/>
-      <c r="H135" s="26"/>
-      <c r="I135" s="25"/>
+      <c r="H135" s="56"/>
+      <c r="I135" s="56"/>
       <c r="J135" s="25"/>
-      <c r="K135" s="23"/>
+      <c r="K135" s="57"/>
       <c r="L135" s="24"/>
       <c r="M135" s="24"/>
       <c r="N135" s="1"/>
@@ -5517,10 +5525,10 @@
       <c r="E136" s="4"/>
       <c r="F136" s="5"/>
       <c r="G136" s="6"/>
-      <c r="H136" s="26"/>
-      <c r="I136" s="25"/>
+      <c r="H136" s="56"/>
+      <c r="I136" s="56"/>
       <c r="J136" s="25"/>
-      <c r="K136" s="23"/>
+      <c r="K136" s="57"/>
       <c r="L136" s="24"/>
       <c r="M136" s="24"/>
       <c r="N136" s="1"/>
@@ -5550,10 +5558,10 @@
       <c r="E137" s="4"/>
       <c r="F137" s="5"/>
       <c r="G137" s="6"/>
-      <c r="H137" s="26"/>
-      <c r="I137" s="25"/>
+      <c r="H137" s="56"/>
+      <c r="I137" s="56"/>
       <c r="J137" s="25"/>
-      <c r="K137" s="23"/>
+      <c r="K137" s="57"/>
       <c r="L137" s="24"/>
       <c r="M137" s="24"/>
       <c r="N137" s="1"/>
@@ -5583,10 +5591,10 @@
       <c r="E138" s="4"/>
       <c r="F138" s="5"/>
       <c r="G138" s="6"/>
-      <c r="H138" s="26"/>
-      <c r="I138" s="25"/>
+      <c r="H138" s="56"/>
+      <c r="I138" s="56"/>
       <c r="J138" s="25"/>
-      <c r="K138" s="23"/>
+      <c r="K138" s="57"/>
       <c r="L138" s="24"/>
       <c r="M138" s="24"/>
       <c r="N138" s="1"/>
@@ -5616,10 +5624,10 @@
       <c r="E139" s="4"/>
       <c r="F139" s="5"/>
       <c r="G139" s="6"/>
-      <c r="H139" s="26"/>
-      <c r="I139" s="25"/>
+      <c r="H139" s="56"/>
+      <c r="I139" s="56"/>
       <c r="J139" s="25"/>
-      <c r="K139" s="23"/>
+      <c r="K139" s="57"/>
       <c r="L139" s="24"/>
       <c r="M139" s="24"/>
       <c r="N139" s="1"/>
@@ -5649,10 +5657,10 @@
       <c r="E140" s="4"/>
       <c r="F140" s="5"/>
       <c r="G140" s="6"/>
-      <c r="H140" s="26"/>
-      <c r="I140" s="25"/>
+      <c r="H140" s="56"/>
+      <c r="I140" s="56"/>
       <c r="J140" s="25"/>
-      <c r="K140" s="23"/>
+      <c r="K140" s="57"/>
       <c r="L140" s="24"/>
       <c r="M140" s="24"/>
       <c r="N140" s="1"/>
@@ -5682,10 +5690,10 @@
       <c r="E141" s="4"/>
       <c r="F141" s="5"/>
       <c r="G141" s="6"/>
-      <c r="H141" s="26"/>
-      <c r="I141" s="25"/>
+      <c r="H141" s="56"/>
+      <c r="I141" s="56"/>
       <c r="J141" s="25"/>
-      <c r="K141" s="23"/>
+      <c r="K141" s="57"/>
       <c r="L141" s="24"/>
       <c r="M141" s="24"/>
       <c r="N141" s="1"/>
@@ -5715,10 +5723,10 @@
       <c r="E142" s="4"/>
       <c r="F142" s="5"/>
       <c r="G142" s="6"/>
-      <c r="H142" s="26"/>
-      <c r="I142" s="25"/>
+      <c r="H142" s="56"/>
+      <c r="I142" s="56"/>
       <c r="J142" s="25"/>
-      <c r="K142" s="23"/>
+      <c r="K142" s="57"/>
       <c r="L142" s="24"/>
       <c r="M142" s="24"/>
       <c r="N142" s="1"/>
@@ -5748,10 +5756,10 @@
       <c r="E143" s="4"/>
       <c r="F143" s="5"/>
       <c r="G143" s="6"/>
-      <c r="H143" s="26"/>
-      <c r="I143" s="25"/>
+      <c r="H143" s="56"/>
+      <c r="I143" s="56"/>
       <c r="J143" s="25"/>
-      <c r="K143" s="23"/>
+      <c r="K143" s="57"/>
       <c r="L143" s="24"/>
       <c r="M143" s="24"/>
       <c r="N143" s="1"/>
@@ -5781,10 +5789,10 @@
       <c r="E144" s="4"/>
       <c r="F144" s="5"/>
       <c r="G144" s="6"/>
-      <c r="H144" s="26"/>
-      <c r="I144" s="25"/>
+      <c r="H144" s="56"/>
+      <c r="I144" s="56"/>
       <c r="J144" s="25"/>
-      <c r="K144" s="23"/>
+      <c r="K144" s="57"/>
       <c r="L144" s="24"/>
       <c r="M144" s="24"/>
       <c r="N144" s="1"/>
@@ -5814,10 +5822,10 @@
       <c r="E145" s="4"/>
       <c r="F145" s="5"/>
       <c r="G145" s="6"/>
-      <c r="H145" s="26"/>
-      <c r="I145" s="25"/>
+      <c r="H145" s="56"/>
+      <c r="I145" s="56"/>
       <c r="J145" s="25"/>
-      <c r="K145" s="23"/>
+      <c r="K145" s="57"/>
       <c r="L145" s="24"/>
       <c r="M145" s="24"/>
       <c r="N145" s="1"/>
@@ -5847,10 +5855,10 @@
       <c r="E146" s="4"/>
       <c r="F146" s="5"/>
       <c r="G146" s="6"/>
-      <c r="H146" s="26"/>
-      <c r="I146" s="25"/>
+      <c r="H146" s="56"/>
+      <c r="I146" s="56"/>
       <c r="J146" s="25"/>
-      <c r="K146" s="23"/>
+      <c r="K146" s="57"/>
       <c r="L146" s="24"/>
       <c r="M146" s="24"/>
       <c r="N146" s="1"/>
@@ -5880,10 +5888,10 @@
       <c r="E147" s="4"/>
       <c r="F147" s="5"/>
       <c r="G147" s="6"/>
-      <c r="H147" s="26"/>
-      <c r="I147" s="25"/>
+      <c r="H147" s="56"/>
+      <c r="I147" s="56"/>
       <c r="J147" s="25"/>
-      <c r="K147" s="23"/>
+      <c r="K147" s="57"/>
       <c r="L147" s="24"/>
       <c r="M147" s="24"/>
       <c r="N147" s="1"/>
@@ -5913,10 +5921,10 @@
       <c r="E148" s="4"/>
       <c r="F148" s="5"/>
       <c r="G148" s="6"/>
-      <c r="H148" s="26"/>
-      <c r="I148" s="25"/>
+      <c r="H148" s="56"/>
+      <c r="I148" s="56"/>
       <c r="J148" s="25"/>
-      <c r="K148" s="23"/>
+      <c r="K148" s="57"/>
       <c r="L148" s="24"/>
       <c r="M148" s="24"/>
       <c r="N148" s="1"/>
@@ -5946,10 +5954,10 @@
       <c r="E149" s="4"/>
       <c r="F149" s="5"/>
       <c r="G149" s="6"/>
-      <c r="H149" s="26"/>
-      <c r="I149" s="25"/>
+      <c r="H149" s="56"/>
+      <c r="I149" s="56"/>
       <c r="J149" s="25"/>
-      <c r="K149" s="23"/>
+      <c r="K149" s="57"/>
       <c r="L149" s="24"/>
       <c r="M149" s="24"/>
       <c r="N149" s="1"/>
@@ -5979,10 +5987,10 @@
       <c r="E150" s="4"/>
       <c r="F150" s="5"/>
       <c r="G150" s="6"/>
-      <c r="H150" s="26"/>
-      <c r="I150" s="25"/>
+      <c r="H150" s="56"/>
+      <c r="I150" s="56"/>
       <c r="J150" s="25"/>
-      <c r="K150" s="23"/>
+      <c r="K150" s="57"/>
       <c r="L150" s="24"/>
       <c r="M150" s="24"/>
       <c r="N150" s="1"/>
@@ -6012,10 +6020,10 @@
       <c r="E151" s="4"/>
       <c r="F151" s="5"/>
       <c r="G151" s="6"/>
-      <c r="H151" s="26"/>
-      <c r="I151" s="25"/>
+      <c r="H151" s="56"/>
+      <c r="I151" s="56"/>
       <c r="J151" s="25"/>
-      <c r="K151" s="23"/>
+      <c r="K151" s="57"/>
       <c r="L151" s="24"/>
       <c r="M151" s="24"/>
       <c r="N151" s="1"/>
@@ -6045,10 +6053,10 @@
       <c r="E152" s="4"/>
       <c r="F152" s="5"/>
       <c r="G152" s="6"/>
-      <c r="H152" s="26"/>
-      <c r="I152" s="25"/>
+      <c r="H152" s="56"/>
+      <c r="I152" s="56"/>
       <c r="J152" s="25"/>
-      <c r="K152" s="23"/>
+      <c r="K152" s="57"/>
       <c r="L152" s="24"/>
       <c r="M152" s="24"/>
       <c r="N152" s="1"/>
@@ -6078,10 +6086,10 @@
       <c r="E153" s="4"/>
       <c r="F153" s="5"/>
       <c r="G153" s="6"/>
-      <c r="H153" s="26"/>
-      <c r="I153" s="25"/>
+      <c r="H153" s="56"/>
+      <c r="I153" s="56"/>
       <c r="J153" s="25"/>
-      <c r="K153" s="23"/>
+      <c r="K153" s="57"/>
       <c r="L153" s="24"/>
       <c r="M153" s="24"/>
       <c r="N153" s="1"/>
@@ -6111,10 +6119,10 @@
       <c r="E154" s="4"/>
       <c r="F154" s="5"/>
       <c r="G154" s="6"/>
-      <c r="H154" s="26"/>
-      <c r="I154" s="25"/>
+      <c r="H154" s="56"/>
+      <c r="I154" s="56"/>
       <c r="J154" s="25"/>
-      <c r="K154" s="23"/>
+      <c r="K154" s="57"/>
       <c r="L154" s="24"/>
       <c r="M154" s="24"/>
       <c r="N154" s="1"/>
@@ -6144,10 +6152,10 @@
       <c r="E155" s="4"/>
       <c r="F155" s="5"/>
       <c r="G155" s="6"/>
-      <c r="H155" s="26"/>
-      <c r="I155" s="25"/>
+      <c r="H155" s="56"/>
+      <c r="I155" s="56"/>
       <c r="J155" s="25"/>
-      <c r="K155" s="23"/>
+      <c r="K155" s="57"/>
       <c r="L155" s="24"/>
       <c r="M155" s="24"/>
       <c r="N155" s="1"/>
@@ -6177,10 +6185,10 @@
       <c r="E156" s="4"/>
       <c r="F156" s="5"/>
       <c r="G156" s="6"/>
-      <c r="H156" s="26"/>
-      <c r="I156" s="25"/>
+      <c r="H156" s="56"/>
+      <c r="I156" s="56"/>
       <c r="J156" s="25"/>
-      <c r="K156" s="23"/>
+      <c r="K156" s="57"/>
       <c r="L156" s="24"/>
       <c r="M156" s="24"/>
       <c r="N156" s="1"/>
@@ -6210,10 +6218,10 @@
       <c r="E157" s="4"/>
       <c r="F157" s="5"/>
       <c r="G157" s="6"/>
-      <c r="H157" s="26"/>
-      <c r="I157" s="25"/>
+      <c r="H157" s="56"/>
+      <c r="I157" s="56"/>
       <c r="J157" s="25"/>
-      <c r="K157" s="23"/>
+      <c r="K157" s="57"/>
       <c r="L157" s="24"/>
       <c r="M157" s="24"/>
       <c r="N157" s="1"/>
@@ -6243,10 +6251,10 @@
       <c r="E158" s="4"/>
       <c r="F158" s="5"/>
       <c r="G158" s="6"/>
-      <c r="H158" s="26"/>
-      <c r="I158" s="25"/>
+      <c r="H158" s="56"/>
+      <c r="I158" s="56"/>
       <c r="J158" s="25"/>
-      <c r="K158" s="23"/>
+      <c r="K158" s="57"/>
       <c r="L158" s="24"/>
       <c r="M158" s="24"/>
       <c r="N158" s="1"/>
@@ -6276,10 +6284,10 @@
       <c r="E159" s="4"/>
       <c r="F159" s="5"/>
       <c r="G159" s="6"/>
-      <c r="H159" s="26"/>
-      <c r="I159" s="25"/>
+      <c r="H159" s="56"/>
+      <c r="I159" s="56"/>
       <c r="J159" s="25"/>
-      <c r="K159" s="23"/>
+      <c r="K159" s="57"/>
       <c r="L159" s="24"/>
       <c r="M159" s="24"/>
       <c r="N159" s="1"/>
@@ -6309,10 +6317,10 @@
       <c r="E160" s="4"/>
       <c r="F160" s="5"/>
       <c r="G160" s="6"/>
-      <c r="H160" s="26"/>
-      <c r="I160" s="25"/>
+      <c r="H160" s="56"/>
+      <c r="I160" s="56"/>
       <c r="J160" s="25"/>
-      <c r="K160" s="23"/>
+      <c r="K160" s="57"/>
       <c r="L160" s="24"/>
       <c r="M160" s="24"/>
       <c r="N160" s="1"/>
@@ -6342,10 +6350,10 @@
       <c r="E161" s="4"/>
       <c r="F161" s="5"/>
       <c r="G161" s="6"/>
-      <c r="H161" s="26"/>
-      <c r="I161" s="25"/>
+      <c r="H161" s="56"/>
+      <c r="I161" s="56"/>
       <c r="J161" s="25"/>
-      <c r="K161" s="23"/>
+      <c r="K161" s="57"/>
       <c r="L161" s="24"/>
       <c r="M161" s="24"/>
       <c r="N161" s="1"/>
@@ -6375,10 +6383,10 @@
       <c r="E162" s="4"/>
       <c r="F162" s="5"/>
       <c r="G162" s="6"/>
-      <c r="H162" s="26"/>
-      <c r="I162" s="25"/>
+      <c r="H162" s="56"/>
+      <c r="I162" s="56"/>
       <c r="J162" s="25"/>
-      <c r="K162" s="23"/>
+      <c r="K162" s="57"/>
       <c r="L162" s="24"/>
       <c r="M162" s="24"/>
       <c r="N162" s="1"/>
@@ -6408,10 +6416,10 @@
       <c r="E163" s="4"/>
       <c r="F163" s="5"/>
       <c r="G163" s="6"/>
-      <c r="H163" s="26"/>
-      <c r="I163" s="25"/>
+      <c r="H163" s="56"/>
+      <c r="I163" s="56"/>
       <c r="J163" s="25"/>
-      <c r="K163" s="23"/>
+      <c r="K163" s="57"/>
       <c r="L163" s="24"/>
       <c r="M163" s="24"/>
       <c r="N163" s="1"/>
@@ -6441,10 +6449,10 @@
       <c r="E164" s="4"/>
       <c r="F164" s="5"/>
       <c r="G164" s="6"/>
-      <c r="H164" s="26"/>
-      <c r="I164" s="25"/>
+      <c r="H164" s="56"/>
+      <c r="I164" s="56"/>
       <c r="J164" s="25"/>
-      <c r="K164" s="23"/>
+      <c r="K164" s="57"/>
       <c r="L164" s="24"/>
       <c r="M164" s="24"/>
       <c r="N164" s="1"/>
@@ -6474,10 +6482,10 @@
       <c r="E165" s="4"/>
       <c r="F165" s="5"/>
       <c r="G165" s="6"/>
-      <c r="H165" s="26"/>
-      <c r="I165" s="25"/>
+      <c r="H165" s="56"/>
+      <c r="I165" s="56"/>
       <c r="J165" s="25"/>
-      <c r="K165" s="23"/>
+      <c r="K165" s="57"/>
       <c r="L165" s="24"/>
       <c r="M165" s="24"/>
       <c r="N165" s="1"/>
@@ -6507,10 +6515,10 @@
       <c r="E166" s="4"/>
       <c r="F166" s="5"/>
       <c r="G166" s="6"/>
-      <c r="H166" s="26"/>
-      <c r="I166" s="25"/>
+      <c r="H166" s="56"/>
+      <c r="I166" s="56"/>
       <c r="J166" s="25"/>
-      <c r="K166" s="23"/>
+      <c r="K166" s="57"/>
       <c r="L166" s="24"/>
       <c r="M166" s="24"/>
       <c r="N166" s="1"/>
@@ -6540,10 +6548,10 @@
       <c r="E167" s="4"/>
       <c r="F167" s="5"/>
       <c r="G167" s="6"/>
-      <c r="H167" s="26"/>
-      <c r="I167" s="25"/>
+      <c r="H167" s="56"/>
+      <c r="I167" s="56"/>
       <c r="J167" s="25"/>
-      <c r="K167" s="23"/>
+      <c r="K167" s="57"/>
       <c r="L167" s="24"/>
       <c r="M167" s="24"/>
       <c r="N167" s="1"/>
@@ -6573,10 +6581,10 @@
       <c r="E168" s="4"/>
       <c r="F168" s="5"/>
       <c r="G168" s="6"/>
-      <c r="H168" s="26"/>
-      <c r="I168" s="25"/>
+      <c r="H168" s="56"/>
+      <c r="I168" s="56"/>
       <c r="J168" s="25"/>
-      <c r="K168" s="23"/>
+      <c r="K168" s="57"/>
       <c r="L168" s="24"/>
       <c r="M168" s="24"/>
       <c r="N168" s="1"/>
@@ -6606,10 +6614,10 @@
       <c r="E169" s="4"/>
       <c r="F169" s="5"/>
       <c r="G169" s="6"/>
-      <c r="H169" s="26"/>
-      <c r="I169" s="25"/>
+      <c r="H169" s="56"/>
+      <c r="I169" s="56"/>
       <c r="J169" s="25"/>
-      <c r="K169" s="23"/>
+      <c r="K169" s="57"/>
       <c r="L169" s="24"/>
       <c r="M169" s="24"/>
       <c r="N169" s="1"/>
@@ -6639,10 +6647,10 @@
       <c r="E170" s="4"/>
       <c r="F170" s="5"/>
       <c r="G170" s="6"/>
-      <c r="H170" s="26"/>
-      <c r="I170" s="25"/>
+      <c r="H170" s="56"/>
+      <c r="I170" s="56"/>
       <c r="J170" s="25"/>
-      <c r="K170" s="23"/>
+      <c r="K170" s="57"/>
       <c r="L170" s="24"/>
       <c r="M170" s="24"/>
       <c r="N170" s="1"/>
@@ -6672,10 +6680,10 @@
       <c r="E171" s="4"/>
       <c r="F171" s="5"/>
       <c r="G171" s="6"/>
-      <c r="H171" s="26"/>
-      <c r="I171" s="25"/>
+      <c r="H171" s="56"/>
+      <c r="I171" s="56"/>
       <c r="J171" s="25"/>
-      <c r="K171" s="23"/>
+      <c r="K171" s="57"/>
       <c r="L171" s="24"/>
       <c r="M171" s="24"/>
       <c r="N171" s="1"/>
@@ -6705,10 +6713,10 @@
       <c r="E172" s="4"/>
       <c r="F172" s="5"/>
       <c r="G172" s="6"/>
-      <c r="H172" s="26"/>
-      <c r="I172" s="25"/>
+      <c r="H172" s="56"/>
+      <c r="I172" s="56"/>
       <c r="J172" s="25"/>
-      <c r="K172" s="23"/>
+      <c r="K172" s="57"/>
       <c r="L172" s="24"/>
       <c r="M172" s="24"/>
       <c r="N172" s="1"/>
@@ -6738,10 +6746,10 @@
       <c r="E173" s="4"/>
       <c r="F173" s="5"/>
       <c r="G173" s="6"/>
-      <c r="H173" s="26"/>
-      <c r="I173" s="25"/>
+      <c r="H173" s="56"/>
+      <c r="I173" s="56"/>
       <c r="J173" s="25"/>
-      <c r="K173" s="23"/>
+      <c r="K173" s="57"/>
       <c r="L173" s="24"/>
       <c r="M173" s="24"/>
       <c r="N173" s="1"/>
@@ -6771,10 +6779,10 @@
       <c r="E174" s="4"/>
       <c r="F174" s="5"/>
       <c r="G174" s="6"/>
-      <c r="H174" s="26"/>
-      <c r="I174" s="25"/>
+      <c r="H174" s="56"/>
+      <c r="I174" s="56"/>
       <c r="J174" s="25"/>
-      <c r="K174" s="23"/>
+      <c r="K174" s="57"/>
       <c r="L174" s="24"/>
       <c r="M174" s="24"/>
       <c r="N174" s="1"/>
@@ -6804,10 +6812,10 @@
       <c r="E175" s="4"/>
       <c r="F175" s="5"/>
       <c r="G175" s="6"/>
-      <c r="H175" s="26"/>
-      <c r="I175" s="25"/>
+      <c r="H175" s="56"/>
+      <c r="I175" s="56"/>
       <c r="J175" s="25"/>
-      <c r="K175" s="23"/>
+      <c r="K175" s="57"/>
       <c r="L175" s="24"/>
       <c r="M175" s="24"/>
       <c r="N175" s="1"/>
@@ -6837,10 +6845,10 @@
       <c r="E176" s="4"/>
       <c r="F176" s="5"/>
       <c r="G176" s="6"/>
-      <c r="H176" s="26"/>
-      <c r="I176" s="25"/>
+      <c r="H176" s="56"/>
+      <c r="I176" s="56"/>
       <c r="J176" s="25"/>
-      <c r="K176" s="23"/>
+      <c r="K176" s="57"/>
       <c r="L176" s="24"/>
       <c r="M176" s="24"/>
       <c r="N176" s="1"/>
@@ -6870,10 +6878,10 @@
       <c r="E177" s="4"/>
       <c r="F177" s="5"/>
       <c r="G177" s="6"/>
-      <c r="H177" s="26"/>
-      <c r="I177" s="25"/>
+      <c r="H177" s="56"/>
+      <c r="I177" s="56"/>
       <c r="J177" s="25"/>
-      <c r="K177" s="23"/>
+      <c r="K177" s="57"/>
       <c r="L177" s="24"/>
       <c r="M177" s="24"/>
       <c r="N177" s="1"/>
@@ -6903,10 +6911,10 @@
       <c r="E178" s="4"/>
       <c r="F178" s="5"/>
       <c r="G178" s="6"/>
-      <c r="H178" s="26"/>
-      <c r="I178" s="25"/>
+      <c r="H178" s="56"/>
+      <c r="I178" s="56"/>
       <c r="J178" s="25"/>
-      <c r="K178" s="23"/>
+      <c r="K178" s="57"/>
       <c r="L178" s="24"/>
       <c r="M178" s="24"/>
       <c r="N178" s="1"/>
@@ -6936,10 +6944,10 @@
       <c r="E179" s="4"/>
       <c r="F179" s="5"/>
       <c r="G179" s="6"/>
-      <c r="H179" s="26"/>
-      <c r="I179" s="25"/>
+      <c r="H179" s="56"/>
+      <c r="I179" s="56"/>
       <c r="J179" s="25"/>
-      <c r="K179" s="23"/>
+      <c r="K179" s="57"/>
       <c r="L179" s="24"/>
       <c r="M179" s="24"/>
       <c r="N179" s="1"/>
@@ -6969,10 +6977,10 @@
       <c r="E180" s="4"/>
       <c r="F180" s="5"/>
       <c r="G180" s="6"/>
-      <c r="H180" s="26"/>
-      <c r="I180" s="25"/>
+      <c r="H180" s="56"/>
+      <c r="I180" s="56"/>
       <c r="J180" s="25"/>
-      <c r="K180" s="23"/>
+      <c r="K180" s="57"/>
       <c r="L180" s="24"/>
       <c r="M180" s="24"/>
       <c r="N180" s="1"/>
@@ -7002,10 +7010,10 @@
       <c r="E181" s="4"/>
       <c r="F181" s="5"/>
       <c r="G181" s="6"/>
-      <c r="H181" s="26"/>
-      <c r="I181" s="25"/>
+      <c r="H181" s="56"/>
+      <c r="I181" s="56"/>
       <c r="J181" s="25"/>
-      <c r="K181" s="23"/>
+      <c r="K181" s="57"/>
       <c r="L181" s="24"/>
       <c r="M181" s="24"/>
       <c r="N181" s="1"/>
@@ -7035,10 +7043,10 @@
       <c r="E182" s="4"/>
       <c r="F182" s="5"/>
       <c r="G182" s="6"/>
-      <c r="H182" s="26"/>
-      <c r="I182" s="25"/>
+      <c r="H182" s="56"/>
+      <c r="I182" s="56"/>
       <c r="J182" s="25"/>
-      <c r="K182" s="23"/>
+      <c r="K182" s="57"/>
       <c r="L182" s="24"/>
       <c r="M182" s="24"/>
       <c r="N182" s="1"/>
@@ -7068,10 +7076,10 @@
       <c r="E183" s="4"/>
       <c r="F183" s="5"/>
       <c r="G183" s="6"/>
-      <c r="H183" s="26"/>
-      <c r="I183" s="25"/>
+      <c r="H183" s="56"/>
+      <c r="I183" s="56"/>
       <c r="J183" s="25"/>
-      <c r="K183" s="23"/>
+      <c r="K183" s="57"/>
       <c r="L183" s="24"/>
       <c r="M183" s="24"/>
       <c r="N183" s="1"/>
@@ -7101,10 +7109,10 @@
       <c r="E184" s="4"/>
       <c r="F184" s="5"/>
       <c r="G184" s="6"/>
-      <c r="H184" s="26"/>
-      <c r="I184" s="25"/>
+      <c r="H184" s="56"/>
+      <c r="I184" s="56"/>
       <c r="J184" s="25"/>
-      <c r="K184" s="23"/>
+      <c r="K184" s="57"/>
       <c r="L184" s="24"/>
       <c r="M184" s="24"/>
       <c r="N184" s="1"/>
@@ -7134,10 +7142,10 @@
       <c r="E185" s="4"/>
       <c r="F185" s="5"/>
       <c r="G185" s="6"/>
-      <c r="H185" s="26"/>
-      <c r="I185" s="25"/>
+      <c r="H185" s="56"/>
+      <c r="I185" s="56"/>
       <c r="J185" s="25"/>
-      <c r="K185" s="23"/>
+      <c r="K185" s="57"/>
       <c r="L185" s="24"/>
       <c r="M185" s="24"/>
       <c r="N185" s="1"/>
@@ -7167,10 +7175,10 @@
       <c r="E186" s="4"/>
       <c r="F186" s="5"/>
       <c r="G186" s="6"/>
-      <c r="H186" s="26"/>
-      <c r="I186" s="25"/>
+      <c r="H186" s="56"/>
+      <c r="I186" s="56"/>
       <c r="J186" s="25"/>
-      <c r="K186" s="23"/>
+      <c r="K186" s="57"/>
       <c r="L186" s="24"/>
       <c r="M186" s="24"/>
       <c r="N186" s="1"/>
@@ -7200,10 +7208,10 @@
       <c r="E187" s="4"/>
       <c r="F187" s="5"/>
       <c r="G187" s="6"/>
-      <c r="H187" s="26"/>
-      <c r="I187" s="25"/>
+      <c r="H187" s="56"/>
+      <c r="I187" s="56"/>
       <c r="J187" s="25"/>
-      <c r="K187" s="23"/>
+      <c r="K187" s="57"/>
       <c r="L187" s="24"/>
       <c r="M187" s="24"/>
       <c r="N187" s="1"/>
@@ -7233,10 +7241,10 @@
       <c r="E188" s="4"/>
       <c r="F188" s="5"/>
       <c r="G188" s="6"/>
-      <c r="H188" s="26"/>
-      <c r="I188" s="25"/>
+      <c r="H188" s="56"/>
+      <c r="I188" s="56"/>
       <c r="J188" s="25"/>
-      <c r="K188" s="23"/>
+      <c r="K188" s="57"/>
       <c r="L188" s="24"/>
       <c r="M188" s="24"/>
       <c r="N188" s="1"/>
@@ -7266,10 +7274,10 @@
       <c r="E189" s="4"/>
       <c r="F189" s="5"/>
       <c r="G189" s="6"/>
-      <c r="H189" s="26"/>
-      <c r="I189" s="25"/>
+      <c r="H189" s="56"/>
+      <c r="I189" s="56"/>
       <c r="J189" s="25"/>
-      <c r="K189" s="23"/>
+      <c r="K189" s="57"/>
       <c r="L189" s="24"/>
       <c r="M189" s="24"/>
       <c r="N189" s="1"/>
@@ -7299,10 +7307,10 @@
       <c r="E190" s="4"/>
       <c r="F190" s="5"/>
       <c r="G190" s="6"/>
-      <c r="H190" s="26"/>
-      <c r="I190" s="25"/>
+      <c r="H190" s="56"/>
+      <c r="I190" s="56"/>
       <c r="J190" s="25"/>
-      <c r="K190" s="23"/>
+      <c r="K190" s="57"/>
       <c r="L190" s="24"/>
       <c r="M190" s="24"/>
       <c r="N190" s="1"/>
@@ -7332,10 +7340,10 @@
       <c r="E191" s="4"/>
       <c r="F191" s="5"/>
       <c r="G191" s="6"/>
-      <c r="H191" s="26"/>
-      <c r="I191" s="25"/>
+      <c r="H191" s="56"/>
+      <c r="I191" s="56"/>
       <c r="J191" s="25"/>
-      <c r="K191" s="23"/>
+      <c r="K191" s="57"/>
       <c r="L191" s="24"/>
       <c r="M191" s="24"/>
       <c r="N191" s="1"/>
@@ -7365,10 +7373,10 @@
       <c r="E192" s="4"/>
       <c r="F192" s="5"/>
       <c r="G192" s="6"/>
-      <c r="H192" s="26"/>
-      <c r="I192" s="25"/>
+      <c r="H192" s="56"/>
+      <c r="I192" s="56"/>
       <c r="J192" s="25"/>
-      <c r="K192" s="23"/>
+      <c r="K192" s="57"/>
       <c r="L192" s="24"/>
       <c r="M192" s="24"/>
       <c r="N192" s="1"/>
@@ -7398,10 +7406,10 @@
       <c r="E193" s="4"/>
       <c r="F193" s="5"/>
       <c r="G193" s="6"/>
-      <c r="H193" s="26"/>
-      <c r="I193" s="25"/>
+      <c r="H193" s="56"/>
+      <c r="I193" s="56"/>
       <c r="J193" s="25"/>
-      <c r="K193" s="23"/>
+      <c r="K193" s="57"/>
       <c r="L193" s="24"/>
       <c r="M193" s="24"/>
       <c r="N193" s="1"/>
@@ -7431,10 +7439,10 @@
       <c r="E194" s="4"/>
       <c r="F194" s="5"/>
       <c r="G194" s="6"/>
-      <c r="H194" s="26"/>
-      <c r="I194" s="25"/>
+      <c r="H194" s="56"/>
+      <c r="I194" s="56"/>
       <c r="J194" s="25"/>
-      <c r="K194" s="23"/>
+      <c r="K194" s="57"/>
       <c r="L194" s="24"/>
       <c r="M194" s="24"/>
       <c r="N194" s="1"/>
@@ -7464,10 +7472,10 @@
       <c r="E195" s="4"/>
       <c r="F195" s="5"/>
       <c r="G195" s="6"/>
-      <c r="H195" s="26"/>
-      <c r="I195" s="25"/>
+      <c r="H195" s="56"/>
+      <c r="I195" s="56"/>
       <c r="J195" s="25"/>
-      <c r="K195" s="23"/>
+      <c r="K195" s="57"/>
       <c r="L195" s="24"/>
       <c r="M195" s="24"/>
       <c r="N195" s="1"/>
@@ -7497,10 +7505,10 @@
       <c r="E196" s="4"/>
       <c r="F196" s="5"/>
       <c r="G196" s="6"/>
-      <c r="H196" s="26"/>
-      <c r="I196" s="25"/>
+      <c r="H196" s="56"/>
+      <c r="I196" s="56"/>
       <c r="J196" s="25"/>
-      <c r="K196" s="23"/>
+      <c r="K196" s="57"/>
       <c r="L196" s="24"/>
       <c r="M196" s="24"/>
       <c r="N196" s="1"/>
@@ -7530,10 +7538,10 @@
       <c r="E197" s="4"/>
       <c r="F197" s="5"/>
       <c r="G197" s="6"/>
-      <c r="H197" s="26"/>
-      <c r="I197" s="25"/>
+      <c r="H197" s="56"/>
+      <c r="I197" s="56"/>
       <c r="J197" s="25"/>
-      <c r="K197" s="23"/>
+      <c r="K197" s="57"/>
       <c r="L197" s="24"/>
       <c r="M197" s="24"/>
       <c r="N197" s="1"/>
@@ -7563,10 +7571,10 @@
       <c r="E198" s="4"/>
       <c r="F198" s="5"/>
       <c r="G198" s="6"/>
-      <c r="H198" s="26"/>
-      <c r="I198" s="25"/>
+      <c r="H198" s="56"/>
+      <c r="I198" s="56"/>
       <c r="J198" s="25"/>
-      <c r="K198" s="23"/>
+      <c r="K198" s="57"/>
       <c r="L198" s="24"/>
       <c r="M198" s="24"/>
       <c r="N198" s="1"/>
@@ -7596,10 +7604,10 @@
       <c r="E199" s="4"/>
       <c r="F199" s="5"/>
       <c r="G199" s="6"/>
-      <c r="H199" s="26"/>
-      <c r="I199" s="25"/>
+      <c r="H199" s="56"/>
+      <c r="I199" s="56"/>
       <c r="J199" s="25"/>
-      <c r="K199" s="23"/>
+      <c r="K199" s="57"/>
       <c r="L199" s="24"/>
       <c r="M199" s="24"/>
       <c r="N199" s="1"/>
@@ -7629,10 +7637,10 @@
       <c r="E200" s="4"/>
       <c r="F200" s="5"/>
       <c r="G200" s="6"/>
-      <c r="H200" s="26"/>
-      <c r="I200" s="25"/>
+      <c r="H200" s="56"/>
+      <c r="I200" s="56"/>
       <c r="J200" s="25"/>
-      <c r="K200" s="23"/>
+      <c r="K200" s="57"/>
       <c r="L200" s="24"/>
       <c r="M200" s="24"/>
       <c r="N200" s="1"/>
@@ -7662,10 +7670,10 @@
       <c r="E201" s="4"/>
       <c r="F201" s="5"/>
       <c r="G201" s="6"/>
-      <c r="H201" s="26"/>
-      <c r="I201" s="25"/>
+      <c r="H201" s="56"/>
+      <c r="I201" s="56"/>
       <c r="J201" s="25"/>
-      <c r="K201" s="23"/>
+      <c r="K201" s="57"/>
       <c r="L201" s="24"/>
       <c r="M201" s="24"/>
       <c r="N201" s="1"/>
@@ -7695,10 +7703,10 @@
       <c r="E202" s="4"/>
       <c r="F202" s="5"/>
       <c r="G202" s="6"/>
-      <c r="H202" s="26"/>
-      <c r="I202" s="25"/>
+      <c r="H202" s="56"/>
+      <c r="I202" s="56"/>
       <c r="J202" s="25"/>
-      <c r="K202" s="23"/>
+      <c r="K202" s="57"/>
       <c r="L202" s="24"/>
       <c r="M202" s="24"/>
       <c r="N202" s="1"/>
@@ -7728,10 +7736,10 @@
       <c r="E203" s="4"/>
       <c r="F203" s="5"/>
       <c r="G203" s="6"/>
-      <c r="H203" s="26"/>
-      <c r="I203" s="25"/>
+      <c r="H203" s="56"/>
+      <c r="I203" s="56"/>
       <c r="J203" s="25"/>
-      <c r="K203" s="23"/>
+      <c r="K203" s="57"/>
       <c r="L203" s="24"/>
       <c r="M203" s="24"/>
       <c r="N203" s="1"/>
@@ -7761,10 +7769,10 @@
       <c r="E204" s="4"/>
       <c r="F204" s="5"/>
       <c r="G204" s="6"/>
-      <c r="H204" s="26"/>
-      <c r="I204" s="25"/>
+      <c r="H204" s="56"/>
+      <c r="I204" s="56"/>
       <c r="J204" s="25"/>
-      <c r="K204" s="23"/>
+      <c r="K204" s="57"/>
       <c r="L204" s="24"/>
       <c r="M204" s="24"/>
       <c r="N204" s="1"/>
@@ -7794,10 +7802,10 @@
       <c r="E205" s="4"/>
       <c r="F205" s="5"/>
       <c r="G205" s="6"/>
-      <c r="H205" s="26"/>
-      <c r="I205" s="25"/>
+      <c r="H205" s="56"/>
+      <c r="I205" s="56"/>
       <c r="J205" s="25"/>
-      <c r="K205" s="23"/>
+      <c r="K205" s="57"/>
       <c r="L205" s="24"/>
       <c r="M205" s="24"/>
       <c r="N205" s="1"/>
@@ -28828,23 +28836,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC984BB-0605-48FE-8CE1-7AAC539A0292}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:I999"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="C1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -28867,13 +28863,13 @@
         <v>16</v>
       </c>
       <c r="D1" s="44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" s="48" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" s="49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G1" s="36" t="s">
         <v>14</v>
@@ -28884,25 +28880,25 @@
     </row>
     <row r="2" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="31" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="D2" s="45" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
-      <c r="E2" s="50" t="s">
-        <v>30</v>
+      <c r="E2" s="62" t="s">
+        <v>34</v>
       </c>
       <c r="F2" s="51" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -28915,8 +28911,8 @@
       <c r="D3" s="46">
         <v>4</v>
       </c>
-      <c r="E3" s="52" t="s">
-        <v>31</v>
+      <c r="E3" s="50" t="s">
+        <v>29</v>
       </c>
       <c r="F3" s="51">
         <v>0.1</v>
@@ -28938,8 +28934,8 @@
       <c r="D4" s="46">
         <v>8</v>
       </c>
-      <c r="E4" s="53" t="s">
-        <v>32</v>
+      <c r="E4" s="52" t="s">
+        <v>30</v>
       </c>
       <c r="F4" s="51">
         <v>0.5</v>
@@ -28962,7 +28958,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="53" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F5" s="51">
         <v>1</v>
@@ -28977,7 +28973,7 @@
         <v>1.5</v>
       </c>
       <c r="E6" s="53" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F6" s="51">
         <v>1.5</v>
@@ -28990,6 +28986,9 @@
     <row r="7" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="41">
         <v>2</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>33</v>
       </c>
       <c r="F7" s="51">
         <v>2</v>

</xml_diff>

<commit_message>
Se crea componente para carga masiva de clientes
</commit_message>
<xml_diff>
--- a/public/DownloadExcels/Equipos_Herramientas_y_Maquinaria.xlsx
+++ b/public/DownloadExcels/Equipos_Herramientas_y_Maquinaria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Mario\Desktop\Ecopcion Desarrollo\ecopFront-Desarrollo\public\DownloadExcels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E7752A-8C6D-428F-805A-6E4A8AF0F8E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457BEDCC-2F2C-4CCF-8A89-83BABFB437F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INVENTARIO DE ACTIVOS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
   <si>
     <t>INVENTARIO DE MAQUINARIA, EQUIPOS Y/O HERRAMIENTAS</t>
   </si>
@@ -130,117 +130,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nunito Sans"/>
-      </rPr>
-      <t xml:space="preserve">1. LAS COLUMNAS EN VERDE SON OBLIGATORIAS. DEBES DILIGENCIAR TODAS LAS COLUMNAS VERDES EN UN 100% PARA QUE PUEDAS HACER LA CARGA MASIVA DEL INVENTARIO EN EL SOFTWARE DE ECOPCIÓN. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nunito Sans"/>
-      </rPr>
-      <t xml:space="preserve">
-2. Escribe el nombre de la máquina, equipo o herramienta </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nunito Sans"/>
-      </rPr>
-      <t>SIEMPRE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nunito Sans"/>
-      </rPr>
-      <t xml:space="preserve"> empezando con letra mayúscula. Las demás letras deben ir en minúscula. 
-3. Si el nombre de la máquina, equipo o herramienta tiene dos palabras, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nunito Sans"/>
-      </rPr>
-      <t>SOLO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nunito Sans"/>
-      </rPr>
-      <t xml:space="preserve"> debes poner en mayúscula la primera letra de la primera palabra.
-4</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nunito Sans"/>
-      </rPr>
-      <t xml:space="preserve">. OBLIGATORIO: En la columna B, REGISTRA LA MÁQUINA, EQUIPO O HERRAMIENTA UNA (1) SOLA VEZ.
-5. OBLIGATORIO: En la columna C, ESCRIBE EL INVENTARIO EN NÚMEROS. 
-6. OBLIGATORIO: En la columna D, ESCRIBE EN NÚMEROS EL PRECIO DE COMPRA ANTES DE IMPUESTOS.  
-7. OBLGATORIO: En la columna E, ELIGE DE LA LISTA DESPLEGABLE, EL PORCENTAJE DEL IVA APLICABLE A TU MÁQUINA, EQUIPO O HERRAMIENTA.  
-8. OBLIGATORIO: En la columna F, ELIGE DE LA LISTA DESPLEGABLE, EL TIPO DE RETENCIÓN EN LA FUENTE APLICABLE A TU PRODUCTO.
-9.  OBLIGATORIO: En la columna G, ELIGE DE LA LISTA DESPLEGABLE, EL TIPO DE RETENCIÓN DE IVA APLICABLE A TU PRODUCTO.
-10.  OBLIGATORIO: En la columna H, ELIGE DE LA LISTA DESPLEGABLE, EL TIPO DE RETENCIÓN DE ICA APLICABLE A TU PRODUCTO. 
-11. OBLIGATORIO: En la cokumna I, COPIA EL CÓDIGO DE BARRAS A MANO O CON EL LECTOR DE CÓDIGO. 
-12. OBLIGATORIO: En la columna J, ESCRIBE LA MARCA. 
-13. OBLIGATORIO: En la columna K, ESCRIBE LA REFERENCIA COMPLETA INCLUYENDO LETRAS, NÚMEROS, SIMBOLOS, MAYÚSCULAS Y/O MINÚSCULAS.
-11. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nunito Sans"/>
-      </rPr>
-      <t>En las columnas</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nunito Sans"/>
-      </rPr>
-      <t xml:space="preserve"> E, F, G y H, ELIGE LA RESPUESTA DE LA LISTA DESPLEGABLE. 
-12. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nunito Sans"/>
-      </rPr>
-      <t>En las columnas</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nunito Sans"/>
-      </rPr>
-      <t xml:space="preserve"> C, D e I, ESCRIBE EL NÚMERO. 
-</t>
-    </r>
-  </si>
-  <si>
     <t>Impuesto al consumo</t>
   </si>
   <si>
@@ -279,6 +168,51 @@
   </si>
   <si>
     <t>No aplica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. LAS COLUMNAS EN VERDE SON OBLIGATORIAS. DEBES DILIGENCIAR TODAS LAS COLUMNAS VERDES EN UN 100% PARA QUE PUEDAS HACER LA CARGA MASIVA DEL INVENTARIO EN EL SOFTWARE DE ECOPCIÓN. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Escribe el nombre de la máquina, equipo o herramienta SIEMPRE empezando con letra mayúscula. Las demás letras deben ir en minúscula. </t>
+  </si>
+  <si>
+    <t>3. Si el nombre de la máquina, equipo o herramienta tiene dos palabras, SOLO debes poner en mayúscula la primera letra de la primera palabra.</t>
+  </si>
+  <si>
+    <t>4. OBLIGATORIO: En la columna B, REGISTRA LA MÁQUINA, EQUIPO O HERRAMIENTA UNA (1) SOLA VEZ.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. OBLIGATORIO: En la columna C, ESCRIBE EL INVENTARIO EN NÚMEROS. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. OBLIGATORIO: En la columna D, ESCRIBE EN NÚMEROS EL PRECIO DE COMPRA ANTES DE IMPUESTOS.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. OBLGATORIO: En la columna E, ELIGE DE LA LISTA DESPLEGABLE, EL PORCENTAJE DEL IVA APLICABLE A TU MÁQUINA, EQUIPO O HERRAMIENTA.  </t>
+  </si>
+  <si>
+    <t>8. OBLIGATORIO: En la columna F, ELIGE DE LA LISTA DESPLEGABLE, EL TIPO DE RETENCIÓN EN LA FUENTE APLICABLE A TU PRODUCTO.</t>
+  </si>
+  <si>
+    <t>9.  OBLIGATORIO: En la columna G, ELIGE DE LA LISTA DESPLEGABLE, EL TIPO DE RETENCIÓN DE IVA APLICABLE A TU PRODUCTO.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.  OBLIGATORIO: En la columna H, ELIGE DE LA LISTA DESPLEGABLE, EL TIPO DE RETENCIÓN DE ICA APLICABLE A TU PRODUCTO. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11. OBLIGATORIO: En la cokumna I, COPIA EL CÓDIGO DE BARRAS A MANO O CON EL LECTOR DE CÓDIGO. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12. OBLIGATORIO: En la columna J, ESCRIBE LA MARCA. </t>
+  </si>
+  <si>
+    <t>13. OBLIGATORIO: En la columna K, ESCRIBE LA REFERENCIA COMPLETA INCLUYENDO LETRAS, NÚMEROS, SIMBOLOS, MAYÚSCULAS Y/O MINÚSCULAS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11. En las columnas E, F, G y H, ELIGE LA RESPUESTA DE LA LISTA DESPLEGABLE. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12. En las columnas C, D e I, ESCRIBE EL NÚMERO. </t>
   </si>
 </sst>
 </file>
@@ -505,7 +439,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -680,12 +614,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -959,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC881"/>
+  <dimension ref="A1:AC879"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:M1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1011,55 +939,101 @@
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
     </row>
-    <row r="2" spans="1:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
-        <v>1</v>
+    <row r="2" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="19" t="s">
+        <v>5</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-    </row>
-    <row r="3" spans="1:29" ht="246.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="C2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
+      <c r="J2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+    </row>
+    <row r="3" spans="1:29" ht="107.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>18</v>
+      </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -1077,101 +1051,55 @@
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
     </row>
-    <row r="4" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="19" t="s">
-        <v>5</v>
+    <row r="4" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>1</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="8" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+    </row>
+    <row r="5" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
         <v>2</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="2"/>
-      <c r="AC4" s="2"/>
-    </row>
-    <row r="5" spans="1:29" ht="107.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5" s="13" t="s">
-        <v>18</v>
-      </c>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -1191,7 +1119,7 @@
     </row>
     <row r="6" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -1201,7 +1129,7 @@
       <c r="G6" s="56"/>
       <c r="H6" s="49"/>
       <c r="I6" s="49"/>
-      <c r="J6" s="17"/>
+      <c r="J6" s="49"/>
       <c r="K6" s="49"/>
       <c r="L6" s="18"/>
       <c r="M6" s="18"/>
@@ -1224,7 +1152,7 @@
     </row>
     <row r="7" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -1234,7 +1162,7 @@
       <c r="G7" s="56"/>
       <c r="H7" s="49"/>
       <c r="I7" s="49"/>
-      <c r="J7" s="17"/>
+      <c r="J7" s="49"/>
       <c r="K7" s="49"/>
       <c r="L7" s="18"/>
       <c r="M7" s="18"/>
@@ -1257,7 +1185,7 @@
     </row>
     <row r="8" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -1267,7 +1195,7 @@
       <c r="G8" s="56"/>
       <c r="H8" s="49"/>
       <c r="I8" s="49"/>
-      <c r="J8" s="17"/>
+      <c r="J8" s="49"/>
       <c r="K8" s="49"/>
       <c r="L8" s="18"/>
       <c r="M8" s="18"/>
@@ -1290,7 +1218,7 @@
     </row>
     <row r="9" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -1300,7 +1228,7 @@
       <c r="G9" s="56"/>
       <c r="H9" s="49"/>
       <c r="I9" s="49"/>
-      <c r="J9" s="17"/>
+      <c r="J9" s="49"/>
       <c r="K9" s="49"/>
       <c r="L9" s="18"/>
       <c r="M9" s="18"/>
@@ -1323,7 +1251,7 @@
     </row>
     <row r="10" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -1333,7 +1261,7 @@
       <c r="G10" s="56"/>
       <c r="H10" s="49"/>
       <c r="I10" s="49"/>
-      <c r="J10" s="17"/>
+      <c r="J10" s="49"/>
       <c r="K10" s="49"/>
       <c r="L10" s="18"/>
       <c r="M10" s="18"/>
@@ -1356,7 +1284,7 @@
     </row>
     <row r="11" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
@@ -1366,7 +1294,7 @@
       <c r="G11" s="56"/>
       <c r="H11" s="49"/>
       <c r="I11" s="49"/>
-      <c r="J11" s="17"/>
+      <c r="J11" s="49"/>
       <c r="K11" s="49"/>
       <c r="L11" s="18"/>
       <c r="M11" s="18"/>
@@ -1388,18 +1316,18 @@
       <c r="AC11" s="1"/>
     </row>
     <row r="12" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
-        <v>7</v>
+      <c r="A12" s="5">
+        <v>9</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="56"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="57"/>
       <c r="H12" s="49"/>
       <c r="I12" s="49"/>
-      <c r="J12" s="17"/>
+      <c r="J12" s="49"/>
       <c r="K12" s="49"/>
       <c r="L12" s="18"/>
       <c r="M12" s="18"/>
@@ -1421,18 +1349,18 @@
       <c r="AC12" s="1"/>
     </row>
     <row r="13" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
-        <v>8</v>
+      <c r="A13" s="3">
+        <v>10</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="56"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="58"/>
       <c r="H13" s="49"/>
       <c r="I13" s="49"/>
-      <c r="J13" s="17"/>
+      <c r="J13" s="49"/>
       <c r="K13" s="49"/>
       <c r="L13" s="18"/>
       <c r="M13" s="18"/>
@@ -1454,18 +1382,18 @@
       <c r="AC13" s="1"/>
     </row>
     <row r="14" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>9</v>
+      <c r="A14" s="3">
+        <v>11</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="57"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="58"/>
       <c r="H14" s="49"/>
       <c r="I14" s="49"/>
-      <c r="J14" s="17"/>
+      <c r="J14" s="49"/>
       <c r="K14" s="49"/>
       <c r="L14" s="18"/>
       <c r="M14" s="18"/>
@@ -1488,7 +1416,7 @@
     </row>
     <row r="15" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1498,7 +1426,7 @@
       <c r="G15" s="58"/>
       <c r="H15" s="49"/>
       <c r="I15" s="49"/>
-      <c r="J15" s="17"/>
+      <c r="J15" s="49"/>
       <c r="K15" s="49"/>
       <c r="L15" s="18"/>
       <c r="M15" s="18"/>
@@ -1521,7 +1449,7 @@
     </row>
     <row r="16" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1531,7 +1459,7 @@
       <c r="G16" s="58"/>
       <c r="H16" s="49"/>
       <c r="I16" s="49"/>
-      <c r="J16" s="17"/>
+      <c r="J16" s="49"/>
       <c r="K16" s="49"/>
       <c r="L16" s="18"/>
       <c r="M16" s="18"/>
@@ -1554,7 +1482,7 @@
     </row>
     <row r="17" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1564,7 +1492,7 @@
       <c r="G17" s="58"/>
       <c r="H17" s="49"/>
       <c r="I17" s="49"/>
-      <c r="J17" s="17"/>
+      <c r="J17" s="49"/>
       <c r="K17" s="49"/>
       <c r="L17" s="18"/>
       <c r="M17" s="18"/>
@@ -1587,7 +1515,7 @@
     </row>
     <row r="18" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1597,7 +1525,7 @@
       <c r="G18" s="58"/>
       <c r="H18" s="49"/>
       <c r="I18" s="49"/>
-      <c r="J18" s="17"/>
+      <c r="J18" s="49"/>
       <c r="K18" s="49"/>
       <c r="L18" s="18"/>
       <c r="M18" s="18"/>
@@ -1620,7 +1548,7 @@
     </row>
     <row r="19" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1630,7 +1558,7 @@
       <c r="G19" s="58"/>
       <c r="H19" s="49"/>
       <c r="I19" s="49"/>
-      <c r="J19" s="17"/>
+      <c r="J19" s="49"/>
       <c r="K19" s="49"/>
       <c r="L19" s="18"/>
       <c r="M19" s="18"/>
@@ -1653,7 +1581,7 @@
     </row>
     <row r="20" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1663,7 +1591,7 @@
       <c r="G20" s="58"/>
       <c r="H20" s="49"/>
       <c r="I20" s="49"/>
-      <c r="J20" s="17"/>
+      <c r="J20" s="49"/>
       <c r="K20" s="49"/>
       <c r="L20" s="18"/>
       <c r="M20" s="18"/>
@@ -1686,7 +1614,7 @@
     </row>
     <row r="21" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1696,7 +1624,7 @@
       <c r="G21" s="58"/>
       <c r="H21" s="49"/>
       <c r="I21" s="49"/>
-      <c r="J21" s="17"/>
+      <c r="J21" s="49"/>
       <c r="K21" s="49"/>
       <c r="L21" s="18"/>
       <c r="M21" s="18"/>
@@ -1719,7 +1647,7 @@
     </row>
     <row r="22" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1729,7 +1657,7 @@
       <c r="G22" s="58"/>
       <c r="H22" s="49"/>
       <c r="I22" s="49"/>
-      <c r="J22" s="17"/>
+      <c r="J22" s="49"/>
       <c r="K22" s="49"/>
       <c r="L22" s="18"/>
       <c r="M22" s="18"/>
@@ -1752,7 +1680,7 @@
     </row>
     <row r="23" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1762,7 +1690,7 @@
       <c r="G23" s="58"/>
       <c r="H23" s="49"/>
       <c r="I23" s="49"/>
-      <c r="J23" s="17"/>
+      <c r="J23" s="49"/>
       <c r="K23" s="49"/>
       <c r="L23" s="18"/>
       <c r="M23" s="18"/>
@@ -1785,7 +1713,7 @@
     </row>
     <row r="24" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1795,7 +1723,7 @@
       <c r="G24" s="58"/>
       <c r="H24" s="49"/>
       <c r="I24" s="49"/>
-      <c r="J24" s="17"/>
+      <c r="J24" s="49"/>
       <c r="K24" s="49"/>
       <c r="L24" s="18"/>
       <c r="M24" s="18"/>
@@ -1818,7 +1746,7 @@
     </row>
     <row r="25" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1828,7 +1756,7 @@
       <c r="G25" s="58"/>
       <c r="H25" s="49"/>
       <c r="I25" s="49"/>
-      <c r="J25" s="17"/>
+      <c r="J25" s="49"/>
       <c r="K25" s="49"/>
       <c r="L25" s="18"/>
       <c r="M25" s="18"/>
@@ -1851,7 +1779,7 @@
     </row>
     <row r="26" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1861,7 +1789,7 @@
       <c r="G26" s="58"/>
       <c r="H26" s="49"/>
       <c r="I26" s="49"/>
-      <c r="J26" s="17"/>
+      <c r="J26" s="49"/>
       <c r="K26" s="49"/>
       <c r="L26" s="18"/>
       <c r="M26" s="18"/>
@@ -1884,7 +1812,7 @@
     </row>
     <row r="27" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1894,7 +1822,7 @@
       <c r="G27" s="58"/>
       <c r="H27" s="49"/>
       <c r="I27" s="49"/>
-      <c r="J27" s="17"/>
+      <c r="J27" s="49"/>
       <c r="K27" s="49"/>
       <c r="L27" s="18"/>
       <c r="M27" s="18"/>
@@ -1917,7 +1845,7 @@
     </row>
     <row r="28" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1927,7 +1855,7 @@
       <c r="G28" s="58"/>
       <c r="H28" s="49"/>
       <c r="I28" s="49"/>
-      <c r="J28" s="17"/>
+      <c r="J28" s="49"/>
       <c r="K28" s="49"/>
       <c r="L28" s="18"/>
       <c r="M28" s="18"/>
@@ -1950,7 +1878,7 @@
     </row>
     <row r="29" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1960,7 +1888,7 @@
       <c r="G29" s="58"/>
       <c r="H29" s="49"/>
       <c r="I29" s="49"/>
-      <c r="J29" s="17"/>
+      <c r="J29" s="49"/>
       <c r="K29" s="49"/>
       <c r="L29" s="18"/>
       <c r="M29" s="18"/>
@@ -1983,7 +1911,7 @@
     </row>
     <row r="30" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1993,7 +1921,7 @@
       <c r="G30" s="58"/>
       <c r="H30" s="49"/>
       <c r="I30" s="49"/>
-      <c r="J30" s="17"/>
+      <c r="J30" s="49"/>
       <c r="K30" s="49"/>
       <c r="L30" s="18"/>
       <c r="M30" s="18"/>
@@ -2016,7 +1944,7 @@
     </row>
     <row r="31" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2026,7 +1954,7 @@
       <c r="G31" s="58"/>
       <c r="H31" s="49"/>
       <c r="I31" s="49"/>
-      <c r="J31" s="17"/>
+      <c r="J31" s="49"/>
       <c r="K31" s="49"/>
       <c r="L31" s="18"/>
       <c r="M31" s="18"/>
@@ -2049,7 +1977,7 @@
     </row>
     <row r="32" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2059,7 +1987,7 @@
       <c r="G32" s="58"/>
       <c r="H32" s="49"/>
       <c r="I32" s="49"/>
-      <c r="J32" s="17"/>
+      <c r="J32" s="49"/>
       <c r="K32" s="49"/>
       <c r="L32" s="18"/>
       <c r="M32" s="18"/>
@@ -2082,7 +2010,7 @@
     </row>
     <row r="33" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2092,7 +2020,7 @@
       <c r="G33" s="58"/>
       <c r="H33" s="49"/>
       <c r="I33" s="49"/>
-      <c r="J33" s="17"/>
+      <c r="J33" s="49"/>
       <c r="K33" s="49"/>
       <c r="L33" s="18"/>
       <c r="M33" s="18"/>
@@ -2115,7 +2043,7 @@
     </row>
     <row r="34" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -2125,7 +2053,7 @@
       <c r="G34" s="58"/>
       <c r="H34" s="49"/>
       <c r="I34" s="49"/>
-      <c r="J34" s="17"/>
+      <c r="J34" s="49"/>
       <c r="K34" s="49"/>
       <c r="L34" s="18"/>
       <c r="M34" s="18"/>
@@ -2148,7 +2076,7 @@
     </row>
     <row r="35" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -2158,7 +2086,7 @@
       <c r="G35" s="58"/>
       <c r="H35" s="49"/>
       <c r="I35" s="49"/>
-      <c r="J35" s="17"/>
+      <c r="J35" s="49"/>
       <c r="K35" s="49"/>
       <c r="L35" s="18"/>
       <c r="M35" s="18"/>
@@ -2181,7 +2109,7 @@
     </row>
     <row r="36" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -2191,7 +2119,7 @@
       <c r="G36" s="58"/>
       <c r="H36" s="49"/>
       <c r="I36" s="49"/>
-      <c r="J36" s="17"/>
+      <c r="J36" s="49"/>
       <c r="K36" s="49"/>
       <c r="L36" s="18"/>
       <c r="M36" s="18"/>
@@ -2214,7 +2142,7 @@
     </row>
     <row r="37" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -2224,7 +2152,7 @@
       <c r="G37" s="58"/>
       <c r="H37" s="49"/>
       <c r="I37" s="49"/>
-      <c r="J37" s="17"/>
+      <c r="J37" s="49"/>
       <c r="K37" s="49"/>
       <c r="L37" s="18"/>
       <c r="M37" s="18"/>
@@ -2247,7 +2175,7 @@
     </row>
     <row r="38" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -2257,7 +2185,7 @@
       <c r="G38" s="58"/>
       <c r="H38" s="49"/>
       <c r="I38" s="49"/>
-      <c r="J38" s="17"/>
+      <c r="J38" s="49"/>
       <c r="K38" s="49"/>
       <c r="L38" s="18"/>
       <c r="M38" s="18"/>
@@ -2280,7 +2208,7 @@
     </row>
     <row r="39" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2290,7 +2218,7 @@
       <c r="G39" s="58"/>
       <c r="H39" s="49"/>
       <c r="I39" s="49"/>
-      <c r="J39" s="17"/>
+      <c r="J39" s="49"/>
       <c r="K39" s="49"/>
       <c r="L39" s="18"/>
       <c r="M39" s="18"/>
@@ -2313,7 +2241,7 @@
     </row>
     <row r="40" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -2323,7 +2251,7 @@
       <c r="G40" s="58"/>
       <c r="H40" s="49"/>
       <c r="I40" s="49"/>
-      <c r="J40" s="17"/>
+      <c r="J40" s="49"/>
       <c r="K40" s="49"/>
       <c r="L40" s="18"/>
       <c r="M40" s="18"/>
@@ -2346,7 +2274,7 @@
     </row>
     <row r="41" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -2356,7 +2284,7 @@
       <c r="G41" s="58"/>
       <c r="H41" s="49"/>
       <c r="I41" s="49"/>
-      <c r="J41" s="17"/>
+      <c r="J41" s="49"/>
       <c r="K41" s="49"/>
       <c r="L41" s="18"/>
       <c r="M41" s="18"/>
@@ -2379,7 +2307,7 @@
     </row>
     <row r="42" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2389,7 +2317,7 @@
       <c r="G42" s="58"/>
       <c r="H42" s="49"/>
       <c r="I42" s="49"/>
-      <c r="J42" s="17"/>
+      <c r="J42" s="49"/>
       <c r="K42" s="49"/>
       <c r="L42" s="18"/>
       <c r="M42" s="18"/>
@@ -2412,7 +2340,7 @@
     </row>
     <row r="43" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -2422,7 +2350,7 @@
       <c r="G43" s="58"/>
       <c r="H43" s="49"/>
       <c r="I43" s="49"/>
-      <c r="J43" s="17"/>
+      <c r="J43" s="49"/>
       <c r="K43" s="49"/>
       <c r="L43" s="18"/>
       <c r="M43" s="18"/>
@@ -2445,7 +2373,7 @@
     </row>
     <row r="44" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -2455,7 +2383,7 @@
       <c r="G44" s="58"/>
       <c r="H44" s="49"/>
       <c r="I44" s="49"/>
-      <c r="J44" s="17"/>
+      <c r="J44" s="49"/>
       <c r="K44" s="49"/>
       <c r="L44" s="18"/>
       <c r="M44" s="18"/>
@@ -2478,7 +2406,7 @@
     </row>
     <row r="45" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -2488,7 +2416,7 @@
       <c r="G45" s="58"/>
       <c r="H45" s="49"/>
       <c r="I45" s="49"/>
-      <c r="J45" s="17"/>
+      <c r="J45" s="49"/>
       <c r="K45" s="49"/>
       <c r="L45" s="18"/>
       <c r="M45" s="18"/>
@@ -2511,7 +2439,7 @@
     </row>
     <row r="46" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -2521,7 +2449,7 @@
       <c r="G46" s="58"/>
       <c r="H46" s="49"/>
       <c r="I46" s="49"/>
-      <c r="J46" s="17"/>
+      <c r="J46" s="49"/>
       <c r="K46" s="49"/>
       <c r="L46" s="18"/>
       <c r="M46" s="18"/>
@@ -2544,7 +2472,7 @@
     </row>
     <row r="47" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -2554,7 +2482,7 @@
       <c r="G47" s="58"/>
       <c r="H47" s="49"/>
       <c r="I47" s="49"/>
-      <c r="J47" s="17"/>
+      <c r="J47" s="49"/>
       <c r="K47" s="49"/>
       <c r="L47" s="18"/>
       <c r="M47" s="18"/>
@@ -2577,7 +2505,7 @@
     </row>
     <row r="48" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -2587,7 +2515,7 @@
       <c r="G48" s="58"/>
       <c r="H48" s="49"/>
       <c r="I48" s="49"/>
-      <c r="J48" s="17"/>
+      <c r="J48" s="49"/>
       <c r="K48" s="49"/>
       <c r="L48" s="18"/>
       <c r="M48" s="18"/>
@@ -2610,7 +2538,7 @@
     </row>
     <row r="49" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -2620,7 +2548,7 @@
       <c r="G49" s="58"/>
       <c r="H49" s="49"/>
       <c r="I49" s="49"/>
-      <c r="J49" s="17"/>
+      <c r="J49" s="49"/>
       <c r="K49" s="49"/>
       <c r="L49" s="18"/>
       <c r="M49" s="18"/>
@@ -2643,7 +2571,7 @@
     </row>
     <row r="50" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -2653,7 +2581,7 @@
       <c r="G50" s="58"/>
       <c r="H50" s="49"/>
       <c r="I50" s="49"/>
-      <c r="J50" s="17"/>
+      <c r="J50" s="49"/>
       <c r="K50" s="49"/>
       <c r="L50" s="18"/>
       <c r="M50" s="18"/>
@@ -2676,7 +2604,7 @@
     </row>
     <row r="51" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -2686,7 +2614,7 @@
       <c r="G51" s="58"/>
       <c r="H51" s="49"/>
       <c r="I51" s="49"/>
-      <c r="J51" s="17"/>
+      <c r="J51" s="49"/>
       <c r="K51" s="49"/>
       <c r="L51" s="18"/>
       <c r="M51" s="18"/>
@@ -2709,7 +2637,7 @@
     </row>
     <row r="52" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -2719,7 +2647,7 @@
       <c r="G52" s="58"/>
       <c r="H52" s="49"/>
       <c r="I52" s="49"/>
-      <c r="J52" s="17"/>
+      <c r="J52" s="49"/>
       <c r="K52" s="49"/>
       <c r="L52" s="18"/>
       <c r="M52" s="18"/>
@@ -2742,7 +2670,7 @@
     </row>
     <row r="53" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -2752,7 +2680,7 @@
       <c r="G53" s="58"/>
       <c r="H53" s="49"/>
       <c r="I53" s="49"/>
-      <c r="J53" s="17"/>
+      <c r="J53" s="49"/>
       <c r="K53" s="49"/>
       <c r="L53" s="18"/>
       <c r="M53" s="18"/>
@@ -2775,7 +2703,7 @@
     </row>
     <row r="54" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -2785,7 +2713,7 @@
       <c r="G54" s="58"/>
       <c r="H54" s="49"/>
       <c r="I54" s="49"/>
-      <c r="J54" s="17"/>
+      <c r="J54" s="49"/>
       <c r="K54" s="49"/>
       <c r="L54" s="18"/>
       <c r="M54" s="18"/>
@@ -2808,7 +2736,7 @@
     </row>
     <row r="55" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -2818,7 +2746,7 @@
       <c r="G55" s="58"/>
       <c r="H55" s="49"/>
       <c r="I55" s="49"/>
-      <c r="J55" s="17"/>
+      <c r="J55" s="49"/>
       <c r="K55" s="49"/>
       <c r="L55" s="18"/>
       <c r="M55" s="18"/>
@@ -2841,7 +2769,7 @@
     </row>
     <row r="56" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -2851,7 +2779,7 @@
       <c r="G56" s="58"/>
       <c r="H56" s="49"/>
       <c r="I56" s="49"/>
-      <c r="J56" s="17"/>
+      <c r="J56" s="49"/>
       <c r="K56" s="49"/>
       <c r="L56" s="18"/>
       <c r="M56" s="18"/>
@@ -2874,7 +2802,7 @@
     </row>
     <row r="57" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -2884,7 +2812,7 @@
       <c r="G57" s="58"/>
       <c r="H57" s="49"/>
       <c r="I57" s="49"/>
-      <c r="J57" s="17"/>
+      <c r="J57" s="49"/>
       <c r="K57" s="49"/>
       <c r="L57" s="18"/>
       <c r="M57" s="18"/>
@@ -2907,7 +2835,7 @@
     </row>
     <row r="58" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -2917,7 +2845,7 @@
       <c r="G58" s="58"/>
       <c r="H58" s="49"/>
       <c r="I58" s="49"/>
-      <c r="J58" s="17"/>
+      <c r="J58" s="49"/>
       <c r="K58" s="49"/>
       <c r="L58" s="18"/>
       <c r="M58" s="18"/>
@@ -2940,7 +2868,7 @@
     </row>
     <row r="59" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -2950,7 +2878,7 @@
       <c r="G59" s="58"/>
       <c r="H59" s="49"/>
       <c r="I59" s="49"/>
-      <c r="J59" s="17"/>
+      <c r="J59" s="49"/>
       <c r="K59" s="49"/>
       <c r="L59" s="18"/>
       <c r="M59" s="18"/>
@@ -2973,7 +2901,7 @@
     </row>
     <row r="60" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -2983,7 +2911,7 @@
       <c r="G60" s="58"/>
       <c r="H60" s="49"/>
       <c r="I60" s="49"/>
-      <c r="J60" s="17"/>
+      <c r="J60" s="49"/>
       <c r="K60" s="49"/>
       <c r="L60" s="18"/>
       <c r="M60" s="18"/>
@@ -3006,7 +2934,7 @@
     </row>
     <row r="61" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -3016,7 +2944,7 @@
       <c r="G61" s="58"/>
       <c r="H61" s="49"/>
       <c r="I61" s="49"/>
-      <c r="J61" s="17"/>
+      <c r="J61" s="49"/>
       <c r="K61" s="49"/>
       <c r="L61" s="18"/>
       <c r="M61" s="18"/>
@@ -3039,7 +2967,7 @@
     </row>
     <row r="62" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -3049,7 +2977,7 @@
       <c r="G62" s="58"/>
       <c r="H62" s="49"/>
       <c r="I62" s="49"/>
-      <c r="J62" s="17"/>
+      <c r="J62" s="49"/>
       <c r="K62" s="49"/>
       <c r="L62" s="18"/>
       <c r="M62" s="18"/>
@@ -3072,7 +3000,7 @@
     </row>
     <row r="63" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -3082,7 +3010,7 @@
       <c r="G63" s="58"/>
       <c r="H63" s="49"/>
       <c r="I63" s="49"/>
-      <c r="J63" s="17"/>
+      <c r="J63" s="49"/>
       <c r="K63" s="49"/>
       <c r="L63" s="18"/>
       <c r="M63" s="18"/>
@@ -3105,7 +3033,7 @@
     </row>
     <row r="64" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -3115,7 +3043,7 @@
       <c r="G64" s="58"/>
       <c r="H64" s="49"/>
       <c r="I64" s="49"/>
-      <c r="J64" s="17"/>
+      <c r="J64" s="49"/>
       <c r="K64" s="49"/>
       <c r="L64" s="18"/>
       <c r="M64" s="18"/>
@@ -3138,7 +3066,7 @@
     </row>
     <row r="65" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -3148,7 +3076,7 @@
       <c r="G65" s="58"/>
       <c r="H65" s="49"/>
       <c r="I65" s="49"/>
-      <c r="J65" s="17"/>
+      <c r="J65" s="49"/>
       <c r="K65" s="49"/>
       <c r="L65" s="18"/>
       <c r="M65" s="18"/>
@@ -3171,7 +3099,7 @@
     </row>
     <row r="66" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -3181,7 +3109,7 @@
       <c r="G66" s="58"/>
       <c r="H66" s="49"/>
       <c r="I66" s="49"/>
-      <c r="J66" s="17"/>
+      <c r="J66" s="49"/>
       <c r="K66" s="49"/>
       <c r="L66" s="18"/>
       <c r="M66" s="18"/>
@@ -3204,7 +3132,7 @@
     </row>
     <row r="67" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -3214,7 +3142,7 @@
       <c r="G67" s="58"/>
       <c r="H67" s="49"/>
       <c r="I67" s="49"/>
-      <c r="J67" s="17"/>
+      <c r="J67" s="49"/>
       <c r="K67" s="49"/>
       <c r="L67" s="18"/>
       <c r="M67" s="18"/>
@@ -3237,7 +3165,7 @@
     </row>
     <row r="68" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -3247,7 +3175,7 @@
       <c r="G68" s="58"/>
       <c r="H68" s="49"/>
       <c r="I68" s="49"/>
-      <c r="J68" s="17"/>
+      <c r="J68" s="49"/>
       <c r="K68" s="49"/>
       <c r="L68" s="18"/>
       <c r="M68" s="18"/>
@@ -3270,7 +3198,7 @@
     </row>
     <row r="69" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -3280,7 +3208,7 @@
       <c r="G69" s="58"/>
       <c r="H69" s="49"/>
       <c r="I69" s="49"/>
-      <c r="J69" s="17"/>
+      <c r="J69" s="49"/>
       <c r="K69" s="49"/>
       <c r="L69" s="18"/>
       <c r="M69" s="18"/>
@@ -3303,7 +3231,7 @@
     </row>
     <row r="70" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -3313,7 +3241,7 @@
       <c r="G70" s="58"/>
       <c r="H70" s="49"/>
       <c r="I70" s="49"/>
-      <c r="J70" s="17"/>
+      <c r="J70" s="49"/>
       <c r="K70" s="49"/>
       <c r="L70" s="18"/>
       <c r="M70" s="18"/>
@@ -3336,7 +3264,7 @@
     </row>
     <row r="71" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -3346,7 +3274,7 @@
       <c r="G71" s="58"/>
       <c r="H71" s="49"/>
       <c r="I71" s="49"/>
-      <c r="J71" s="17"/>
+      <c r="J71" s="49"/>
       <c r="K71" s="49"/>
       <c r="L71" s="18"/>
       <c r="M71" s="18"/>
@@ -3369,7 +3297,7 @@
     </row>
     <row r="72" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -3379,7 +3307,7 @@
       <c r="G72" s="58"/>
       <c r="H72" s="49"/>
       <c r="I72" s="49"/>
-      <c r="J72" s="17"/>
+      <c r="J72" s="49"/>
       <c r="K72" s="49"/>
       <c r="L72" s="18"/>
       <c r="M72" s="18"/>
@@ -3402,7 +3330,7 @@
     </row>
     <row r="73" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -3412,7 +3340,7 @@
       <c r="G73" s="58"/>
       <c r="H73" s="49"/>
       <c r="I73" s="49"/>
-      <c r="J73" s="17"/>
+      <c r="J73" s="49"/>
       <c r="K73" s="49"/>
       <c r="L73" s="18"/>
       <c r="M73" s="18"/>
@@ -3435,7 +3363,7 @@
     </row>
     <row r="74" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -3445,7 +3373,7 @@
       <c r="G74" s="58"/>
       <c r="H74" s="49"/>
       <c r="I74" s="49"/>
-      <c r="J74" s="17"/>
+      <c r="J74" s="49"/>
       <c r="K74" s="49"/>
       <c r="L74" s="18"/>
       <c r="M74" s="18"/>
@@ -3468,7 +3396,7 @@
     </row>
     <row r="75" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -3478,7 +3406,7 @@
       <c r="G75" s="58"/>
       <c r="H75" s="49"/>
       <c r="I75" s="49"/>
-      <c r="J75" s="17"/>
+      <c r="J75" s="49"/>
       <c r="K75" s="49"/>
       <c r="L75" s="18"/>
       <c r="M75" s="18"/>
@@ -3501,7 +3429,7 @@
     </row>
     <row r="76" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -3511,7 +3439,7 @@
       <c r="G76" s="58"/>
       <c r="H76" s="49"/>
       <c r="I76" s="49"/>
-      <c r="J76" s="17"/>
+      <c r="J76" s="49"/>
       <c r="K76" s="49"/>
       <c r="L76" s="18"/>
       <c r="M76" s="18"/>
@@ -3534,7 +3462,7 @@
     </row>
     <row r="77" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -3544,7 +3472,7 @@
       <c r="G77" s="58"/>
       <c r="H77" s="49"/>
       <c r="I77" s="49"/>
-      <c r="J77" s="17"/>
+      <c r="J77" s="49"/>
       <c r="K77" s="49"/>
       <c r="L77" s="18"/>
       <c r="M77" s="18"/>
@@ -3567,7 +3495,7 @@
     </row>
     <row r="78" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -3577,7 +3505,7 @@
       <c r="G78" s="58"/>
       <c r="H78" s="49"/>
       <c r="I78" s="49"/>
-      <c r="J78" s="17"/>
+      <c r="J78" s="49"/>
       <c r="K78" s="49"/>
       <c r="L78" s="18"/>
       <c r="M78" s="18"/>
@@ -3600,7 +3528,7 @@
     </row>
     <row r="79" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -3610,7 +3538,7 @@
       <c r="G79" s="58"/>
       <c r="H79" s="49"/>
       <c r="I79" s="49"/>
-      <c r="J79" s="17"/>
+      <c r="J79" s="49"/>
       <c r="K79" s="49"/>
       <c r="L79" s="18"/>
       <c r="M79" s="18"/>
@@ -3633,7 +3561,7 @@
     </row>
     <row r="80" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -3643,7 +3571,7 @@
       <c r="G80" s="58"/>
       <c r="H80" s="49"/>
       <c r="I80" s="49"/>
-      <c r="J80" s="17"/>
+      <c r="J80" s="49"/>
       <c r="K80" s="49"/>
       <c r="L80" s="18"/>
       <c r="M80" s="18"/>
@@ -3666,7 +3594,7 @@
     </row>
     <row r="81" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -3676,7 +3604,7 @@
       <c r="G81" s="58"/>
       <c r="H81" s="49"/>
       <c r="I81" s="49"/>
-      <c r="J81" s="17"/>
+      <c r="J81" s="49"/>
       <c r="K81" s="49"/>
       <c r="L81" s="18"/>
       <c r="M81" s="18"/>
@@ -3699,7 +3627,7 @@
     </row>
     <row r="82" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -3709,7 +3637,7 @@
       <c r="G82" s="58"/>
       <c r="H82" s="49"/>
       <c r="I82" s="49"/>
-      <c r="J82" s="17"/>
+      <c r="J82" s="49"/>
       <c r="K82" s="49"/>
       <c r="L82" s="18"/>
       <c r="M82" s="18"/>
@@ -3732,7 +3660,7 @@
     </row>
     <row r="83" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -3742,7 +3670,7 @@
       <c r="G83" s="58"/>
       <c r="H83" s="49"/>
       <c r="I83" s="49"/>
-      <c r="J83" s="17"/>
+      <c r="J83" s="49"/>
       <c r="K83" s="49"/>
       <c r="L83" s="18"/>
       <c r="M83" s="18"/>
@@ -3765,7 +3693,7 @@
     </row>
     <row r="84" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -3775,7 +3703,7 @@
       <c r="G84" s="58"/>
       <c r="H84" s="49"/>
       <c r="I84" s="49"/>
-      <c r="J84" s="17"/>
+      <c r="J84" s="49"/>
       <c r="K84" s="49"/>
       <c r="L84" s="18"/>
       <c r="M84" s="18"/>
@@ -3798,7 +3726,7 @@
     </row>
     <row r="85" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -3808,7 +3736,7 @@
       <c r="G85" s="58"/>
       <c r="H85" s="49"/>
       <c r="I85" s="49"/>
-      <c r="J85" s="17"/>
+      <c r="J85" s="49"/>
       <c r="K85" s="49"/>
       <c r="L85" s="18"/>
       <c r="M85" s="18"/>
@@ -3831,7 +3759,7 @@
     </row>
     <row r="86" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -3841,7 +3769,7 @@
       <c r="G86" s="58"/>
       <c r="H86" s="49"/>
       <c r="I86" s="49"/>
-      <c r="J86" s="17"/>
+      <c r="J86" s="49"/>
       <c r="K86" s="49"/>
       <c r="L86" s="18"/>
       <c r="M86" s="18"/>
@@ -3864,7 +3792,7 @@
     </row>
     <row r="87" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -3874,7 +3802,7 @@
       <c r="G87" s="58"/>
       <c r="H87" s="49"/>
       <c r="I87" s="49"/>
-      <c r="J87" s="17"/>
+      <c r="J87" s="49"/>
       <c r="K87" s="49"/>
       <c r="L87" s="18"/>
       <c r="M87" s="18"/>
@@ -3897,7 +3825,7 @@
     </row>
     <row r="88" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -3907,7 +3835,7 @@
       <c r="G88" s="58"/>
       <c r="H88" s="49"/>
       <c r="I88" s="49"/>
-      <c r="J88" s="17"/>
+      <c r="J88" s="49"/>
       <c r="K88" s="49"/>
       <c r="L88" s="18"/>
       <c r="M88" s="18"/>
@@ -3930,7 +3858,7 @@
     </row>
     <row r="89" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -3940,7 +3868,7 @@
       <c r="G89" s="58"/>
       <c r="H89" s="49"/>
       <c r="I89" s="49"/>
-      <c r="J89" s="17"/>
+      <c r="J89" s="49"/>
       <c r="K89" s="49"/>
       <c r="L89" s="18"/>
       <c r="M89" s="18"/>
@@ -3963,7 +3891,7 @@
     </row>
     <row r="90" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -3973,7 +3901,7 @@
       <c r="G90" s="58"/>
       <c r="H90" s="49"/>
       <c r="I90" s="49"/>
-      <c r="J90" s="17"/>
+      <c r="J90" s="49"/>
       <c r="K90" s="49"/>
       <c r="L90" s="18"/>
       <c r="M90" s="18"/>
@@ -3996,7 +3924,7 @@
     </row>
     <row r="91" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
@@ -4006,7 +3934,7 @@
       <c r="G91" s="58"/>
       <c r="H91" s="49"/>
       <c r="I91" s="49"/>
-      <c r="J91" s="17"/>
+      <c r="J91" s="49"/>
       <c r="K91" s="49"/>
       <c r="L91" s="18"/>
       <c r="M91" s="18"/>
@@ -4029,7 +3957,7 @@
     </row>
     <row r="92" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
@@ -4039,7 +3967,7 @@
       <c r="G92" s="58"/>
       <c r="H92" s="49"/>
       <c r="I92" s="49"/>
-      <c r="J92" s="17"/>
+      <c r="J92" s="49"/>
       <c r="K92" s="49"/>
       <c r="L92" s="18"/>
       <c r="M92" s="18"/>
@@ -4062,7 +3990,7 @@
     </row>
     <row r="93" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -4072,7 +4000,7 @@
       <c r="G93" s="58"/>
       <c r="H93" s="49"/>
       <c r="I93" s="49"/>
-      <c r="J93" s="17"/>
+      <c r="J93" s="49"/>
       <c r="K93" s="49"/>
       <c r="L93" s="18"/>
       <c r="M93" s="18"/>
@@ -4095,7 +4023,7 @@
     </row>
     <row r="94" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
@@ -4105,7 +4033,7 @@
       <c r="G94" s="58"/>
       <c r="H94" s="49"/>
       <c r="I94" s="49"/>
-      <c r="J94" s="17"/>
+      <c r="J94" s="49"/>
       <c r="K94" s="49"/>
       <c r="L94" s="18"/>
       <c r="M94" s="18"/>
@@ -4128,7 +4056,7 @@
     </row>
     <row r="95" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
@@ -4138,7 +4066,7 @@
       <c r="G95" s="58"/>
       <c r="H95" s="49"/>
       <c r="I95" s="49"/>
-      <c r="J95" s="17"/>
+      <c r="J95" s="49"/>
       <c r="K95" s="49"/>
       <c r="L95" s="18"/>
       <c r="M95" s="18"/>
@@ -4161,7 +4089,7 @@
     </row>
     <row r="96" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
@@ -4171,7 +4099,7 @@
       <c r="G96" s="58"/>
       <c r="H96" s="49"/>
       <c r="I96" s="49"/>
-      <c r="J96" s="17"/>
+      <c r="J96" s="49"/>
       <c r="K96" s="49"/>
       <c r="L96" s="18"/>
       <c r="M96" s="18"/>
@@ -4194,7 +4122,7 @@
     </row>
     <row r="97" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
@@ -4204,7 +4132,7 @@
       <c r="G97" s="58"/>
       <c r="H97" s="49"/>
       <c r="I97" s="49"/>
-      <c r="J97" s="17"/>
+      <c r="J97" s="49"/>
       <c r="K97" s="49"/>
       <c r="L97" s="18"/>
       <c r="M97" s="18"/>
@@ -4227,7 +4155,7 @@
     </row>
     <row r="98" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
@@ -4237,7 +4165,7 @@
       <c r="G98" s="58"/>
       <c r="H98" s="49"/>
       <c r="I98" s="49"/>
-      <c r="J98" s="17"/>
+      <c r="J98" s="49"/>
       <c r="K98" s="49"/>
       <c r="L98" s="18"/>
       <c r="M98" s="18"/>
@@ -4260,7 +4188,7 @@
     </row>
     <row r="99" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
@@ -4270,7 +4198,7 @@
       <c r="G99" s="58"/>
       <c r="H99" s="49"/>
       <c r="I99" s="49"/>
-      <c r="J99" s="17"/>
+      <c r="J99" s="49"/>
       <c r="K99" s="49"/>
       <c r="L99" s="18"/>
       <c r="M99" s="18"/>
@@ -4293,7 +4221,7 @@
     </row>
     <row r="100" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
@@ -4303,7 +4231,7 @@
       <c r="G100" s="58"/>
       <c r="H100" s="49"/>
       <c r="I100" s="49"/>
-      <c r="J100" s="17"/>
+      <c r="J100" s="49"/>
       <c r="K100" s="49"/>
       <c r="L100" s="18"/>
       <c r="M100" s="18"/>
@@ -4326,7 +4254,7 @@
     </row>
     <row r="101" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
@@ -4336,7 +4264,7 @@
       <c r="G101" s="58"/>
       <c r="H101" s="49"/>
       <c r="I101" s="49"/>
-      <c r="J101" s="17"/>
+      <c r="J101" s="49"/>
       <c r="K101" s="49"/>
       <c r="L101" s="18"/>
       <c r="M101" s="18"/>
@@ -4359,7 +4287,7 @@
     </row>
     <row r="102" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
@@ -4369,7 +4297,7 @@
       <c r="G102" s="58"/>
       <c r="H102" s="49"/>
       <c r="I102" s="49"/>
-      <c r="J102" s="17"/>
+      <c r="J102" s="49"/>
       <c r="K102" s="49"/>
       <c r="L102" s="18"/>
       <c r="M102" s="18"/>
@@ -4392,7 +4320,7 @@
     </row>
     <row r="103" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
@@ -4402,7 +4330,7 @@
       <c r="G103" s="58"/>
       <c r="H103" s="49"/>
       <c r="I103" s="49"/>
-      <c r="J103" s="17"/>
+      <c r="J103" s="49"/>
       <c r="K103" s="49"/>
       <c r="L103" s="18"/>
       <c r="M103" s="18"/>
@@ -4425,7 +4353,7 @@
     </row>
     <row r="104" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
@@ -4435,7 +4363,7 @@
       <c r="G104" s="58"/>
       <c r="H104" s="49"/>
       <c r="I104" s="49"/>
-      <c r="J104" s="17"/>
+      <c r="J104" s="49"/>
       <c r="K104" s="49"/>
       <c r="L104" s="18"/>
       <c r="M104" s="18"/>
@@ -4458,7 +4386,7 @@
     </row>
     <row r="105" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
@@ -4468,7 +4396,7 @@
       <c r="G105" s="58"/>
       <c r="H105" s="49"/>
       <c r="I105" s="49"/>
-      <c r="J105" s="17"/>
+      <c r="J105" s="49"/>
       <c r="K105" s="49"/>
       <c r="L105" s="18"/>
       <c r="M105" s="18"/>
@@ -4491,7 +4419,7 @@
     </row>
     <row r="106" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
@@ -4501,7 +4429,7 @@
       <c r="G106" s="58"/>
       <c r="H106" s="49"/>
       <c r="I106" s="49"/>
-      <c r="J106" s="17"/>
+      <c r="J106" s="49"/>
       <c r="K106" s="49"/>
       <c r="L106" s="18"/>
       <c r="M106" s="18"/>
@@ -4524,7 +4452,7 @@
     </row>
     <row r="107" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
@@ -4534,7 +4462,7 @@
       <c r="G107" s="58"/>
       <c r="H107" s="49"/>
       <c r="I107" s="49"/>
-      <c r="J107" s="17"/>
+      <c r="J107" s="49"/>
       <c r="K107" s="49"/>
       <c r="L107" s="18"/>
       <c r="M107" s="18"/>
@@ -4557,7 +4485,7 @@
     </row>
     <row r="108" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
@@ -4567,7 +4495,7 @@
       <c r="G108" s="58"/>
       <c r="H108" s="49"/>
       <c r="I108" s="49"/>
-      <c r="J108" s="17"/>
+      <c r="J108" s="49"/>
       <c r="K108" s="49"/>
       <c r="L108" s="18"/>
       <c r="M108" s="18"/>
@@ -4590,7 +4518,7 @@
     </row>
     <row r="109" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
@@ -4600,7 +4528,7 @@
       <c r="G109" s="58"/>
       <c r="H109" s="49"/>
       <c r="I109" s="49"/>
-      <c r="J109" s="17"/>
+      <c r="J109" s="49"/>
       <c r="K109" s="49"/>
       <c r="L109" s="18"/>
       <c r="M109" s="18"/>
@@ -4623,7 +4551,7 @@
     </row>
     <row r="110" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
@@ -4633,7 +4561,7 @@
       <c r="G110" s="58"/>
       <c r="H110" s="49"/>
       <c r="I110" s="49"/>
-      <c r="J110" s="17"/>
+      <c r="J110" s="49"/>
       <c r="K110" s="49"/>
       <c r="L110" s="18"/>
       <c r="M110" s="18"/>
@@ -4656,7 +4584,7 @@
     </row>
     <row r="111" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
@@ -4666,7 +4594,7 @@
       <c r="G111" s="58"/>
       <c r="H111" s="49"/>
       <c r="I111" s="49"/>
-      <c r="J111" s="17"/>
+      <c r="J111" s="49"/>
       <c r="K111" s="49"/>
       <c r="L111" s="18"/>
       <c r="M111" s="18"/>
@@ -4689,7 +4617,7 @@
     </row>
     <row r="112" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
@@ -4699,7 +4627,7 @@
       <c r="G112" s="58"/>
       <c r="H112" s="49"/>
       <c r="I112" s="49"/>
-      <c r="J112" s="17"/>
+      <c r="J112" s="49"/>
       <c r="K112" s="49"/>
       <c r="L112" s="18"/>
       <c r="M112" s="18"/>
@@ -4722,7 +4650,7 @@
     </row>
     <row r="113" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
@@ -4732,7 +4660,7 @@
       <c r="G113" s="58"/>
       <c r="H113" s="49"/>
       <c r="I113" s="49"/>
-      <c r="J113" s="17"/>
+      <c r="J113" s="49"/>
       <c r="K113" s="49"/>
       <c r="L113" s="18"/>
       <c r="M113" s="18"/>
@@ -4755,7 +4683,7 @@
     </row>
     <row r="114" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
@@ -4765,7 +4693,7 @@
       <c r="G114" s="58"/>
       <c r="H114" s="49"/>
       <c r="I114" s="49"/>
-      <c r="J114" s="17"/>
+      <c r="J114" s="49"/>
       <c r="K114" s="49"/>
       <c r="L114" s="18"/>
       <c r="M114" s="18"/>
@@ -4788,7 +4716,7 @@
     </row>
     <row r="115" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
@@ -4798,7 +4726,7 @@
       <c r="G115" s="58"/>
       <c r="H115" s="49"/>
       <c r="I115" s="49"/>
-      <c r="J115" s="17"/>
+      <c r="J115" s="49"/>
       <c r="K115" s="49"/>
       <c r="L115" s="18"/>
       <c r="M115" s="18"/>
@@ -4821,7 +4749,7 @@
     </row>
     <row r="116" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
@@ -4831,7 +4759,7 @@
       <c r="G116" s="58"/>
       <c r="H116" s="49"/>
       <c r="I116" s="49"/>
-      <c r="J116" s="17"/>
+      <c r="J116" s="49"/>
       <c r="K116" s="49"/>
       <c r="L116" s="18"/>
       <c r="M116" s="18"/>
@@ -4854,7 +4782,7 @@
     </row>
     <row r="117" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
@@ -4864,7 +4792,7 @@
       <c r="G117" s="58"/>
       <c r="H117" s="49"/>
       <c r="I117" s="49"/>
-      <c r="J117" s="17"/>
+      <c r="J117" s="49"/>
       <c r="K117" s="49"/>
       <c r="L117" s="18"/>
       <c r="M117" s="18"/>
@@ -4887,7 +4815,7 @@
     </row>
     <row r="118" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
@@ -4897,7 +4825,7 @@
       <c r="G118" s="58"/>
       <c r="H118" s="49"/>
       <c r="I118" s="49"/>
-      <c r="J118" s="17"/>
+      <c r="J118" s="49"/>
       <c r="K118" s="49"/>
       <c r="L118" s="18"/>
       <c r="M118" s="18"/>
@@ -4920,7 +4848,7 @@
     </row>
     <row r="119" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
@@ -4930,7 +4858,7 @@
       <c r="G119" s="58"/>
       <c r="H119" s="49"/>
       <c r="I119" s="49"/>
-      <c r="J119" s="17"/>
+      <c r="J119" s="49"/>
       <c r="K119" s="49"/>
       <c r="L119" s="18"/>
       <c r="M119" s="18"/>
@@ -4953,7 +4881,7 @@
     </row>
     <row r="120" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B120" s="4"/>
       <c r="C120" s="4"/>
@@ -4963,7 +4891,7 @@
       <c r="G120" s="58"/>
       <c r="H120" s="49"/>
       <c r="I120" s="49"/>
-      <c r="J120" s="17"/>
+      <c r="J120" s="49"/>
       <c r="K120" s="49"/>
       <c r="L120" s="18"/>
       <c r="M120" s="18"/>
@@ -4986,7 +4914,7 @@
     </row>
     <row r="121" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
@@ -4996,7 +4924,7 @@
       <c r="G121" s="58"/>
       <c r="H121" s="49"/>
       <c r="I121" s="49"/>
-      <c r="J121" s="17"/>
+      <c r="J121" s="49"/>
       <c r="K121" s="49"/>
       <c r="L121" s="18"/>
       <c r="M121" s="18"/>
@@ -5019,7 +4947,7 @@
     </row>
     <row r="122" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
@@ -5029,7 +4957,7 @@
       <c r="G122" s="58"/>
       <c r="H122" s="49"/>
       <c r="I122" s="49"/>
-      <c r="J122" s="17"/>
+      <c r="J122" s="49"/>
       <c r="K122" s="49"/>
       <c r="L122" s="18"/>
       <c r="M122" s="18"/>
@@ -5052,7 +4980,7 @@
     </row>
     <row r="123" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
@@ -5062,7 +4990,7 @@
       <c r="G123" s="58"/>
       <c r="H123" s="49"/>
       <c r="I123" s="49"/>
-      <c r="J123" s="17"/>
+      <c r="J123" s="49"/>
       <c r="K123" s="49"/>
       <c r="L123" s="18"/>
       <c r="M123" s="18"/>
@@ -5085,7 +5013,7 @@
     </row>
     <row r="124" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
@@ -5095,7 +5023,7 @@
       <c r="G124" s="58"/>
       <c r="H124" s="49"/>
       <c r="I124" s="49"/>
-      <c r="J124" s="17"/>
+      <c r="J124" s="49"/>
       <c r="K124" s="49"/>
       <c r="L124" s="18"/>
       <c r="M124" s="18"/>
@@ -5118,7 +5046,7 @@
     </row>
     <row r="125" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
@@ -5128,7 +5056,7 @@
       <c r="G125" s="58"/>
       <c r="H125" s="49"/>
       <c r="I125" s="49"/>
-      <c r="J125" s="17"/>
+      <c r="J125" s="49"/>
       <c r="K125" s="49"/>
       <c r="L125" s="18"/>
       <c r="M125" s="18"/>
@@ -5151,7 +5079,7 @@
     </row>
     <row r="126" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
@@ -5161,7 +5089,7 @@
       <c r="G126" s="58"/>
       <c r="H126" s="49"/>
       <c r="I126" s="49"/>
-      <c r="J126" s="17"/>
+      <c r="J126" s="49"/>
       <c r="K126" s="49"/>
       <c r="L126" s="18"/>
       <c r="M126" s="18"/>
@@ -5184,7 +5112,7 @@
     </row>
     <row r="127" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
@@ -5194,7 +5122,7 @@
       <c r="G127" s="58"/>
       <c r="H127" s="49"/>
       <c r="I127" s="49"/>
-      <c r="J127" s="17"/>
+      <c r="J127" s="49"/>
       <c r="K127" s="49"/>
       <c r="L127" s="18"/>
       <c r="M127" s="18"/>
@@ -5217,7 +5145,7 @@
     </row>
     <row r="128" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
@@ -5227,7 +5155,7 @@
       <c r="G128" s="58"/>
       <c r="H128" s="49"/>
       <c r="I128" s="49"/>
-      <c r="J128" s="17"/>
+      <c r="J128" s="49"/>
       <c r="K128" s="49"/>
       <c r="L128" s="18"/>
       <c r="M128" s="18"/>
@@ -5250,7 +5178,7 @@
     </row>
     <row r="129" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
@@ -5260,7 +5188,7 @@
       <c r="G129" s="58"/>
       <c r="H129" s="49"/>
       <c r="I129" s="49"/>
-      <c r="J129" s="17"/>
+      <c r="J129" s="49"/>
       <c r="K129" s="49"/>
       <c r="L129" s="18"/>
       <c r="M129" s="18"/>
@@ -5283,7 +5211,7 @@
     </row>
     <row r="130" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
@@ -5293,7 +5221,7 @@
       <c r="G130" s="58"/>
       <c r="H130" s="49"/>
       <c r="I130" s="49"/>
-      <c r="J130" s="17"/>
+      <c r="J130" s="49"/>
       <c r="K130" s="49"/>
       <c r="L130" s="18"/>
       <c r="M130" s="18"/>
@@ -5316,7 +5244,7 @@
     </row>
     <row r="131" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
@@ -5326,7 +5254,7 @@
       <c r="G131" s="58"/>
       <c r="H131" s="49"/>
       <c r="I131" s="49"/>
-      <c r="J131" s="17"/>
+      <c r="J131" s="49"/>
       <c r="K131" s="49"/>
       <c r="L131" s="18"/>
       <c r="M131" s="18"/>
@@ -5349,7 +5277,7 @@
     </row>
     <row r="132" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
@@ -5359,7 +5287,7 @@
       <c r="G132" s="58"/>
       <c r="H132" s="49"/>
       <c r="I132" s="49"/>
-      <c r="J132" s="17"/>
+      <c r="J132" s="49"/>
       <c r="K132" s="49"/>
       <c r="L132" s="18"/>
       <c r="M132" s="18"/>
@@ -5382,7 +5310,7 @@
     </row>
     <row r="133" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
@@ -5392,7 +5320,7 @@
       <c r="G133" s="58"/>
       <c r="H133" s="49"/>
       <c r="I133" s="49"/>
-      <c r="J133" s="17"/>
+      <c r="J133" s="49"/>
       <c r="K133" s="49"/>
       <c r="L133" s="18"/>
       <c r="M133" s="18"/>
@@ -5415,7 +5343,7 @@
     </row>
     <row r="134" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
@@ -5425,7 +5353,7 @@
       <c r="G134" s="58"/>
       <c r="H134" s="49"/>
       <c r="I134" s="49"/>
-      <c r="J134" s="17"/>
+      <c r="J134" s="49"/>
       <c r="K134" s="49"/>
       <c r="L134" s="18"/>
       <c r="M134" s="18"/>
@@ -5448,7 +5376,7 @@
     </row>
     <row r="135" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
@@ -5458,7 +5386,7 @@
       <c r="G135" s="58"/>
       <c r="H135" s="49"/>
       <c r="I135" s="49"/>
-      <c r="J135" s="17"/>
+      <c r="J135" s="49"/>
       <c r="K135" s="49"/>
       <c r="L135" s="18"/>
       <c r="M135" s="18"/>
@@ -5481,7 +5409,7 @@
     </row>
     <row r="136" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
@@ -5491,7 +5419,7 @@
       <c r="G136" s="58"/>
       <c r="H136" s="49"/>
       <c r="I136" s="49"/>
-      <c r="J136" s="17"/>
+      <c r="J136" s="49"/>
       <c r="K136" s="49"/>
       <c r="L136" s="18"/>
       <c r="M136" s="18"/>
@@ -5514,7 +5442,7 @@
     </row>
     <row r="137" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>
@@ -5524,7 +5452,7 @@
       <c r="G137" s="58"/>
       <c r="H137" s="49"/>
       <c r="I137" s="49"/>
-      <c r="J137" s="17"/>
+      <c r="J137" s="49"/>
       <c r="K137" s="49"/>
       <c r="L137" s="18"/>
       <c r="M137" s="18"/>
@@ -5547,7 +5475,7 @@
     </row>
     <row r="138" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
@@ -5557,7 +5485,7 @@
       <c r="G138" s="58"/>
       <c r="H138" s="49"/>
       <c r="I138" s="49"/>
-      <c r="J138" s="17"/>
+      <c r="J138" s="49"/>
       <c r="K138" s="49"/>
       <c r="L138" s="18"/>
       <c r="M138" s="18"/>
@@ -5580,7 +5508,7 @@
     </row>
     <row r="139" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
@@ -5590,7 +5518,7 @@
       <c r="G139" s="58"/>
       <c r="H139" s="49"/>
       <c r="I139" s="49"/>
-      <c r="J139" s="17"/>
+      <c r="J139" s="49"/>
       <c r="K139" s="49"/>
       <c r="L139" s="18"/>
       <c r="M139" s="18"/>
@@ -5613,7 +5541,7 @@
     </row>
     <row r="140" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
@@ -5623,7 +5551,7 @@
       <c r="G140" s="58"/>
       <c r="H140" s="49"/>
       <c r="I140" s="49"/>
-      <c r="J140" s="17"/>
+      <c r="J140" s="49"/>
       <c r="K140" s="49"/>
       <c r="L140" s="18"/>
       <c r="M140" s="18"/>
@@ -5646,7 +5574,7 @@
     </row>
     <row r="141" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
@@ -5656,7 +5584,7 @@
       <c r="G141" s="58"/>
       <c r="H141" s="49"/>
       <c r="I141" s="49"/>
-      <c r="J141" s="17"/>
+      <c r="J141" s="49"/>
       <c r="K141" s="49"/>
       <c r="L141" s="18"/>
       <c r="M141" s="18"/>
@@ -5679,7 +5607,7 @@
     </row>
     <row r="142" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
@@ -5689,7 +5617,7 @@
       <c r="G142" s="58"/>
       <c r="H142" s="49"/>
       <c r="I142" s="49"/>
-      <c r="J142" s="17"/>
+      <c r="J142" s="49"/>
       <c r="K142" s="49"/>
       <c r="L142" s="18"/>
       <c r="M142" s="18"/>
@@ -5712,7 +5640,7 @@
     </row>
     <row r="143" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B143" s="4"/>
       <c r="C143" s="4"/>
@@ -5722,7 +5650,7 @@
       <c r="G143" s="58"/>
       <c r="H143" s="49"/>
       <c r="I143" s="49"/>
-      <c r="J143" s="17"/>
+      <c r="J143" s="49"/>
       <c r="K143" s="49"/>
       <c r="L143" s="18"/>
       <c r="M143" s="18"/>
@@ -5745,7 +5673,7 @@
     </row>
     <row r="144" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B144" s="4"/>
       <c r="C144" s="4"/>
@@ -5755,7 +5683,7 @@
       <c r="G144" s="58"/>
       <c r="H144" s="49"/>
       <c r="I144" s="49"/>
-      <c r="J144" s="17"/>
+      <c r="J144" s="49"/>
       <c r="K144" s="49"/>
       <c r="L144" s="18"/>
       <c r="M144" s="18"/>
@@ -5778,7 +5706,7 @@
     </row>
     <row r="145" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="3">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B145" s="4"/>
       <c r="C145" s="4"/>
@@ -5788,7 +5716,7 @@
       <c r="G145" s="58"/>
       <c r="H145" s="49"/>
       <c r="I145" s="49"/>
-      <c r="J145" s="17"/>
+      <c r="J145" s="49"/>
       <c r="K145" s="49"/>
       <c r="L145" s="18"/>
       <c r="M145" s="18"/>
@@ -5811,7 +5739,7 @@
     </row>
     <row r="146" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
@@ -5821,7 +5749,7 @@
       <c r="G146" s="58"/>
       <c r="H146" s="49"/>
       <c r="I146" s="49"/>
-      <c r="J146" s="17"/>
+      <c r="J146" s="49"/>
       <c r="K146" s="49"/>
       <c r="L146" s="18"/>
       <c r="M146" s="18"/>
@@ -5844,7 +5772,7 @@
     </row>
     <row r="147" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
@@ -5854,7 +5782,7 @@
       <c r="G147" s="58"/>
       <c r="H147" s="49"/>
       <c r="I147" s="49"/>
-      <c r="J147" s="17"/>
+      <c r="J147" s="49"/>
       <c r="K147" s="49"/>
       <c r="L147" s="18"/>
       <c r="M147" s="18"/>
@@ -5877,7 +5805,7 @@
     </row>
     <row r="148" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B148" s="4"/>
       <c r="C148" s="4"/>
@@ -5887,7 +5815,7 @@
       <c r="G148" s="58"/>
       <c r="H148" s="49"/>
       <c r="I148" s="49"/>
-      <c r="J148" s="17"/>
+      <c r="J148" s="49"/>
       <c r="K148" s="49"/>
       <c r="L148" s="18"/>
       <c r="M148" s="18"/>
@@ -5910,7 +5838,7 @@
     </row>
     <row r="149" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B149" s="4"/>
       <c r="C149" s="4"/>
@@ -5920,7 +5848,7 @@
       <c r="G149" s="58"/>
       <c r="H149" s="49"/>
       <c r="I149" s="49"/>
-      <c r="J149" s="17"/>
+      <c r="J149" s="49"/>
       <c r="K149" s="49"/>
       <c r="L149" s="18"/>
       <c r="M149" s="18"/>
@@ -5943,7 +5871,7 @@
     </row>
     <row r="150" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B150" s="4"/>
       <c r="C150" s="4"/>
@@ -5953,7 +5881,7 @@
       <c r="G150" s="58"/>
       <c r="H150" s="49"/>
       <c r="I150" s="49"/>
-      <c r="J150" s="17"/>
+      <c r="J150" s="49"/>
       <c r="K150" s="49"/>
       <c r="L150" s="18"/>
       <c r="M150" s="18"/>
@@ -5976,7 +5904,7 @@
     </row>
     <row r="151" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B151" s="4"/>
       <c r="C151" s="4"/>
@@ -5986,7 +5914,7 @@
       <c r="G151" s="58"/>
       <c r="H151" s="49"/>
       <c r="I151" s="49"/>
-      <c r="J151" s="17"/>
+      <c r="J151" s="49"/>
       <c r="K151" s="49"/>
       <c r="L151" s="18"/>
       <c r="M151" s="18"/>
@@ -6009,7 +5937,7 @@
     </row>
     <row r="152" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B152" s="4"/>
       <c r="C152" s="4"/>
@@ -6019,7 +5947,7 @@
       <c r="G152" s="58"/>
       <c r="H152" s="49"/>
       <c r="I152" s="49"/>
-      <c r="J152" s="17"/>
+      <c r="J152" s="49"/>
       <c r="K152" s="49"/>
       <c r="L152" s="18"/>
       <c r="M152" s="18"/>
@@ -6042,7 +5970,7 @@
     </row>
     <row r="153" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B153" s="4"/>
       <c r="C153" s="4"/>
@@ -6052,7 +5980,7 @@
       <c r="G153" s="58"/>
       <c r="H153" s="49"/>
       <c r="I153" s="49"/>
-      <c r="J153" s="17"/>
+      <c r="J153" s="49"/>
       <c r="K153" s="49"/>
       <c r="L153" s="18"/>
       <c r="M153" s="18"/>
@@ -6075,7 +6003,7 @@
     </row>
     <row r="154" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B154" s="4"/>
       <c r="C154" s="4"/>
@@ -6085,7 +6013,7 @@
       <c r="G154" s="58"/>
       <c r="H154" s="49"/>
       <c r="I154" s="49"/>
-      <c r="J154" s="17"/>
+      <c r="J154" s="49"/>
       <c r="K154" s="49"/>
       <c r="L154" s="18"/>
       <c r="M154" s="18"/>
@@ -6108,7 +6036,7 @@
     </row>
     <row r="155" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B155" s="4"/>
       <c r="C155" s="4"/>
@@ -6118,7 +6046,7 @@
       <c r="G155" s="58"/>
       <c r="H155" s="49"/>
       <c r="I155" s="49"/>
-      <c r="J155" s="17"/>
+      <c r="J155" s="49"/>
       <c r="K155" s="49"/>
       <c r="L155" s="18"/>
       <c r="M155" s="18"/>
@@ -6141,7 +6069,7 @@
     </row>
     <row r="156" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="3">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B156" s="4"/>
       <c r="C156" s="4"/>
@@ -6151,7 +6079,7 @@
       <c r="G156" s="58"/>
       <c r="H156" s="49"/>
       <c r="I156" s="49"/>
-      <c r="J156" s="17"/>
+      <c r="J156" s="49"/>
       <c r="K156" s="49"/>
       <c r="L156" s="18"/>
       <c r="M156" s="18"/>
@@ -6174,7 +6102,7 @@
     </row>
     <row r="157" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B157" s="4"/>
       <c r="C157" s="4"/>
@@ -6184,7 +6112,7 @@
       <c r="G157" s="58"/>
       <c r="H157" s="49"/>
       <c r="I157" s="49"/>
-      <c r="J157" s="17"/>
+      <c r="J157" s="49"/>
       <c r="K157" s="49"/>
       <c r="L157" s="18"/>
       <c r="M157" s="18"/>
@@ -6207,7 +6135,7 @@
     </row>
     <row r="158" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="3">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B158" s="4"/>
       <c r="C158" s="4"/>
@@ -6217,7 +6145,7 @@
       <c r="G158" s="58"/>
       <c r="H158" s="49"/>
       <c r="I158" s="49"/>
-      <c r="J158" s="17"/>
+      <c r="J158" s="49"/>
       <c r="K158" s="49"/>
       <c r="L158" s="18"/>
       <c r="M158" s="18"/>
@@ -6240,7 +6168,7 @@
     </row>
     <row r="159" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="3">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B159" s="4"/>
       <c r="C159" s="4"/>
@@ -6250,7 +6178,7 @@
       <c r="G159" s="58"/>
       <c r="H159" s="49"/>
       <c r="I159" s="49"/>
-      <c r="J159" s="17"/>
+      <c r="J159" s="49"/>
       <c r="K159" s="49"/>
       <c r="L159" s="18"/>
       <c r="M159" s="18"/>
@@ -6273,7 +6201,7 @@
     </row>
     <row r="160" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="3">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B160" s="4"/>
       <c r="C160" s="4"/>
@@ -6283,7 +6211,7 @@
       <c r="G160" s="58"/>
       <c r="H160" s="49"/>
       <c r="I160" s="49"/>
-      <c r="J160" s="17"/>
+      <c r="J160" s="49"/>
       <c r="K160" s="49"/>
       <c r="L160" s="18"/>
       <c r="M160" s="18"/>
@@ -6306,7 +6234,7 @@
     </row>
     <row r="161" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B161" s="4"/>
       <c r="C161" s="4"/>
@@ -6316,7 +6244,7 @@
       <c r="G161" s="58"/>
       <c r="H161" s="49"/>
       <c r="I161" s="49"/>
-      <c r="J161" s="17"/>
+      <c r="J161" s="49"/>
       <c r="K161" s="49"/>
       <c r="L161" s="18"/>
       <c r="M161" s="18"/>
@@ -6339,7 +6267,7 @@
     </row>
     <row r="162" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="3">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B162" s="4"/>
       <c r="C162" s="4"/>
@@ -6349,7 +6277,7 @@
       <c r="G162" s="58"/>
       <c r="H162" s="49"/>
       <c r="I162" s="49"/>
-      <c r="J162" s="17"/>
+      <c r="J162" s="49"/>
       <c r="K162" s="49"/>
       <c r="L162" s="18"/>
       <c r="M162" s="18"/>
@@ -6372,7 +6300,7 @@
     </row>
     <row r="163" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="3">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
@@ -6382,7 +6310,7 @@
       <c r="G163" s="58"/>
       <c r="H163" s="49"/>
       <c r="I163" s="49"/>
-      <c r="J163" s="17"/>
+      <c r="J163" s="49"/>
       <c r="K163" s="49"/>
       <c r="L163" s="18"/>
       <c r="M163" s="18"/>
@@ -6405,7 +6333,7 @@
     </row>
     <row r="164" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="3">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B164" s="4"/>
       <c r="C164" s="4"/>
@@ -6415,7 +6343,7 @@
       <c r="G164" s="58"/>
       <c r="H164" s="49"/>
       <c r="I164" s="49"/>
-      <c r="J164" s="17"/>
+      <c r="J164" s="49"/>
       <c r="K164" s="49"/>
       <c r="L164" s="18"/>
       <c r="M164" s="18"/>
@@ -6438,7 +6366,7 @@
     </row>
     <row r="165" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="3">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B165" s="4"/>
       <c r="C165" s="4"/>
@@ -6448,7 +6376,7 @@
       <c r="G165" s="58"/>
       <c r="H165" s="49"/>
       <c r="I165" s="49"/>
-      <c r="J165" s="17"/>
+      <c r="J165" s="49"/>
       <c r="K165" s="49"/>
       <c r="L165" s="18"/>
       <c r="M165" s="18"/>
@@ -6471,7 +6399,7 @@
     </row>
     <row r="166" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="3">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
@@ -6481,7 +6409,7 @@
       <c r="G166" s="58"/>
       <c r="H166" s="49"/>
       <c r="I166" s="49"/>
-      <c r="J166" s="17"/>
+      <c r="J166" s="49"/>
       <c r="K166" s="49"/>
       <c r="L166" s="18"/>
       <c r="M166" s="18"/>
@@ -6504,7 +6432,7 @@
     </row>
     <row r="167" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="3">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B167" s="4"/>
       <c r="C167" s="4"/>
@@ -6514,7 +6442,7 @@
       <c r="G167" s="58"/>
       <c r="H167" s="49"/>
       <c r="I167" s="49"/>
-      <c r="J167" s="17"/>
+      <c r="J167" s="49"/>
       <c r="K167" s="49"/>
       <c r="L167" s="18"/>
       <c r="M167" s="18"/>
@@ -6537,7 +6465,7 @@
     </row>
     <row r="168" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="3">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B168" s="4"/>
       <c r="C168" s="4"/>
@@ -6547,7 +6475,7 @@
       <c r="G168" s="58"/>
       <c r="H168" s="49"/>
       <c r="I168" s="49"/>
-      <c r="J168" s="17"/>
+      <c r="J168" s="49"/>
       <c r="K168" s="49"/>
       <c r="L168" s="18"/>
       <c r="M168" s="18"/>
@@ -6570,7 +6498,7 @@
     </row>
     <row r="169" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="3">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
@@ -6580,7 +6508,7 @@
       <c r="G169" s="58"/>
       <c r="H169" s="49"/>
       <c r="I169" s="49"/>
-      <c r="J169" s="17"/>
+      <c r="J169" s="49"/>
       <c r="K169" s="49"/>
       <c r="L169" s="18"/>
       <c r="M169" s="18"/>
@@ -6603,7 +6531,7 @@
     </row>
     <row r="170" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="3">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B170" s="4"/>
       <c r="C170" s="4"/>
@@ -6613,7 +6541,7 @@
       <c r="G170" s="58"/>
       <c r="H170" s="49"/>
       <c r="I170" s="49"/>
-      <c r="J170" s="17"/>
+      <c r="J170" s="49"/>
       <c r="K170" s="49"/>
       <c r="L170" s="18"/>
       <c r="M170" s="18"/>
@@ -6636,7 +6564,7 @@
     </row>
     <row r="171" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="3">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B171" s="4"/>
       <c r="C171" s="4"/>
@@ -6646,7 +6574,7 @@
       <c r="G171" s="58"/>
       <c r="H171" s="49"/>
       <c r="I171" s="49"/>
-      <c r="J171" s="17"/>
+      <c r="J171" s="49"/>
       <c r="K171" s="49"/>
       <c r="L171" s="18"/>
       <c r="M171" s="18"/>
@@ -6669,7 +6597,7 @@
     </row>
     <row r="172" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="3">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B172" s="4"/>
       <c r="C172" s="4"/>
@@ -6679,7 +6607,7 @@
       <c r="G172" s="58"/>
       <c r="H172" s="49"/>
       <c r="I172" s="49"/>
-      <c r="J172" s="17"/>
+      <c r="J172" s="49"/>
       <c r="K172" s="49"/>
       <c r="L172" s="18"/>
       <c r="M172" s="18"/>
@@ -6702,7 +6630,7 @@
     </row>
     <row r="173" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="3">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B173" s="4"/>
       <c r="C173" s="4"/>
@@ -6712,7 +6640,7 @@
       <c r="G173" s="58"/>
       <c r="H173" s="49"/>
       <c r="I173" s="49"/>
-      <c r="J173" s="17"/>
+      <c r="J173" s="49"/>
       <c r="K173" s="49"/>
       <c r="L173" s="18"/>
       <c r="M173" s="18"/>
@@ -6735,7 +6663,7 @@
     </row>
     <row r="174" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="3">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B174" s="4"/>
       <c r="C174" s="4"/>
@@ -6745,7 +6673,7 @@
       <c r="G174" s="58"/>
       <c r="H174" s="49"/>
       <c r="I174" s="49"/>
-      <c r="J174" s="17"/>
+      <c r="J174" s="49"/>
       <c r="K174" s="49"/>
       <c r="L174" s="18"/>
       <c r="M174" s="18"/>
@@ -6768,7 +6696,7 @@
     </row>
     <row r="175" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="3">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B175" s="4"/>
       <c r="C175" s="4"/>
@@ -6778,7 +6706,7 @@
       <c r="G175" s="58"/>
       <c r="H175" s="49"/>
       <c r="I175" s="49"/>
-      <c r="J175" s="17"/>
+      <c r="J175" s="49"/>
       <c r="K175" s="49"/>
       <c r="L175" s="18"/>
       <c r="M175" s="18"/>
@@ -6801,7 +6729,7 @@
     </row>
     <row r="176" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="3">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B176" s="4"/>
       <c r="C176" s="4"/>
@@ -6811,7 +6739,7 @@
       <c r="G176" s="58"/>
       <c r="H176" s="49"/>
       <c r="I176" s="49"/>
-      <c r="J176" s="17"/>
+      <c r="J176" s="49"/>
       <c r="K176" s="49"/>
       <c r="L176" s="18"/>
       <c r="M176" s="18"/>
@@ -6834,7 +6762,7 @@
     </row>
     <row r="177" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="3">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B177" s="4"/>
       <c r="C177" s="4"/>
@@ -6844,7 +6772,7 @@
       <c r="G177" s="58"/>
       <c r="H177" s="49"/>
       <c r="I177" s="49"/>
-      <c r="J177" s="17"/>
+      <c r="J177" s="49"/>
       <c r="K177" s="49"/>
       <c r="L177" s="18"/>
       <c r="M177" s="18"/>
@@ -6867,7 +6795,7 @@
     </row>
     <row r="178" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="3">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B178" s="4"/>
       <c r="C178" s="4"/>
@@ -6877,7 +6805,7 @@
       <c r="G178" s="58"/>
       <c r="H178" s="49"/>
       <c r="I178" s="49"/>
-      <c r="J178" s="17"/>
+      <c r="J178" s="49"/>
       <c r="K178" s="49"/>
       <c r="L178" s="18"/>
       <c r="M178" s="18"/>
@@ -6900,7 +6828,7 @@
     </row>
     <row r="179" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="3">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B179" s="4"/>
       <c r="C179" s="4"/>
@@ -6910,7 +6838,7 @@
       <c r="G179" s="58"/>
       <c r="H179" s="49"/>
       <c r="I179" s="49"/>
-      <c r="J179" s="17"/>
+      <c r="J179" s="49"/>
       <c r="K179" s="49"/>
       <c r="L179" s="18"/>
       <c r="M179" s="18"/>
@@ -6933,7 +6861,7 @@
     </row>
     <row r="180" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="3">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B180" s="4"/>
       <c r="C180" s="4"/>
@@ -6943,7 +6871,7 @@
       <c r="G180" s="58"/>
       <c r="H180" s="49"/>
       <c r="I180" s="49"/>
-      <c r="J180" s="17"/>
+      <c r="J180" s="49"/>
       <c r="K180" s="49"/>
       <c r="L180" s="18"/>
       <c r="M180" s="18"/>
@@ -6966,7 +6894,7 @@
     </row>
     <row r="181" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="3">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B181" s="4"/>
       <c r="C181" s="4"/>
@@ -6976,7 +6904,7 @@
       <c r="G181" s="58"/>
       <c r="H181" s="49"/>
       <c r="I181" s="49"/>
-      <c r="J181" s="17"/>
+      <c r="J181" s="49"/>
       <c r="K181" s="49"/>
       <c r="L181" s="18"/>
       <c r="M181" s="18"/>
@@ -6999,7 +6927,7 @@
     </row>
     <row r="182" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="3">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B182" s="4"/>
       <c r="C182" s="4"/>
@@ -7009,7 +6937,7 @@
       <c r="G182" s="58"/>
       <c r="H182" s="49"/>
       <c r="I182" s="49"/>
-      <c r="J182" s="17"/>
+      <c r="J182" s="49"/>
       <c r="K182" s="49"/>
       <c r="L182" s="18"/>
       <c r="M182" s="18"/>
@@ -7032,7 +6960,7 @@
     </row>
     <row r="183" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="3">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B183" s="4"/>
       <c r="C183" s="4"/>
@@ -7042,7 +6970,7 @@
       <c r="G183" s="58"/>
       <c r="H183" s="49"/>
       <c r="I183" s="49"/>
-      <c r="J183" s="17"/>
+      <c r="J183" s="49"/>
       <c r="K183" s="49"/>
       <c r="L183" s="18"/>
       <c r="M183" s="18"/>
@@ -7065,7 +6993,7 @@
     </row>
     <row r="184" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="3">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B184" s="4"/>
       <c r="C184" s="4"/>
@@ -7075,7 +7003,7 @@
       <c r="G184" s="58"/>
       <c r="H184" s="49"/>
       <c r="I184" s="49"/>
-      <c r="J184" s="17"/>
+      <c r="J184" s="49"/>
       <c r="K184" s="49"/>
       <c r="L184" s="18"/>
       <c r="M184" s="18"/>
@@ -7098,7 +7026,7 @@
     </row>
     <row r="185" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="3">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B185" s="4"/>
       <c r="C185" s="4"/>
@@ -7108,7 +7036,7 @@
       <c r="G185" s="58"/>
       <c r="H185" s="49"/>
       <c r="I185" s="49"/>
-      <c r="J185" s="17"/>
+      <c r="J185" s="49"/>
       <c r="K185" s="49"/>
       <c r="L185" s="18"/>
       <c r="M185" s="18"/>
@@ -7131,7 +7059,7 @@
     </row>
     <row r="186" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="3">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B186" s="4"/>
       <c r="C186" s="4"/>
@@ -7141,7 +7069,7 @@
       <c r="G186" s="58"/>
       <c r="H186" s="49"/>
       <c r="I186" s="49"/>
-      <c r="J186" s="17"/>
+      <c r="J186" s="49"/>
       <c r="K186" s="49"/>
       <c r="L186" s="18"/>
       <c r="M186" s="18"/>
@@ -7164,7 +7092,7 @@
     </row>
     <row r="187" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="3">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B187" s="4"/>
       <c r="C187" s="4"/>
@@ -7174,7 +7102,7 @@
       <c r="G187" s="58"/>
       <c r="H187" s="49"/>
       <c r="I187" s="49"/>
-      <c r="J187" s="17"/>
+      <c r="J187" s="49"/>
       <c r="K187" s="49"/>
       <c r="L187" s="18"/>
       <c r="M187" s="18"/>
@@ -7197,7 +7125,7 @@
     </row>
     <row r="188" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="3">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B188" s="4"/>
       <c r="C188" s="4"/>
@@ -7207,7 +7135,7 @@
       <c r="G188" s="58"/>
       <c r="H188" s="49"/>
       <c r="I188" s="49"/>
-      <c r="J188" s="17"/>
+      <c r="J188" s="49"/>
       <c r="K188" s="49"/>
       <c r="L188" s="18"/>
       <c r="M188" s="18"/>
@@ -7230,7 +7158,7 @@
     </row>
     <row r="189" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="3">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B189" s="4"/>
       <c r="C189" s="4"/>
@@ -7240,7 +7168,7 @@
       <c r="G189" s="58"/>
       <c r="H189" s="49"/>
       <c r="I189" s="49"/>
-      <c r="J189" s="17"/>
+      <c r="J189" s="49"/>
       <c r="K189" s="49"/>
       <c r="L189" s="18"/>
       <c r="M189" s="18"/>
@@ -7263,7 +7191,7 @@
     </row>
     <row r="190" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="3">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B190" s="4"/>
       <c r="C190" s="4"/>
@@ -7273,7 +7201,7 @@
       <c r="G190" s="58"/>
       <c r="H190" s="49"/>
       <c r="I190" s="49"/>
-      <c r="J190" s="17"/>
+      <c r="J190" s="49"/>
       <c r="K190" s="49"/>
       <c r="L190" s="18"/>
       <c r="M190" s="18"/>
@@ -7296,7 +7224,7 @@
     </row>
     <row r="191" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="3">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B191" s="4"/>
       <c r="C191" s="4"/>
@@ -7306,7 +7234,7 @@
       <c r="G191" s="58"/>
       <c r="H191" s="49"/>
       <c r="I191" s="49"/>
-      <c r="J191" s="17"/>
+      <c r="J191" s="49"/>
       <c r="K191" s="49"/>
       <c r="L191" s="18"/>
       <c r="M191" s="18"/>
@@ -7329,7 +7257,7 @@
     </row>
     <row r="192" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="3">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B192" s="4"/>
       <c r="C192" s="4"/>
@@ -7339,7 +7267,7 @@
       <c r="G192" s="58"/>
       <c r="H192" s="49"/>
       <c r="I192" s="49"/>
-      <c r="J192" s="17"/>
+      <c r="J192" s="49"/>
       <c r="K192" s="49"/>
       <c r="L192" s="18"/>
       <c r="M192" s="18"/>
@@ -7362,7 +7290,7 @@
     </row>
     <row r="193" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="3">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B193" s="4"/>
       <c r="C193" s="4"/>
@@ -7372,7 +7300,7 @@
       <c r="G193" s="58"/>
       <c r="H193" s="49"/>
       <c r="I193" s="49"/>
-      <c r="J193" s="17"/>
+      <c r="J193" s="49"/>
       <c r="K193" s="49"/>
       <c r="L193" s="18"/>
       <c r="M193" s="18"/>
@@ -7395,7 +7323,7 @@
     </row>
     <row r="194" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="3">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B194" s="4"/>
       <c r="C194" s="4"/>
@@ -7405,7 +7333,7 @@
       <c r="G194" s="58"/>
       <c r="H194" s="49"/>
       <c r="I194" s="49"/>
-      <c r="J194" s="17"/>
+      <c r="J194" s="49"/>
       <c r="K194" s="49"/>
       <c r="L194" s="18"/>
       <c r="M194" s="18"/>
@@ -7428,7 +7356,7 @@
     </row>
     <row r="195" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="3">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B195" s="4"/>
       <c r="C195" s="4"/>
@@ -7438,7 +7366,7 @@
       <c r="G195" s="58"/>
       <c r="H195" s="49"/>
       <c r="I195" s="49"/>
-      <c r="J195" s="17"/>
+      <c r="J195" s="49"/>
       <c r="K195" s="49"/>
       <c r="L195" s="18"/>
       <c r="M195" s="18"/>
@@ -7461,7 +7389,7 @@
     </row>
     <row r="196" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="3">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B196" s="4"/>
       <c r="C196" s="4"/>
@@ -7471,7 +7399,7 @@
       <c r="G196" s="58"/>
       <c r="H196" s="49"/>
       <c r="I196" s="49"/>
-      <c r="J196" s="17"/>
+      <c r="J196" s="49"/>
       <c r="K196" s="49"/>
       <c r="L196" s="18"/>
       <c r="M196" s="18"/>
@@ -7494,7 +7422,7 @@
     </row>
     <row r="197" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="3">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B197" s="4"/>
       <c r="C197" s="4"/>
@@ -7504,7 +7432,7 @@
       <c r="G197" s="58"/>
       <c r="H197" s="49"/>
       <c r="I197" s="49"/>
-      <c r="J197" s="17"/>
+      <c r="J197" s="49"/>
       <c r="K197" s="49"/>
       <c r="L197" s="18"/>
       <c r="M197" s="18"/>
@@ -7527,7 +7455,7 @@
     </row>
     <row r="198" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="3">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B198" s="4"/>
       <c r="C198" s="4"/>
@@ -7537,7 +7465,7 @@
       <c r="G198" s="58"/>
       <c r="H198" s="49"/>
       <c r="I198" s="49"/>
-      <c r="J198" s="17"/>
+      <c r="J198" s="49"/>
       <c r="K198" s="49"/>
       <c r="L198" s="18"/>
       <c r="M198" s="18"/>
@@ -7560,7 +7488,7 @@
     </row>
     <row r="199" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="3">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B199" s="4"/>
       <c r="C199" s="4"/>
@@ -7570,7 +7498,7 @@
       <c r="G199" s="58"/>
       <c r="H199" s="49"/>
       <c r="I199" s="49"/>
-      <c r="J199" s="17"/>
+      <c r="J199" s="49"/>
       <c r="K199" s="49"/>
       <c r="L199" s="18"/>
       <c r="M199" s="18"/>
@@ -7593,7 +7521,7 @@
     </row>
     <row r="200" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="3">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B200" s="4"/>
       <c r="C200" s="4"/>
@@ -7603,7 +7531,7 @@
       <c r="G200" s="58"/>
       <c r="H200" s="49"/>
       <c r="I200" s="49"/>
-      <c r="J200" s="17"/>
+      <c r="J200" s="49"/>
       <c r="K200" s="49"/>
       <c r="L200" s="18"/>
       <c r="M200" s="18"/>
@@ -7626,7 +7554,7 @@
     </row>
     <row r="201" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="3">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B201" s="4"/>
       <c r="C201" s="4"/>
@@ -7636,7 +7564,7 @@
       <c r="G201" s="58"/>
       <c r="H201" s="49"/>
       <c r="I201" s="49"/>
-      <c r="J201" s="17"/>
+      <c r="J201" s="49"/>
       <c r="K201" s="49"/>
       <c r="L201" s="18"/>
       <c r="M201" s="18"/>
@@ -7659,7 +7587,7 @@
     </row>
     <row r="202" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="3">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B202" s="4"/>
       <c r="C202" s="4"/>
@@ -7669,7 +7597,7 @@
       <c r="G202" s="58"/>
       <c r="H202" s="49"/>
       <c r="I202" s="49"/>
-      <c r="J202" s="17"/>
+      <c r="J202" s="49"/>
       <c r="K202" s="49"/>
       <c r="L202" s="18"/>
       <c r="M202" s="18"/>
@@ -7692,7 +7620,7 @@
     </row>
     <row r="203" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="3">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B203" s="4"/>
       <c r="C203" s="4"/>
@@ -7702,7 +7630,7 @@
       <c r="G203" s="58"/>
       <c r="H203" s="49"/>
       <c r="I203" s="49"/>
-      <c r="J203" s="17"/>
+      <c r="J203" s="49"/>
       <c r="K203" s="49"/>
       <c r="L203" s="18"/>
       <c r="M203" s="18"/>
@@ -7724,21 +7652,19 @@
       <c r="AC203" s="1"/>
     </row>
     <row r="204" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="3">
-        <v>199</v>
-      </c>
-      <c r="B204" s="4"/>
-      <c r="C204" s="4"/>
-      <c r="D204" s="4"/>
-      <c r="E204" s="4"/>
-      <c r="F204" s="52"/>
-      <c r="G204" s="58"/>
-      <c r="H204" s="49"/>
-      <c r="I204" s="49"/>
-      <c r="J204" s="17"/>
-      <c r="K204" s="49"/>
-      <c r="L204" s="18"/>
-      <c r="M204" s="18"/>
+      <c r="A204" s="1"/>
+      <c r="B204" s="1"/>
+      <c r="C204" s="1"/>
+      <c r="D204" s="1"/>
+      <c r="E204" s="1"/>
+      <c r="F204" s="53"/>
+      <c r="G204" s="55"/>
+      <c r="H204" s="1"/>
+      <c r="I204" s="1"/>
+      <c r="J204" s="1"/>
+      <c r="K204" s="1"/>
+      <c r="L204" s="1"/>
+      <c r="M204" s="1"/>
       <c r="N204" s="1"/>
       <c r="O204" s="1"/>
       <c r="P204" s="1"/>
@@ -7757,21 +7683,19 @@
       <c r="AC204" s="1"/>
     </row>
     <row r="205" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="3">
-        <v>200</v>
-      </c>
-      <c r="B205" s="4"/>
-      <c r="C205" s="4"/>
-      <c r="D205" s="4"/>
-      <c r="E205" s="4"/>
-      <c r="F205" s="52"/>
-      <c r="G205" s="58"/>
-      <c r="H205" s="49"/>
-      <c r="I205" s="49"/>
-      <c r="J205" s="17"/>
-      <c r="K205" s="49"/>
-      <c r="L205" s="18"/>
-      <c r="M205" s="18"/>
+      <c r="A205" s="1"/>
+      <c r="B205" s="1"/>
+      <c r="C205" s="1"/>
+      <c r="D205" s="1"/>
+      <c r="E205" s="1"/>
+      <c r="F205" s="53"/>
+      <c r="G205" s="55"/>
+      <c r="H205" s="1"/>
+      <c r="I205" s="1"/>
+      <c r="J205" s="1"/>
+      <c r="K205" s="1"/>
+      <c r="L205" s="1"/>
+      <c r="M205" s="1"/>
       <c r="N205" s="1"/>
       <c r="O205" s="1"/>
       <c r="P205" s="1"/>
@@ -28683,73 +28607,9 @@
       <c r="AB879" s="1"/>
       <c r="AC879" s="1"/>
     </row>
-    <row r="880" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A880" s="1"/>
-      <c r="B880" s="1"/>
-      <c r="C880" s="1"/>
-      <c r="D880" s="1"/>
-      <c r="E880" s="1"/>
-      <c r="F880" s="53"/>
-      <c r="G880" s="55"/>
-      <c r="H880" s="1"/>
-      <c r="I880" s="1"/>
-      <c r="J880" s="1"/>
-      <c r="K880" s="1"/>
-      <c r="L880" s="1"/>
-      <c r="M880" s="1"/>
-      <c r="N880" s="1"/>
-      <c r="O880" s="1"/>
-      <c r="P880" s="1"/>
-      <c r="Q880" s="1"/>
-      <c r="R880" s="1"/>
-      <c r="S880" s="1"/>
-      <c r="T880" s="1"/>
-      <c r="U880" s="1"/>
-      <c r="V880" s="1"/>
-      <c r="W880" s="1"/>
-      <c r="X880" s="1"/>
-      <c r="Y880" s="1"/>
-      <c r="Z880" s="1"/>
-      <c r="AA880" s="1"/>
-      <c r="AB880" s="1"/>
-      <c r="AC880" s="1"/>
-    </row>
-    <row r="881" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A881" s="1"/>
-      <c r="B881" s="1"/>
-      <c r="C881" s="1"/>
-      <c r="D881" s="1"/>
-      <c r="E881" s="1"/>
-      <c r="F881" s="53"/>
-      <c r="G881" s="55"/>
-      <c r="H881" s="1"/>
-      <c r="I881" s="1"/>
-      <c r="J881" s="1"/>
-      <c r="K881" s="1"/>
-      <c r="L881" s="1"/>
-      <c r="M881" s="1"/>
-      <c r="N881" s="1"/>
-      <c r="O881" s="1"/>
-      <c r="P881" s="1"/>
-      <c r="Q881" s="1"/>
-      <c r="R881" s="1"/>
-      <c r="S881" s="1"/>
-      <c r="T881" s="1"/>
-      <c r="U881" s="1"/>
-      <c r="V881" s="1"/>
-      <c r="W881" s="1"/>
-      <c r="X881" s="1"/>
-      <c r="Y881" s="1"/>
-      <c r="Z881" s="1"/>
-      <c r="AA881" s="1"/>
-      <c r="AB881" s="1"/>
-      <c r="AC881" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="1">
     <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -28761,37 +28621,37 @@
           <x14:formula1>
             <xm:f>'Lista desplegable'!$B$2:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H6:H205</xm:sqref>
+          <xm:sqref>H4:H203</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7F2DB051-E384-43CF-B2ED-0A7452DD5FE7}">
           <x14:formula1>
             <xm:f>'Lista desplegable'!$D$2:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>I6:I205</xm:sqref>
+          <xm:sqref>I4:I203</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{26CB2F67-76D9-4D30-A88C-B082E31F0885}">
           <x14:formula1>
             <xm:f>'Lista desplegable'!$F$2:$F$20</xm:f>
           </x14:formula1>
-          <xm:sqref>K6:K205</xm:sqref>
+          <xm:sqref>K4:K203</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{2CD09D54-636F-4F55-84F8-A3C40B4060A4}">
           <x14:formula1>
             <xm:f>'Lista desplegable'!$G$2:$G$4</xm:f>
           </x14:formula1>
-          <xm:sqref>L6:L205</xm:sqref>
+          <xm:sqref>L4:L203</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{796471EE-F570-4A60-9C8D-6F268F0E3F5D}">
           <x14:formula1>
             <xm:f>'Lista desplegable'!$H$2:$H$11</xm:f>
           </x14:formula1>
-          <xm:sqref>M6:M205</xm:sqref>
+          <xm:sqref>M4:M203</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{92D86DC5-FD93-44F4-891D-99D8CA7D3FBC}">
           <x14:formula1>
             <xm:f>'Lista desplegable'!$E$2:$E$7</xm:f>
           </x14:formula1>
-          <xm:sqref>J6:J205</xm:sqref>
+          <xm:sqref>J4:J203</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -28801,12 +28661,126 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E368BD4B-B338-49C7-8C1A-20391A3EAB94}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AC16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:M1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -28839,13 +28813,13 @@
         <v>16</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" s="40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="28" t="s">
         <v>14</v>
@@ -28856,25 +28830,25 @@
     </row>
     <row r="2" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" s="43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -28888,7 +28862,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="43">
         <v>0.1</v>
@@ -28911,7 +28885,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="44" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="43">
         <v>0.5</v>
@@ -28934,7 +28908,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="43">
         <v>1</v>
@@ -28949,7 +28923,7 @@
         <v>1.5</v>
       </c>
       <c r="E6" s="45" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F6" s="43">
         <v>1.5</v>
@@ -28964,7 +28938,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="43">
         <v>2</v>

</xml_diff>